<commit_message>
fin 17 SEPT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE  HERRADURA  SEPTIEMBRE   2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE  HERRADURA  SEPTIEMBRE   2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="A G O S T O    2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="125">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -363,15 +363,9 @@
     <t>ESPINAZO-BOLA RES-HAMBURGUESA-CABEZA</t>
   </si>
   <si>
-    <t>dejo el producto</t>
-  </si>
-  <si>
     <t>LONGANIZA-ADOBO-SALCHICHAS</t>
   </si>
   <si>
-    <t># 1995</t>
-  </si>
-  <si>
     <t>MANCHEGO</t>
   </si>
   <si>
@@ -486,9 +480,6 @@
     <t>SEGURO</t>
   </si>
   <si>
-    <t>XXXXXX</t>
-  </si>
-  <si>
     <t>FUMIGACION</t>
   </si>
   <si>
@@ -496,6 +487,39 @@
   </si>
   <si>
     <t>BALANCE      ABASTO 4 CARNES    H E R R A D U R A     SEPTIEMBRE            2 0 2 1</t>
+  </si>
+  <si>
+    <t>bolsas- ARERO</t>
+  </si>
+  <si>
+    <t>JAMON</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>LONGANIZA-CHORIZO</t>
+  </si>
+  <si>
+    <t>TOSTADAS--SUADERO-CONCHA-RES-MAIZ</t>
+  </si>
+  <si>
+    <t>NOMINA # 37</t>
+  </si>
+  <si>
+    <t>LONGANIZA-JAMON-CONCHA RES-MAIZ-A¿CONDIMENTOS</t>
+  </si>
+  <si>
+    <t>QUESOS-MAIZ-CONCHA RES</t>
+  </si>
+  <si>
+    <t>#3225</t>
+  </si>
+  <si>
+    <t># 3227</t>
+  </si>
+  <si>
+    <t>CONCHA RES--CHAMBARETE</t>
   </si>
 </sst>
 </file>
@@ -859,7 +883,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -902,6 +926,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="58">
     <border>
@@ -1629,7 +1659,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="254">
+  <cellXfs count="255">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
@@ -1999,138 +2029,6 @@
     <xf numFmtId="44" fontId="31" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="3" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="3" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2146,9 +2044,6 @@
     <xf numFmtId="165" fontId="19" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2158,8 +2053,144 @@
     <xf numFmtId="164" fontId="12" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="44" fontId="41" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="3" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="3" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -3305,8 +3336,8 @@
   </sheetPr>
   <dimension ref="A1:R80"/>
   <sheetViews>
-    <sheetView topLeftCell="G34" workbookViewId="0">
-      <selection activeCell="G34" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="G31" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3328,23 +3359,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="203"/>
-      <c r="C1" s="212" t="s">
+      <c r="B1" s="235"/>
+      <c r="C1" s="244" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="213"/>
-      <c r="E1" s="213"/>
-      <c r="F1" s="213"/>
-      <c r="G1" s="213"/>
-      <c r="H1" s="213"/>
-      <c r="I1" s="213"/>
-      <c r="J1" s="213"/>
-      <c r="K1" s="213"/>
-      <c r="L1" s="213"/>
-      <c r="M1" s="213"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="204"/>
+      <c r="B2" s="236"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -3354,17 +3385,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="205" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="206"/>
+      <c r="B3" s="237" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="238"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="207" t="s">
+      <c r="H3" s="239" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="207"/>
+      <c r="I3" s="239"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -3380,14 +3411,14 @@
       <c r="D4" s="16">
         <v>44410</v>
       </c>
-      <c r="E4" s="208" t="s">
+      <c r="E4" s="240" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="209"/>
-      <c r="H4" s="210" t="s">
+      <c r="F4" s="241"/>
+      <c r="H4" s="242" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="211"/>
+      <c r="I4" s="243"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -3397,10 +3428,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="197" t="s">
+      <c r="P4" s="229" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="198"/>
+      <c r="Q4" s="230"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -4468,7 +4499,7 @@
         <v>1682</v>
       </c>
       <c r="D29" s="64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E29" s="24">
         <v>44438</v>
@@ -4552,7 +4583,7 @@
         <v>366</v>
       </c>
       <c r="D31" s="70" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E31" s="24">
         <v>44440</v>
@@ -4595,7 +4626,7 @@
         <v>5669</v>
       </c>
       <c r="D32" s="73" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E32" s="24">
         <v>44441</v>
@@ -4638,7 +4669,7 @@
         <v>1362</v>
       </c>
       <c r="D33" s="74" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E33" s="24">
         <v>44442</v>
@@ -4681,7 +4712,7 @@
         <v>1000</v>
       </c>
       <c r="D34" s="73" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E34" s="24">
         <v>44443</v>
@@ -4700,7 +4731,7 @@
         <v>44443</v>
       </c>
       <c r="K34" s="187" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L34" s="76">
         <v>10680.95</v>
@@ -4730,7 +4761,7 @@
         <v>3173</v>
       </c>
       <c r="D35" s="77" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E35" s="24">
         <v>44444</v>
@@ -4887,19 +4918,19 @@
       <c r="H39" s="32"/>
       <c r="I39" s="81"/>
       <c r="J39" s="67" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K39" s="82" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L39" s="69">
         <v>454.62</v>
       </c>
-      <c r="M39" s="199">
+      <c r="M39" s="231">
         <f>SUM(M5:M38)</f>
         <v>1393675.5</v>
       </c>
-      <c r="N39" s="201">
+      <c r="N39" s="233">
         <f>SUM(N5:N38)</f>
         <v>28399.97</v>
       </c>
@@ -4923,16 +4954,16 @@
       <c r="H40" s="32"/>
       <c r="I40" s="81"/>
       <c r="J40" s="67" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K40" s="71" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L40" s="69">
         <v>1195.67</v>
       </c>
-      <c r="M40" s="200"/>
-      <c r="N40" s="202"/>
+      <c r="M40" s="232"/>
+      <c r="N40" s="234"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -4940,23 +4971,23 @@
       <c r="A41" s="20"/>
       <c r="B41" s="21"/>
       <c r="C41" s="84"/>
-      <c r="D41" s="241"/>
-      <c r="E41" s="242"/>
-      <c r="F41" s="243"/>
+      <c r="D41" s="197"/>
+      <c r="E41" s="198"/>
+      <c r="F41" s="199"/>
       <c r="G41" s="26"/>
-      <c r="H41" s="244"/>
+      <c r="H41" s="200"/>
       <c r="I41" s="85"/>
       <c r="J41" s="67" t="s">
-        <v>111</v>
-      </c>
-      <c r="K41" s="248" t="s">
-        <v>113</v>
+        <v>109</v>
+      </c>
+      <c r="K41" s="208" t="s">
+        <v>114</v>
       </c>
       <c r="L41" s="75">
         <v>7174.1</v>
       </c>
-      <c r="M41" s="246"/>
-      <c r="N41" s="245"/>
+      <c r="M41" s="202"/>
+      <c r="N41" s="201"/>
       <c r="P41" s="83"/>
       <c r="Q41" s="9"/>
     </row>
@@ -4964,23 +4995,23 @@
       <c r="A42" s="20"/>
       <c r="B42" s="21"/>
       <c r="C42" s="84"/>
-      <c r="D42" s="241"/>
-      <c r="E42" s="242"/>
-      <c r="F42" s="243"/>
+      <c r="D42" s="197"/>
+      <c r="E42" s="198"/>
+      <c r="F42" s="199"/>
       <c r="G42" s="26"/>
-      <c r="H42" s="244"/>
+      <c r="H42" s="200"/>
       <c r="I42" s="85"/>
       <c r="J42" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="K42" s="71" t="s">
         <v>111</v>
-      </c>
-      <c r="K42" s="71" t="s">
-        <v>114</v>
       </c>
       <c r="L42" s="75">
         <v>2552</v>
       </c>
-      <c r="M42" s="246"/>
-      <c r="N42" s="245"/>
+      <c r="M42" s="202"/>
+      <c r="N42" s="201"/>
       <c r="P42" s="83"/>
       <c r="Q42" s="9"/>
     </row>
@@ -4988,23 +5019,23 @@
       <c r="A43" s="20"/>
       <c r="B43" s="21"/>
       <c r="C43" s="84"/>
-      <c r="D43" s="241"/>
-      <c r="E43" s="242"/>
-      <c r="F43" s="243"/>
+      <c r="D43" s="197"/>
+      <c r="E43" s="198"/>
+      <c r="F43" s="199"/>
       <c r="G43" s="26"/>
-      <c r="H43" s="244"/>
+      <c r="H43" s="200"/>
       <c r="I43" s="85"/>
       <c r="J43" s="67" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K43" s="71" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L43" s="75">
         <v>6994</v>
       </c>
-      <c r="M43" s="246"/>
-      <c r="N43" s="245"/>
+      <c r="M43" s="202"/>
+      <c r="N43" s="201"/>
       <c r="P43" s="83"/>
       <c r="Q43" s="9"/>
     </row>
@@ -5012,17 +5043,17 @@
       <c r="A44" s="20"/>
       <c r="B44" s="21"/>
       <c r="C44" s="84"/>
-      <c r="D44" s="241"/>
-      <c r="E44" s="242"/>
-      <c r="F44" s="243"/>
+      <c r="D44" s="197"/>
+      <c r="E44" s="198"/>
+      <c r="F44" s="199"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="244"/>
+      <c r="H44" s="200"/>
       <c r="I44" s="85"/>
       <c r="J44" s="67"/>
       <c r="K44" s="71"/>
       <c r="L44" s="75"/>
-      <c r="M44" s="246"/>
-      <c r="N44" s="245"/>
+      <c r="M44" s="202"/>
+      <c r="N44" s="201"/>
       <c r="P44" s="83"/>
       <c r="Q44" s="9"/>
     </row>
@@ -5030,17 +5061,17 @@
       <c r="A45" s="20"/>
       <c r="B45" s="21"/>
       <c r="C45" s="84"/>
-      <c r="D45" s="241"/>
-      <c r="E45" s="242"/>
-      <c r="F45" s="243"/>
+      <c r="D45" s="197"/>
+      <c r="E45" s="198"/>
+      <c r="F45" s="199"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="244"/>
+      <c r="H45" s="200"/>
       <c r="I45" s="85"/>
       <c r="J45" s="67"/>
       <c r="K45" s="71"/>
       <c r="L45" s="75"/>
-      <c r="M45" s="246"/>
-      <c r="N45" s="245"/>
+      <c r="M45" s="202"/>
+      <c r="N45" s="201"/>
       <c r="P45" s="83"/>
       <c r="Q45" s="9"/>
     </row>
@@ -5048,17 +5079,17 @@
       <c r="A46" s="20"/>
       <c r="B46" s="21"/>
       <c r="C46" s="84"/>
-      <c r="D46" s="241"/>
-      <c r="E46" s="242"/>
-      <c r="F46" s="243"/>
+      <c r="D46" s="197"/>
+      <c r="E46" s="198"/>
+      <c r="F46" s="199"/>
       <c r="G46" s="26"/>
-      <c r="H46" s="244"/>
+      <c r="H46" s="200"/>
       <c r="I46" s="85"/>
       <c r="J46" s="67"/>
       <c r="K46" s="71"/>
       <c r="L46" s="75"/>
-      <c r="M46" s="246"/>
-      <c r="N46" s="245"/>
+      <c r="M46" s="202"/>
+      <c r="N46" s="201"/>
       <c r="P46" s="83"/>
       <c r="Q46" s="9"/>
     </row>
@@ -5066,17 +5097,17 @@
       <c r="A47" s="20"/>
       <c r="B47" s="21"/>
       <c r="C47" s="84"/>
-      <c r="D47" s="241"/>
-      <c r="E47" s="242"/>
-      <c r="F47" s="243"/>
+      <c r="D47" s="197"/>
+      <c r="E47" s="198"/>
+      <c r="F47" s="199"/>
       <c r="G47" s="26"/>
-      <c r="H47" s="244"/>
+      <c r="H47" s="200"/>
       <c r="I47" s="85"/>
       <c r="J47" s="67"/>
       <c r="K47" s="71"/>
       <c r="L47" s="75"/>
-      <c r="M47" s="246"/>
-      <c r="N47" s="245"/>
+      <c r="M47" s="202"/>
+      <c r="N47" s="201"/>
       <c r="P47" s="83"/>
       <c r="Q47" s="9"/>
     </row>
@@ -5084,17 +5115,17 @@
       <c r="A48" s="20"/>
       <c r="B48" s="21"/>
       <c r="C48" s="84"/>
-      <c r="D48" s="241"/>
-      <c r="E48" s="242"/>
-      <c r="F48" s="243"/>
+      <c r="D48" s="197"/>
+      <c r="E48" s="198"/>
+      <c r="F48" s="199"/>
       <c r="G48" s="26"/>
-      <c r="H48" s="244"/>
+      <c r="H48" s="200"/>
       <c r="I48" s="85"/>
       <c r="J48" s="67"/>
       <c r="K48" s="71"/>
       <c r="L48" s="75"/>
-      <c r="M48" s="246"/>
-      <c r="N48" s="245"/>
+      <c r="M48" s="202"/>
+      <c r="N48" s="201"/>
       <c r="P48" s="83"/>
       <c r="Q48" s="9"/>
     </row>
@@ -5109,7 +5140,7 @@
       <c r="F49" s="84"/>
       <c r="H49" s="91"/>
       <c r="I49" s="85"/>
-      <c r="J49" s="247"/>
+      <c r="J49" s="203"/>
       <c r="K49" s="86"/>
       <c r="L49" s="9"/>
       <c r="M49" s="87"/>
@@ -5165,29 +5196,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="214" t="s">
+      <c r="H52" s="219" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="215"/>
+      <c r="I52" s="220"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="216">
+      <c r="K52" s="221">
         <f>I50+L50</f>
         <v>80916.84</v>
       </c>
-      <c r="L52" s="217"/>
-      <c r="M52" s="224">
+      <c r="L52" s="222"/>
+      <c r="M52" s="210">
         <f>N39+M39</f>
         <v>1422075.47</v>
       </c>
-      <c r="N52" s="225"/>
+      <c r="N52" s="211"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="218" t="s">
+      <c r="D53" s="223" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="218"/>
+      <c r="E53" s="223"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1396181.44</v>
@@ -5198,22 +5229,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="219" t="s">
+      <c r="D54" s="224" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="219"/>
+      <c r="E54" s="224"/>
       <c r="F54" s="102">
         <v>-1523111</v>
       </c>
-      <c r="I54" s="220" t="s">
+      <c r="I54" s="225" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="221"/>
-      <c r="K54" s="222">
+      <c r="J54" s="226"/>
+      <c r="K54" s="227">
         <f>F56+F57+F58</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L54" s="223"/>
+      <c r="L54" s="228"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -5244,10 +5275,10 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="226">
-        <v>0</v>
-      </c>
-      <c r="L56" s="227"/>
+      <c r="K56" s="212">
+        <v>0</v>
+      </c>
+      <c r="L56" s="213"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -5264,22 +5295,22 @@
       <c r="C58" s="120">
         <v>44444</v>
       </c>
-      <c r="D58" s="228" t="s">
+      <c r="D58" s="214" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="229"/>
+      <c r="E58" s="215"/>
       <c r="F58" s="121">
         <v>136234.76999999999</v>
       </c>
-      <c r="I58" s="230" t="s">
+      <c r="I58" s="216" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="231"/>
-      <c r="K58" s="232">
+      <c r="J58" s="217"/>
+      <c r="K58" s="218">
         <f>K54+K56</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L58" s="232"/>
+      <c r="L58" s="218"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -5423,6 +5454,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C1:M1"/>
     <mergeCell ref="M52:N52"/>
     <mergeCell ref="K56:L56"/>
     <mergeCell ref="D58:E58"/>
@@ -5434,15 +5474,6 @@
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="C1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5459,7 +5490,7 @@
   <dimension ref="A1:G134"/>
   <sheetViews>
     <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A39" sqref="A1:XFD1048576"/>
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5514,7 +5545,7 @@
       <c r="C3" s="35">
         <v>3015.96</v>
       </c>
-      <c r="D3" s="233" t="s">
+      <c r="D3" s="246" t="s">
         <v>50</v>
       </c>
       <c r="E3" s="9"/>
@@ -5533,7 +5564,7 @@
       <c r="C4" s="35">
         <v>10281</v>
       </c>
-      <c r="D4" s="234"/>
+      <c r="D4" s="247"/>
       <c r="E4" s="183"/>
       <c r="F4" s="145">
         <f>F3+C4-E4</f>
@@ -5551,7 +5582,7 @@
       <c r="C5" s="35">
         <v>12746.2</v>
       </c>
-      <c r="D5" s="234"/>
+      <c r="D5" s="247"/>
       <c r="E5" s="183"/>
       <c r="F5" s="145">
         <f t="shared" ref="F5:F68" si="0">F4+C5-E5</f>
@@ -5568,7 +5599,7 @@
       <c r="C6" s="35">
         <v>28974.78</v>
       </c>
-      <c r="D6" s="234"/>
+      <c r="D6" s="247"/>
       <c r="E6" s="183"/>
       <c r="F6" s="145">
         <f t="shared" si="0"/>
@@ -5585,7 +5616,7 @@
       <c r="C7" s="35">
         <v>44758.6</v>
       </c>
-      <c r="D7" s="234"/>
+      <c r="D7" s="247"/>
       <c r="E7" s="183"/>
       <c r="F7" s="145">
         <f t="shared" si="0"/>
@@ -5602,7 +5633,7 @@
       <c r="C8" s="35">
         <v>12841.78</v>
       </c>
-      <c r="D8" s="234"/>
+      <c r="D8" s="247"/>
       <c r="E8" s="183"/>
       <c r="F8" s="145">
         <f t="shared" si="0"/>
@@ -5619,7 +5650,7 @@
       <c r="C9" s="35">
         <v>3898.05</v>
       </c>
-      <c r="D9" s="234"/>
+      <c r="D9" s="247"/>
       <c r="E9" s="183"/>
       <c r="F9" s="145">
         <f t="shared" si="0"/>
@@ -5636,7 +5667,7 @@
       <c r="C10" s="35">
         <v>1429</v>
       </c>
-      <c r="D10" s="235"/>
+      <c r="D10" s="248"/>
       <c r="E10" s="183"/>
       <c r="F10" s="145">
         <f t="shared" si="0"/>
@@ -5945,7 +5976,7 @@
         <v>44425</v>
       </c>
       <c r="B28" s="142" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C28" s="79">
         <v>49026.7</v>
@@ -5962,7 +5993,7 @@
         <v>44427</v>
       </c>
       <c r="B29" s="142" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C29" s="79">
         <v>29539.7</v>
@@ -5979,7 +6010,7 @@
         <v>44428</v>
       </c>
       <c r="B30" s="142" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C30" s="79">
         <v>61408.86</v>
@@ -5997,7 +6028,7 @@
         <v>44429</v>
       </c>
       <c r="B31" s="142" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C31" s="79">
         <v>18397.5</v>
@@ -6014,7 +6045,7 @@
         <v>44429</v>
       </c>
       <c r="B32" s="142" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C32" s="79">
         <v>47260.800000000003</v>
@@ -6031,7 +6062,7 @@
         <v>44429</v>
       </c>
       <c r="B33" s="142" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C33" s="79">
         <v>9625.7999999999993</v>
@@ -6048,7 +6079,7 @@
         <v>44431</v>
       </c>
       <c r="B34" s="142" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C34" s="79">
         <v>58308.1</v>
@@ -6065,7 +6096,7 @@
         <v>44432</v>
       </c>
       <c r="B35" s="142" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C35" s="79">
         <v>10718.4</v>
@@ -6082,7 +6113,7 @@
         <v>44432</v>
       </c>
       <c r="B36" s="142" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C36" s="79">
         <v>10385</v>
@@ -6103,7 +6134,7 @@
         <v>44433</v>
       </c>
       <c r="B37" s="142" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C37" s="79">
         <v>55844.4</v>
@@ -6120,7 +6151,7 @@
         <v>44433</v>
       </c>
       <c r="B38" s="142" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C38" s="79">
         <v>3492.2</v>
@@ -6137,7 +6168,7 @@
         <v>44434</v>
       </c>
       <c r="B39" s="142" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C39" s="79">
         <v>29683.7</v>
@@ -6154,7 +6185,7 @@
         <v>44435</v>
       </c>
       <c r="B40" s="142" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C40" s="79">
         <v>91570.559999999998</v>
@@ -6171,7 +6202,7 @@
         <v>44435</v>
       </c>
       <c r="B41" s="142" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C41" s="79">
         <v>5069.2</v>
@@ -6188,7 +6219,7 @@
         <v>44436</v>
       </c>
       <c r="B42" s="142" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C42" s="79">
         <v>50991.1</v>
@@ -6205,7 +6236,7 @@
         <v>44436</v>
       </c>
       <c r="B43" s="142" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C43" s="79">
         <v>3137.5</v>
@@ -6222,7 +6253,7 @@
         <v>44436</v>
       </c>
       <c r="B44" s="142" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C44" s="79">
         <v>1545</v>
@@ -6243,7 +6274,7 @@
         <v>44438</v>
       </c>
       <c r="B45" s="188" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C45" s="189">
         <v>59828.6</v>
@@ -6260,7 +6291,7 @@
         <v>44438</v>
       </c>
       <c r="B46" s="188" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C46" s="189">
         <v>7936</v>
@@ -6277,7 +6308,7 @@
         <v>44439</v>
       </c>
       <c r="B47" s="188" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C47" s="189">
         <v>51630.5</v>
@@ -6294,7 +6325,7 @@
         <v>44439</v>
       </c>
       <c r="B48" s="188" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C48" s="189">
         <v>8998</v>
@@ -6311,7 +6342,7 @@
         <v>44440</v>
       </c>
       <c r="B49" s="188" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C49" s="189">
         <v>19868.599999999999</v>
@@ -6328,7 +6359,7 @@
         <v>44441</v>
       </c>
       <c r="B50" s="188" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C50" s="189">
         <v>45543.199999999997</v>
@@ -6345,7 +6376,7 @@
         <v>44441</v>
       </c>
       <c r="B51" s="188" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C51" s="189">
         <v>3212.58</v>
@@ -6362,7 +6393,7 @@
         <v>44441</v>
       </c>
       <c r="B52" s="188" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C52" s="189">
         <v>4028.6</v>
@@ -6379,7 +6410,7 @@
         <v>44442</v>
       </c>
       <c r="B53" s="188" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C53" s="189">
         <v>101013.65</v>
@@ -6396,7 +6427,7 @@
         <v>44443</v>
       </c>
       <c r="B54" s="188" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C54" s="189">
         <v>35635.89</v>
@@ -6413,7 +6444,7 @@
         <v>44443</v>
       </c>
       <c r="B55" s="188" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C55" s="189">
         <v>691.2</v>
@@ -6447,7 +6478,7 @@
         <v>44444</v>
       </c>
       <c r="B57" s="188" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C57" s="189">
         <v>43121.2</v>
@@ -7125,8 +7156,8 @@
   </sheetPr>
   <dimension ref="A1:R80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7148,23 +7179,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="203"/>
-      <c r="C1" s="212" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="213"/>
-      <c r="E1" s="213"/>
-      <c r="F1" s="213"/>
-      <c r="G1" s="213"/>
-      <c r="H1" s="213"/>
-      <c r="I1" s="213"/>
-      <c r="J1" s="213"/>
-      <c r="K1" s="213"/>
-      <c r="L1" s="213"/>
-      <c r="M1" s="213"/>
+      <c r="B1" s="235"/>
+      <c r="C1" s="244" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="204"/>
+      <c r="B2" s="236"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -7174,17 +7205,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="205" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="206"/>
+      <c r="B3" s="237" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="238"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="207" t="s">
+      <c r="H3" s="239" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="207"/>
+      <c r="I3" s="239"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -7200,14 +7231,14 @@
       <c r="D4" s="16">
         <v>44444</v>
       </c>
-      <c r="E4" s="208" t="s">
+      <c r="E4" s="240" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="209"/>
-      <c r="H4" s="210" t="s">
+      <c r="F4" s="241"/>
+      <c r="H4" s="242" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="211"/>
+      <c r="I4" s="243"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -7217,10 +7248,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="197" t="s">
+      <c r="P4" s="229" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="198"/>
+      <c r="Q4" s="230"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -7237,27 +7268,28 @@
         <v>44445</v>
       </c>
       <c r="F5" s="25">
-        <v>0</v>
+        <v>37988</v>
       </c>
       <c r="G5" s="26"/>
       <c r="H5" s="27">
         <v>44445</v>
       </c>
       <c r="I5" s="28">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="29"/>
       <c r="L5" s="9"/>
       <c r="M5" s="138">
-        <v>0</v>
+        <f>15000+22973</f>
+        <v>37973</v>
       </c>
       <c r="N5" s="30">
         <v>0</v>
       </c>
       <c r="P5" s="83">
         <f>N5+M5+L5+I5+C5</f>
-        <v>0</v>
+        <v>37988</v>
       </c>
       <c r="Q5" s="136">
         <f>P5-F5</f>
@@ -7278,27 +7310,28 @@
         <v>44446</v>
       </c>
       <c r="F6" s="25">
-        <v>0</v>
+        <v>37318</v>
       </c>
       <c r="G6" s="26"/>
       <c r="H6" s="32">
         <v>44446</v>
       </c>
       <c r="I6" s="28">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J6" s="33"/>
       <c r="K6" s="34"/>
       <c r="L6" s="35"/>
       <c r="M6" s="138">
-        <v>0</v>
+        <f>15000+22138</f>
+        <v>37138</v>
       </c>
       <c r="N6" s="30">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="P6" s="83">
         <f t="shared" ref="P6:P36" si="0">N6+M6+L6+I6+C6</f>
-        <v>0</v>
+        <v>37318</v>
       </c>
       <c r="Q6" s="136">
         <f t="shared" ref="Q6:Q38" si="1">P6-F6</f>
@@ -7312,34 +7345,37 @@
         <v>44416</v>
       </c>
       <c r="C7" s="22">
-        <v>0</v>
-      </c>
-      <c r="D7" s="36"/>
+        <v>697</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>115</v>
+      </c>
       <c r="E7" s="24">
         <v>44447</v>
       </c>
       <c r="F7" s="25">
-        <v>0</v>
+        <v>25229</v>
       </c>
       <c r="G7" s="26"/>
       <c r="H7" s="32">
         <v>44447</v>
       </c>
       <c r="I7" s="28">
-        <v>0</v>
+        <v>640</v>
       </c>
       <c r="J7" s="33"/>
       <c r="K7" s="37"/>
       <c r="L7" s="35"/>
       <c r="M7" s="138">
-        <v>0</v>
+        <f>10000+12559</f>
+        <v>22559</v>
       </c>
       <c r="N7" s="30">
-        <v>0</v>
+        <v>1333</v>
       </c>
       <c r="P7" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25229</v>
       </c>
       <c r="Q7" s="9">
         <f t="shared" si="1"/>
@@ -7353,38 +7389,42 @@
         <v>44417</v>
       </c>
       <c r="C8" s="22">
-        <v>0</v>
-      </c>
-      <c r="D8" s="38"/>
+        <v>1344</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>117</v>
+      </c>
       <c r="E8" s="24">
         <v>44448</v>
       </c>
       <c r="F8" s="25">
-        <v>0</v>
+        <v>50511</v>
       </c>
       <c r="G8" s="26"/>
       <c r="H8" s="32">
         <v>44448</v>
       </c>
       <c r="I8" s="28">
-        <v>0</v>
+        <v>1326</v>
       </c>
       <c r="J8" s="39"/>
       <c r="K8" s="40"/>
       <c r="L8" s="35"/>
       <c r="M8" s="138">
-        <v>0</v>
+        <f>23544+20000</f>
+        <v>43544</v>
       </c>
       <c r="N8" s="30">
-        <v>0</v>
-      </c>
+        <v>4257</v>
+      </c>
+      <c r="O8" s="209"/>
       <c r="P8" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q8" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>50471</v>
+      </c>
+      <c r="Q8" s="186">
+        <f t="shared" si="1"/>
+        <v>-40</v>
       </c>
       <c r="R8" s="51"/>
     </row>
@@ -7401,30 +7441,31 @@
         <v>44449</v>
       </c>
       <c r="F9" s="25">
-        <v>0</v>
+        <v>55983</v>
       </c>
       <c r="G9" s="26"/>
       <c r="H9" s="32">
         <v>44449</v>
       </c>
       <c r="I9" s="28">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J9" s="33"/>
       <c r="K9" s="41"/>
       <c r="L9" s="35"/>
       <c r="M9" s="138">
-        <v>0</v>
+        <f>30000+23637</f>
+        <v>53637</v>
       </c>
       <c r="N9" s="30">
-        <v>0</v>
+        <v>2331</v>
       </c>
       <c r="P9" s="83">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>N9+M9+L9+I9+C9</f>
+        <v>55983</v>
       </c>
       <c r="Q9" s="9">
-        <f t="shared" si="1"/>
+        <f>P9-F9</f>
         <v>0</v>
       </c>
       <c r="R9" s="26"/>
@@ -7435,38 +7476,47 @@
         <v>44419</v>
       </c>
       <c r="C10" s="22">
-        <v>0</v>
-      </c>
-      <c r="D10" s="36"/>
+        <v>2725</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>118</v>
+      </c>
       <c r="E10" s="24">
         <v>44450</v>
       </c>
       <c r="F10" s="25">
-        <v>0</v>
+        <v>36838</v>
       </c>
       <c r="G10" s="26"/>
       <c r="H10" s="32">
         <v>44450</v>
       </c>
       <c r="I10" s="28">
-        <v>0</v>
-      </c>
-      <c r="J10" s="33"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="43"/>
+        <v>10</v>
+      </c>
+      <c r="J10" s="33">
+        <v>44450</v>
+      </c>
+      <c r="K10" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="L10" s="43">
+        <v>11014.29</v>
+      </c>
       <c r="M10" s="138">
-        <v>0</v>
+        <f>10000+12230</f>
+        <v>22230</v>
       </c>
       <c r="N10" s="30">
-        <v>0</v>
+        <v>859</v>
       </c>
       <c r="P10" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>36838.29</v>
       </c>
       <c r="Q10" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.29000000000087311</v>
       </c>
       <c r="R10" s="51"/>
     </row>
@@ -7483,27 +7533,28 @@
         <v>44451</v>
       </c>
       <c r="F11" s="25">
-        <v>0</v>
+        <v>82970</v>
       </c>
       <c r="G11" s="26"/>
       <c r="H11" s="32">
         <v>44451</v>
       </c>
       <c r="I11" s="28">
-        <v>0</v>
+        <v>3030</v>
       </c>
       <c r="J11" s="39"/>
       <c r="K11" s="44"/>
       <c r="L11" s="35"/>
       <c r="M11" s="138">
-        <v>0</v>
+        <f>16060+60000</f>
+        <v>76060</v>
       </c>
       <c r="N11" s="30">
-        <v>0</v>
+        <v>3880</v>
       </c>
       <c r="P11" s="83">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>N11+M11+L11+I11+C11</f>
+        <v>82970</v>
       </c>
       <c r="Q11" s="9">
         <f t="shared" si="1"/>
@@ -7517,38 +7568,42 @@
         <v>44421</v>
       </c>
       <c r="C12" s="22">
-        <v>0</v>
-      </c>
-      <c r="D12" s="31"/>
+        <v>6078</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>120</v>
+      </c>
       <c r="E12" s="24">
         <v>44452</v>
       </c>
       <c r="F12" s="25">
-        <v>0</v>
+        <v>46580</v>
       </c>
       <c r="G12" s="26"/>
       <c r="H12" s="32">
         <v>44452</v>
       </c>
       <c r="I12" s="28">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J12" s="33"/>
       <c r="K12" s="45"/>
       <c r="L12" s="35"/>
       <c r="M12" s="138">
-        <v>0</v>
+        <f>20000+18339</f>
+        <v>38339</v>
       </c>
       <c r="N12" s="30">
-        <v>0</v>
-      </c>
+        <v>2198</v>
+      </c>
+      <c r="O12" s="254"/>
       <c r="P12" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>46630</v>
+      </c>
+      <c r="Q12" s="186">
+        <f t="shared" si="1"/>
+        <v>50</v>
       </c>
       <c r="R12" s="26"/>
     </row>
@@ -7558,40 +7613,43 @@
         <v>44422</v>
       </c>
       <c r="C13" s="22">
-        <v>0</v>
-      </c>
-      <c r="D13" s="38"/>
+        <v>3282</v>
+      </c>
+      <c r="D13" s="38" t="s">
+        <v>121</v>
+      </c>
       <c r="E13" s="24">
         <v>44453</v>
       </c>
       <c r="F13" s="25">
-        <v>0</v>
+        <v>60579</v>
       </c>
       <c r="G13" s="26"/>
       <c r="H13" s="32">
         <v>44453</v>
       </c>
       <c r="I13" s="28">
-        <v>0</v>
+        <v>931</v>
       </c>
       <c r="J13" s="33"/>
       <c r="K13" s="46"/>
       <c r="L13" s="35"/>
       <c r="M13" s="138">
-        <v>0</v>
+        <f>30000+26366</f>
+        <v>56366</v>
       </c>
       <c r="N13" s="30">
         <v>0</v>
       </c>
       <c r="P13" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="252">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R13" s="253"/>
+        <v>60579</v>
+      </c>
+      <c r="Q13" s="136">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R13" s="207"/>
     </row>
     <row r="14" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="20"/>
@@ -7599,14 +7657,16 @@
         <v>44423</v>
       </c>
       <c r="C14" s="22">
-        <v>0</v>
-      </c>
-      <c r="D14" s="36"/>
+        <v>4078</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>124</v>
+      </c>
       <c r="E14" s="24">
         <v>44454</v>
       </c>
       <c r="F14" s="25">
-        <v>0</v>
+        <v>44141</v>
       </c>
       <c r="G14" s="26"/>
       <c r="H14" s="32">
@@ -7619,20 +7679,21 @@
       <c r="K14" s="40"/>
       <c r="L14" s="35"/>
       <c r="M14" s="138">
-        <v>0</v>
+        <f>20000+19655</f>
+        <v>39655</v>
       </c>
       <c r="N14" s="30">
-        <v>0</v>
+        <v>408</v>
       </c>
       <c r="P14" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>44141</v>
       </c>
       <c r="Q14" s="136">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R14" s="253"/>
+      <c r="R14" s="207"/>
     </row>
     <row r="15" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="20"/>
@@ -7647,7 +7708,7 @@
         <v>44455</v>
       </c>
       <c r="F15" s="25">
-        <v>0</v>
+        <v>45919</v>
       </c>
       <c r="G15" s="26"/>
       <c r="H15" s="32">
@@ -7660,18 +7721,19 @@
       <c r="K15" s="40"/>
       <c r="L15" s="35"/>
       <c r="M15" s="138">
-        <v>0</v>
+        <f>25000</f>
+        <v>25000</v>
       </c>
       <c r="N15" s="30">
         <v>0</v>
       </c>
       <c r="P15" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="Q15" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-20919</v>
       </c>
       <c r="R15" s="26"/>
     </row>
@@ -8609,21 +8671,21 @@
       <c r="J39" s="67"/>
       <c r="K39" s="82"/>
       <c r="L39" s="69"/>
-      <c r="M39" s="199">
+      <c r="M39" s="231">
         <f>SUM(M5:M38)</f>
-        <v>0</v>
-      </c>
-      <c r="N39" s="201">
+        <v>452501</v>
+      </c>
+      <c r="N39" s="233">
         <f>SUM(N5:N38)</f>
-        <v>0</v>
+        <v>15436</v>
       </c>
       <c r="P39" s="83">
         <f>SUM(P5:P38)</f>
-        <v>0</v>
+        <v>503147.29000000004</v>
       </c>
       <c r="Q39" s="9">
         <f>SUM(Q5:Q38)</f>
-        <v>0</v>
+        <v>-20908.71</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -8639,8 +8701,8 @@
       <c r="J40" s="67"/>
       <c r="K40" s="71"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="200"/>
-      <c r="N40" s="202"/>
+      <c r="M40" s="232"/>
+      <c r="N40" s="234"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -8648,17 +8710,17 @@
       <c r="A41" s="20"/>
       <c r="B41" s="21"/>
       <c r="C41" s="84"/>
-      <c r="D41" s="241"/>
-      <c r="E41" s="242"/>
-      <c r="F41" s="243"/>
+      <c r="D41" s="197"/>
+      <c r="E41" s="198"/>
+      <c r="F41" s="199"/>
       <c r="G41" s="26"/>
-      <c r="H41" s="244"/>
+      <c r="H41" s="200"/>
       <c r="I41" s="85"/>
       <c r="J41" s="67"/>
       <c r="K41" s="71"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="246"/>
-      <c r="N41" s="245"/>
+      <c r="M41" s="202"/>
+      <c r="N41" s="201"/>
       <c r="P41" s="83"/>
       <c r="Q41" s="9"/>
     </row>
@@ -8666,17 +8728,17 @@
       <c r="A42" s="20"/>
       <c r="B42" s="21"/>
       <c r="C42" s="84"/>
-      <c r="D42" s="241"/>
-      <c r="E42" s="242"/>
-      <c r="F42" s="243"/>
+      <c r="D42" s="197"/>
+      <c r="E42" s="198"/>
+      <c r="F42" s="199"/>
       <c r="G42" s="26"/>
-      <c r="H42" s="244"/>
+      <c r="H42" s="200"/>
       <c r="I42" s="85"/>
       <c r="J42" s="67"/>
       <c r="K42" s="71"/>
       <c r="L42" s="75"/>
-      <c r="M42" s="246"/>
-      <c r="N42" s="245"/>
+      <c r="M42" s="202"/>
+      <c r="N42" s="201"/>
       <c r="P42" s="83"/>
       <c r="Q42" s="9"/>
     </row>
@@ -8684,17 +8746,17 @@
       <c r="A43" s="20"/>
       <c r="B43" s="21"/>
       <c r="C43" s="84"/>
-      <c r="D43" s="241"/>
-      <c r="E43" s="242"/>
-      <c r="F43" s="243"/>
+      <c r="D43" s="197"/>
+      <c r="E43" s="198"/>
+      <c r="F43" s="199"/>
       <c r="G43" s="26"/>
-      <c r="H43" s="244"/>
+      <c r="H43" s="200"/>
       <c r="I43" s="85"/>
       <c r="J43" s="67"/>
       <c r="K43" s="71"/>
       <c r="L43" s="75"/>
-      <c r="M43" s="246"/>
-      <c r="N43" s="245"/>
+      <c r="M43" s="202"/>
+      <c r="N43" s="201"/>
       <c r="P43" s="83"/>
       <c r="Q43" s="9"/>
     </row>
@@ -8702,17 +8764,17 @@
       <c r="A44" s="20"/>
       <c r="B44" s="21"/>
       <c r="C44" s="84"/>
-      <c r="D44" s="241"/>
-      <c r="E44" s="242"/>
-      <c r="F44" s="243"/>
+      <c r="D44" s="197"/>
+      <c r="E44" s="198"/>
+      <c r="F44" s="199"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="244"/>
+      <c r="H44" s="200"/>
       <c r="I44" s="85"/>
       <c r="J44" s="67"/>
       <c r="K44" s="71"/>
       <c r="L44" s="75"/>
-      <c r="M44" s="246"/>
-      <c r="N44" s="245"/>
+      <c r="M44" s="202"/>
+      <c r="N44" s="201"/>
       <c r="P44" s="83"/>
       <c r="Q44" s="9"/>
     </row>
@@ -8720,17 +8782,17 @@
       <c r="A45" s="20"/>
       <c r="B45" s="21"/>
       <c r="C45" s="84"/>
-      <c r="D45" s="241"/>
-      <c r="E45" s="242"/>
-      <c r="F45" s="243"/>
+      <c r="D45" s="197"/>
+      <c r="E45" s="198"/>
+      <c r="F45" s="199"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="244"/>
+      <c r="H45" s="200"/>
       <c r="I45" s="85"/>
       <c r="J45" s="67"/>
       <c r="K45" s="71"/>
       <c r="L45" s="75"/>
-      <c r="M45" s="246"/>
-      <c r="N45" s="245"/>
+      <c r="M45" s="202"/>
+      <c r="N45" s="201"/>
       <c r="P45" s="83"/>
       <c r="Q45" s="9"/>
     </row>
@@ -8738,17 +8800,17 @@
       <c r="A46" s="20"/>
       <c r="B46" s="21"/>
       <c r="C46" s="84"/>
-      <c r="D46" s="241"/>
-      <c r="E46" s="242"/>
-      <c r="F46" s="243"/>
+      <c r="D46" s="197"/>
+      <c r="E46" s="198"/>
+      <c r="F46" s="199"/>
       <c r="G46" s="26"/>
-      <c r="H46" s="244"/>
+      <c r="H46" s="200"/>
       <c r="I46" s="85"/>
       <c r="J46" s="67"/>
       <c r="K46" s="71"/>
       <c r="L46" s="75"/>
-      <c r="M46" s="246"/>
-      <c r="N46" s="245"/>
+      <c r="M46" s="202"/>
+      <c r="N46" s="201"/>
       <c r="P46" s="83"/>
       <c r="Q46" s="9"/>
     </row>
@@ -8756,17 +8818,17 @@
       <c r="A47" s="20"/>
       <c r="B47" s="21"/>
       <c r="C47" s="84"/>
-      <c r="D47" s="241"/>
-      <c r="E47" s="242"/>
-      <c r="F47" s="243"/>
+      <c r="D47" s="197"/>
+      <c r="E47" s="198"/>
+      <c r="F47" s="199"/>
       <c r="G47" s="26"/>
-      <c r="H47" s="244"/>
+      <c r="H47" s="200"/>
       <c r="I47" s="85"/>
       <c r="J47" s="67"/>
       <c r="K47" s="71"/>
       <c r="L47" s="75"/>
-      <c r="M47" s="246"/>
-      <c r="N47" s="245"/>
+      <c r="M47" s="202"/>
+      <c r="N47" s="201"/>
       <c r="P47" s="83"/>
       <c r="Q47" s="9"/>
     </row>
@@ -8774,17 +8836,17 @@
       <c r="A48" s="20"/>
       <c r="B48" s="21"/>
       <c r="C48" s="84"/>
-      <c r="D48" s="241"/>
-      <c r="E48" s="242"/>
-      <c r="F48" s="243"/>
+      <c r="D48" s="197"/>
+      <c r="E48" s="198"/>
+      <c r="F48" s="199"/>
       <c r="G48" s="26"/>
-      <c r="H48" s="244"/>
+      <c r="H48" s="200"/>
       <c r="I48" s="85"/>
       <c r="J48" s="67"/>
       <c r="K48" s="71"/>
       <c r="L48" s="75"/>
-      <c r="M48" s="246"/>
-      <c r="N48" s="245"/>
+      <c r="M48" s="202"/>
+      <c r="N48" s="201"/>
       <c r="P48" s="83"/>
       <c r="Q48" s="9"/>
     </row>
@@ -8799,7 +8861,7 @@
       <c r="F49" s="84"/>
       <c r="H49" s="91"/>
       <c r="I49" s="85"/>
-      <c r="J49" s="247"/>
+      <c r="J49" s="203"/>
       <c r="K49" s="86"/>
       <c r="L49" s="9"/>
       <c r="M49" s="87"/>
@@ -8813,7 +8875,7 @@
       </c>
       <c r="C50" s="93">
         <f>SUM(C5:C49)</f>
-        <v>0</v>
+        <v>18204</v>
       </c>
       <c r="D50" s="94"/>
       <c r="E50" s="95" t="s">
@@ -8821,7 +8883,7 @@
       </c>
       <c r="F50" s="96">
         <f>SUM(F5:F49)</f>
-        <v>0</v>
+        <v>524056</v>
       </c>
       <c r="G50" s="94"/>
       <c r="H50" s="97" t="s">
@@ -8829,7 +8891,7 @@
       </c>
       <c r="I50" s="98">
         <f>SUM(I5:I49)</f>
-        <v>0</v>
+        <v>5992</v>
       </c>
       <c r="J50" s="99"/>
       <c r="K50" s="100" t="s">
@@ -8837,7 +8899,7 @@
       </c>
       <c r="L50" s="101">
         <f>SUM(L5:L49)</f>
-        <v>0</v>
+        <v>11014.29</v>
       </c>
       <c r="M50" s="102"/>
       <c r="N50" s="102"/>
@@ -8855,32 +8917,32 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="214" t="s">
+      <c r="H52" s="219" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="215"/>
+      <c r="I52" s="220"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="216">
+      <c r="K52" s="221">
         <f>I50+L50</f>
-        <v>0</v>
-      </c>
-      <c r="L52" s="217"/>
-      <c r="M52" s="224">
+        <v>17006.29</v>
+      </c>
+      <c r="L52" s="222"/>
+      <c r="M52" s="210">
         <f>N39+M39</f>
-        <v>0</v>
-      </c>
-      <c r="N52" s="225"/>
+        <v>467937</v>
+      </c>
+      <c r="N52" s="211"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="218" t="s">
+      <c r="D53" s="223" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="218"/>
+      <c r="E53" s="223"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
-        <v>0</v>
+        <v>488845.71</v>
       </c>
       <c r="I53" s="108"/>
       <c r="J53" s="109"/>
@@ -8888,22 +8950,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="219" t="s">
+      <c r="D54" s="224" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="219"/>
+      <c r="E54" s="224"/>
       <c r="F54" s="102">
         <v>0</v>
       </c>
-      <c r="I54" s="220" t="s">
+      <c r="I54" s="225" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="221"/>
-      <c r="K54" s="222">
+      <c r="J54" s="226"/>
+      <c r="K54" s="227">
         <f>F56+F57+F58</f>
-        <v>0</v>
-      </c>
-      <c r="L54" s="223"/>
+        <v>488845.71</v>
+      </c>
+      <c r="L54" s="228"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -8927,17 +8989,17 @@
       </c>
       <c r="F56" s="102">
         <f>SUM(F53:F55)</f>
-        <v>0</v>
+        <v>488845.71</v>
       </c>
       <c r="H56" s="20"/>
       <c r="I56" s="116" t="s">
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="226">
-        <v>0</v>
-      </c>
-      <c r="L56" s="227"/>
+      <c r="K56" s="212">
+        <v>0</v>
+      </c>
+      <c r="L56" s="213"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -8952,22 +9014,22 @@
     </row>
     <row r="58" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C58" s="120"/>
-      <c r="D58" s="228" t="s">
+      <c r="D58" s="214" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="229"/>
+      <c r="E58" s="215"/>
       <c r="F58" s="121">
         <v>0</v>
       </c>
-      <c r="I58" s="230" t="s">
+      <c r="I58" s="216" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="231"/>
-      <c r="K58" s="232">
+      <c r="J58" s="217"/>
+      <c r="K58" s="218">
         <f>K54+K56</f>
-        <v>0</v>
-      </c>
-      <c r="L58" s="232"/>
+        <v>488845.71</v>
+      </c>
+      <c r="L58" s="218"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -9111,11 +9173,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -9125,16 +9188,16 @@
     <mergeCell ref="H52:I52"/>
     <mergeCell ref="K52:L52"/>
     <mergeCell ref="M52:N52"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="K56:L56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -9172,19 +9235,19 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="249" t="s">
+      <c r="A2" s="204" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="249" t="s">
+      <c r="B2" s="204" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="250" t="s">
+      <c r="C2" s="205" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="249" t="s">
+      <c r="D2" s="204" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="250" t="s">
+      <c r="E2" s="205" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="140" t="s">
@@ -9195,7 +9258,7 @@
       <c r="A3" s="141"/>
       <c r="B3" s="182"/>
       <c r="C3" s="79"/>
-      <c r="D3" s="251"/>
+      <c r="D3" s="206"/>
       <c r="E3" s="79"/>
       <c r="F3" s="143">
         <f>C3-E3</f>
@@ -9206,7 +9269,7 @@
       <c r="A4" s="141"/>
       <c r="B4" s="182"/>
       <c r="C4" s="79"/>
-      <c r="D4" s="251"/>
+      <c r="D4" s="206"/>
       <c r="E4" s="79"/>
       <c r="F4" s="145">
         <f>F3+C4-E4</f>
@@ -9218,7 +9281,7 @@
       <c r="A5" s="141"/>
       <c r="B5" s="182"/>
       <c r="C5" s="79"/>
-      <c r="D5" s="251"/>
+      <c r="D5" s="206"/>
       <c r="E5" s="79"/>
       <c r="F5" s="145">
         <f t="shared" ref="F5:F68" si="0">F4+C5-E5</f>
@@ -9229,7 +9292,7 @@
       <c r="A6" s="141"/>
       <c r="B6" s="182"/>
       <c r="C6" s="79"/>
-      <c r="D6" s="251"/>
+      <c r="D6" s="206"/>
       <c r="E6" s="79"/>
       <c r="F6" s="145">
         <f t="shared" si="0"/>
@@ -9240,7 +9303,7 @@
       <c r="A7" s="141"/>
       <c r="B7" s="182"/>
       <c r="C7" s="79"/>
-      <c r="D7" s="251"/>
+      <c r="D7" s="206"/>
       <c r="E7" s="79"/>
       <c r="F7" s="145">
         <f t="shared" si="0"/>
@@ -9251,7 +9314,7 @@
       <c r="A8" s="141"/>
       <c r="B8" s="182"/>
       <c r="C8" s="79"/>
-      <c r="D8" s="251"/>
+      <c r="D8" s="206"/>
       <c r="E8" s="79"/>
       <c r="F8" s="145">
         <f t="shared" si="0"/>
@@ -9262,7 +9325,7 @@
       <c r="A9" s="141"/>
       <c r="B9" s="182"/>
       <c r="C9" s="79"/>
-      <c r="D9" s="251"/>
+      <c r="D9" s="206"/>
       <c r="E9" s="79"/>
       <c r="F9" s="145">
         <f t="shared" si="0"/>
@@ -9273,7 +9336,7 @@
       <c r="A10" s="141"/>
       <c r="B10" s="182"/>
       <c r="C10" s="79"/>
-      <c r="D10" s="251"/>
+      <c r="D10" s="206"/>
       <c r="E10" s="79"/>
       <c r="F10" s="145">
         <f t="shared" si="0"/>
@@ -10472,10 +10535,10 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A30:G52"/>
+  <dimension ref="A23:G53"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="G46" sqref="G46:G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10487,65 +10550,49 @@
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="163"/>
-      <c r="B44" s="236" t="s">
+    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="163"/>
+      <c r="B45" s="249" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="237"/>
-      <c r="D44" s="237"/>
-      <c r="E44" s="238"/>
-      <c r="F44" s="3"/>
-    </row>
-    <row r="45" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="170">
-        <v>44439</v>
-      </c>
-      <c r="B45" s="171" t="s">
-        <v>74</v>
-      </c>
-      <c r="C45" s="172">
-        <v>140</v>
-      </c>
-      <c r="D45" s="173" t="s">
+      <c r="C45" s="250"/>
+      <c r="D45" s="250"/>
+      <c r="E45" s="251"/>
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="170">
+        <v>44454</v>
+      </c>
+      <c r="B46" s="171" t="s">
+        <v>122</v>
+      </c>
+      <c r="C46" s="172">
+        <v>304.5</v>
+      </c>
+      <c r="D46" s="173" t="s">
         <v>32</v>
       </c>
-      <c r="E45" s="174" t="s">
-        <v>48</v>
-      </c>
-      <c r="F45" s="107">
-        <v>0</v>
-      </c>
-      <c r="G45" s="239" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="170"/>
-      <c r="B46" s="171" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="172">
-        <v>0</v>
-      </c>
-      <c r="D46" s="175" t="s">
-        <v>32</v>
-      </c>
       <c r="E46" s="174" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="F46" s="107">
-        <v>0</v>
-      </c>
-      <c r="G46" s="240"/>
-    </row>
-    <row r="47" spans="1:7" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+      <c r="G46" s="252"/>
+    </row>
+    <row r="47" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="170"/>
       <c r="B47" s="171" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C47" s="172">
         <v>0</v>
@@ -10553,12 +10600,13 @@
       <c r="D47" s="175" t="s">
         <v>32</v>
       </c>
-      <c r="E47" s="179" t="s">
+      <c r="E47" s="174" t="s">
         <v>33</v>
       </c>
       <c r="F47" s="107">
         <v>0</v>
       </c>
+      <c r="G47" s="253"/>
     </row>
     <row r="48" spans="1:7" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="170"/>
@@ -10578,15 +10626,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="164"/>
-      <c r="B49" s="165" t="s">
+    <row r="49" spans="1:6" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="170"/>
+      <c r="B49" s="171" t="s">
         <v>33</v>
       </c>
-      <c r="C49" s="166">
-        <v>0</v>
-      </c>
-      <c r="D49" s="167" t="s">
+      <c r="C49" s="172">
+        <v>0</v>
+      </c>
+      <c r="D49" s="175" t="s">
         <v>32</v>
       </c>
       <c r="E49" s="179" t="s">
@@ -10632,15 +10680,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="168"/>
+    <row r="52" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="164"/>
       <c r="B52" s="165" t="s">
         <v>33</v>
       </c>
       <c r="C52" s="166">
         <v>0</v>
       </c>
-      <c r="D52" s="169" t="s">
+      <c r="D52" s="167" t="s">
         <v>32</v>
       </c>
       <c r="E52" s="179" t="s">
@@ -10650,12 +10698,30 @@
         <v>0</v>
       </c>
     </row>
+    <row r="53" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="168"/>
+      <c r="B53" s="165" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="166">
+        <v>0</v>
+      </c>
+      <c r="D53" s="169" t="s">
+        <v>32</v>
+      </c>
+      <c r="E53" s="179" t="s">
+        <v>33</v>
+      </c>
+      <c r="F53" s="107">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="G46:G47"/>
   </mergeCells>
-  <pageMargins left="0.39" right="0.13" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.39" right="0.13" top="0.75" bottom="0.27" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CIERRE 27 SEPT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE  HERRADURA  SEPTIEMBRE   2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE  HERRADURA  SEPTIEMBRE   2021.xlsx
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="152">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -520,6 +520,87 @@
   </si>
   <si>
     <t>CONCHA RES--CHAMBARETE</t>
+  </si>
+  <si>
+    <t>19041 B</t>
+  </si>
+  <si>
+    <t>19190 B</t>
+  </si>
+  <si>
+    <t>19307 B</t>
+  </si>
+  <si>
+    <t>19309 B</t>
+  </si>
+  <si>
+    <t>19417 B</t>
+  </si>
+  <si>
+    <t>19430 B</t>
+  </si>
+  <si>
+    <t>19431 B</t>
+  </si>
+  <si>
+    <t>19561 B</t>
+  </si>
+  <si>
+    <t>19563 B</t>
+  </si>
+  <si>
+    <t>19682 B</t>
+  </si>
+  <si>
+    <t>19731 B</t>
+  </si>
+  <si>
+    <t>19791 B</t>
+  </si>
+  <si>
+    <t>19884 B</t>
+  </si>
+  <si>
+    <t>19890 B</t>
+  </si>
+  <si>
+    <t>19944 B</t>
+  </si>
+  <si>
+    <t>20028 B</t>
+  </si>
+  <si>
+    <t>20029 B</t>
+  </si>
+  <si>
+    <t>20164 B</t>
+  </si>
+  <si>
+    <t>20203 B</t>
+  </si>
+  <si>
+    <t>20260 B</t>
+  </si>
+  <si>
+    <t>20262 B</t>
+  </si>
+  <si>
+    <t>20270 B</t>
+  </si>
+  <si>
+    <t>20412 B</t>
+  </si>
+  <si>
+    <t>20443 B</t>
+  </si>
+  <si>
+    <t>20493 B</t>
+  </si>
+  <si>
+    <t>CHULETA-QUIESOS-TOCINO-BOLSAS</t>
+  </si>
+  <si>
+    <t>NOMINA # 38</t>
   </si>
 </sst>
 </file>
@@ -2058,6 +2139,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="167" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2190,7 +2272,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -3336,7 +3417,7 @@
   </sheetPr>
   <dimension ref="A1:R80"/>
   <sheetViews>
-    <sheetView topLeftCell="G31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
@@ -3359,23 +3440,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="235"/>
-      <c r="C1" s="244" t="s">
+      <c r="B1" s="236"/>
+      <c r="C1" s="245" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
-      <c r="M1" s="245"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
+      <c r="H1" s="246"/>
+      <c r="I1" s="246"/>
+      <c r="J1" s="246"/>
+      <c r="K1" s="246"/>
+      <c r="L1" s="246"/>
+      <c r="M1" s="246"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="236"/>
+      <c r="B2" s="237"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -3385,17 +3466,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="237" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="238"/>
+      <c r="B3" s="238" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="239"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="239" t="s">
+      <c r="H3" s="240" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="239"/>
+      <c r="I3" s="240"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -3411,14 +3492,14 @@
       <c r="D4" s="16">
         <v>44410</v>
       </c>
-      <c r="E4" s="240" t="s">
+      <c r="E4" s="241" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="241"/>
-      <c r="H4" s="242" t="s">
+      <c r="F4" s="242"/>
+      <c r="H4" s="243" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="243"/>
+      <c r="I4" s="244"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -3428,10 +3509,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="229" t="s">
+      <c r="P4" s="230" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="230"/>
+      <c r="Q4" s="231"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -4926,11 +5007,11 @@
       <c r="L39" s="69">
         <v>454.62</v>
       </c>
-      <c r="M39" s="231">
+      <c r="M39" s="232">
         <f>SUM(M5:M38)</f>
         <v>1393675.5</v>
       </c>
-      <c r="N39" s="233">
+      <c r="N39" s="234">
         <f>SUM(N5:N38)</f>
         <v>28399.97</v>
       </c>
@@ -4962,8 +5043,8 @@
       <c r="L40" s="69">
         <v>1195.67</v>
       </c>
-      <c r="M40" s="232"/>
-      <c r="N40" s="234"/>
+      <c r="M40" s="233"/>
+      <c r="N40" s="235"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -5196,29 +5277,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="219" t="s">
+      <c r="H52" s="220" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="220"/>
+      <c r="I52" s="221"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="221">
+      <c r="K52" s="222">
         <f>I50+L50</f>
         <v>80916.84</v>
       </c>
-      <c r="L52" s="222"/>
-      <c r="M52" s="210">
+      <c r="L52" s="223"/>
+      <c r="M52" s="211">
         <f>N39+M39</f>
         <v>1422075.47</v>
       </c>
-      <c r="N52" s="211"/>
+      <c r="N52" s="212"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="223" t="s">
+      <c r="D53" s="224" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="223"/>
+      <c r="E53" s="224"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1396181.44</v>
@@ -5229,22 +5310,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="224" t="s">
+      <c r="D54" s="225" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="224"/>
+      <c r="E54" s="225"/>
       <c r="F54" s="102">
         <v>-1523111</v>
       </c>
-      <c r="I54" s="225" t="s">
+      <c r="I54" s="226" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="226"/>
-      <c r="K54" s="227">
+      <c r="J54" s="227"/>
+      <c r="K54" s="228">
         <f>F56+F57+F58</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L54" s="228"/>
+      <c r="L54" s="229"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -5275,10 +5356,10 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="212">
-        <v>0</v>
-      </c>
-      <c r="L56" s="213"/>
+      <c r="K56" s="213">
+        <v>0</v>
+      </c>
+      <c r="L56" s="214"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -5295,22 +5376,22 @@
       <c r="C58" s="120">
         <v>44444</v>
       </c>
-      <c r="D58" s="214" t="s">
+      <c r="D58" s="215" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="215"/>
+      <c r="E58" s="216"/>
       <c r="F58" s="121">
         <v>136234.76999999999</v>
       </c>
-      <c r="I58" s="216" t="s">
+      <c r="I58" s="217" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="217"/>
-      <c r="K58" s="218">
+      <c r="J58" s="218"/>
+      <c r="K58" s="219">
         <f>K54+K56</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L58" s="218"/>
+      <c r="L58" s="219"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -5489,8 +5570,8 @@
   </sheetPr>
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView topLeftCell="A44" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5545,7 +5626,7 @@
       <c r="C3" s="35">
         <v>3015.96</v>
       </c>
-      <c r="D3" s="246" t="s">
+      <c r="D3" s="247" t="s">
         <v>50</v>
       </c>
       <c r="E3" s="9"/>
@@ -5564,7 +5645,7 @@
       <c r="C4" s="35">
         <v>10281</v>
       </c>
-      <c r="D4" s="247"/>
+      <c r="D4" s="248"/>
       <c r="E4" s="183"/>
       <c r="F4" s="145">
         <f>F3+C4-E4</f>
@@ -5582,7 +5663,7 @@
       <c r="C5" s="35">
         <v>12746.2</v>
       </c>
-      <c r="D5" s="247"/>
+      <c r="D5" s="248"/>
       <c r="E5" s="183"/>
       <c r="F5" s="145">
         <f t="shared" ref="F5:F68" si="0">F4+C5-E5</f>
@@ -5599,7 +5680,7 @@
       <c r="C6" s="35">
         <v>28974.78</v>
       </c>
-      <c r="D6" s="247"/>
+      <c r="D6" s="248"/>
       <c r="E6" s="183"/>
       <c r="F6" s="145">
         <f t="shared" si="0"/>
@@ -5616,7 +5697,7 @@
       <c r="C7" s="35">
         <v>44758.6</v>
       </c>
-      <c r="D7" s="247"/>
+      <c r="D7" s="248"/>
       <c r="E7" s="183"/>
       <c r="F7" s="145">
         <f t="shared" si="0"/>
@@ -5633,7 +5714,7 @@
       <c r="C8" s="35">
         <v>12841.78</v>
       </c>
-      <c r="D8" s="247"/>
+      <c r="D8" s="248"/>
       <c r="E8" s="183"/>
       <c r="F8" s="145">
         <f t="shared" si="0"/>
@@ -5650,7 +5731,7 @@
       <c r="C9" s="35">
         <v>3898.05</v>
       </c>
-      <c r="D9" s="247"/>
+      <c r="D9" s="248"/>
       <c r="E9" s="183"/>
       <c r="F9" s="145">
         <f t="shared" si="0"/>
@@ -5667,7 +5748,7 @@
       <c r="C10" s="35">
         <v>1429</v>
       </c>
-      <c r="D10" s="248"/>
+      <c r="D10" s="249"/>
       <c r="E10" s="183"/>
       <c r="F10" s="145">
         <f t="shared" si="0"/>
@@ -6270,13 +6351,13 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="190">
+      <c r="A45" s="144">
         <v>44438</v>
       </c>
-      <c r="B45" s="188" t="s">
+      <c r="B45" s="142" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="189">
+      <c r="C45" s="79">
         <v>59828.6</v>
       </c>
       <c r="D45" s="144"/>
@@ -6287,13 +6368,13 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="190">
+      <c r="A46" s="144">
         <v>44438</v>
       </c>
-      <c r="B46" s="188" t="s">
+      <c r="B46" s="142" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="189">
+      <c r="C46" s="79">
         <v>7936</v>
       </c>
       <c r="D46" s="144"/>
@@ -6304,13 +6385,13 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="190">
+      <c r="A47" s="144">
         <v>44439</v>
       </c>
-      <c r="B47" s="188" t="s">
+      <c r="B47" s="142" t="s">
         <v>95</v>
       </c>
-      <c r="C47" s="189">
+      <c r="C47" s="79">
         <v>51630.5</v>
       </c>
       <c r="D47" s="144"/>
@@ -6321,13 +6402,13 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="190">
+      <c r="A48" s="144">
         <v>44439</v>
       </c>
-      <c r="B48" s="188" t="s">
+      <c r="B48" s="142" t="s">
         <v>96</v>
       </c>
-      <c r="C48" s="189">
+      <c r="C48" s="79">
         <v>8998</v>
       </c>
       <c r="D48" s="144"/>
@@ -6338,13 +6419,13 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="190">
+      <c r="A49" s="144">
         <v>44440</v>
       </c>
-      <c r="B49" s="188" t="s">
+      <c r="B49" s="142" t="s">
         <v>97</v>
       </c>
-      <c r="C49" s="189">
+      <c r="C49" s="79">
         <v>19868.599999999999</v>
       </c>
       <c r="D49" s="144"/>
@@ -6355,13 +6436,13 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="190">
+      <c r="A50" s="144">
         <v>44441</v>
       </c>
-      <c r="B50" s="188" t="s">
+      <c r="B50" s="142" t="s">
         <v>98</v>
       </c>
-      <c r="C50" s="189">
+      <c r="C50" s="79">
         <v>45543.199999999997</v>
       </c>
       <c r="D50" s="144"/>
@@ -6372,13 +6453,13 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="190">
+      <c r="A51" s="144">
         <v>44441</v>
       </c>
-      <c r="B51" s="188" t="s">
+      <c r="B51" s="142" t="s">
         <v>99</v>
       </c>
-      <c r="C51" s="189">
+      <c r="C51" s="79">
         <v>3212.58</v>
       </c>
       <c r="D51" s="144"/>
@@ -6389,13 +6470,13 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="190">
+      <c r="A52" s="144">
         <v>44441</v>
       </c>
-      <c r="B52" s="188" t="s">
+      <c r="B52" s="142" t="s">
         <v>100</v>
       </c>
-      <c r="C52" s="189">
+      <c r="C52" s="79">
         <v>4028.6</v>
       </c>
       <c r="D52" s="144"/>
@@ -6406,13 +6487,13 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="190">
+      <c r="A53" s="144">
         <v>44442</v>
       </c>
-      <c r="B53" s="188" t="s">
+      <c r="B53" s="142" t="s">
         <v>101</v>
       </c>
-      <c r="C53" s="189">
+      <c r="C53" s="79">
         <v>101013.65</v>
       </c>
       <c r="D53" s="144"/>
@@ -6423,13 +6504,13 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="191">
+      <c r="A54" s="141">
         <v>44443</v>
       </c>
-      <c r="B54" s="188" t="s">
+      <c r="B54" s="142" t="s">
         <v>102</v>
       </c>
-      <c r="C54" s="189">
+      <c r="C54" s="79">
         <v>35635.89</v>
       </c>
       <c r="D54" s="144"/>
@@ -6440,13 +6521,13 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="191">
+      <c r="A55" s="141">
         <v>44443</v>
       </c>
-      <c r="B55" s="188" t="s">
+      <c r="B55" s="142" t="s">
         <v>103</v>
       </c>
-      <c r="C55" s="189">
+      <c r="C55" s="79">
         <v>691.2</v>
       </c>
       <c r="D55" s="144"/>
@@ -6457,92 +6538,100 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="191">
+      <c r="A56" s="141">
         <v>44444</v>
       </c>
-      <c r="B56" s="188">
+      <c r="B56" s="142">
         <v>18966</v>
       </c>
-      <c r="C56" s="189">
+      <c r="C56" s="79">
         <v>4784.3500000000004</v>
       </c>
-      <c r="D56" s="144"/>
-      <c r="E56" s="79"/>
+      <c r="D56" s="144">
+        <v>44449</v>
+      </c>
+      <c r="E56" s="79">
+        <v>343171.17</v>
+      </c>
       <c r="F56" s="145">
         <f t="shared" si="0"/>
-        <v>343171.17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="190">
+      <c r="A57" s="144">
         <v>44444</v>
       </c>
-      <c r="B57" s="188" t="s">
+      <c r="B57" s="142" t="s">
         <v>104</v>
       </c>
-      <c r="C57" s="189">
+      <c r="C57" s="79">
         <v>43121.2</v>
       </c>
-      <c r="D57" s="144"/>
-      <c r="E57" s="79"/>
+      <c r="D57" s="144">
+        <v>44456</v>
+      </c>
+      <c r="E57" s="79">
+        <v>43121.2</v>
+      </c>
       <c r="F57" s="145">
         <f t="shared" si="0"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="190"/>
-      <c r="B58" s="188"/>
-      <c r="C58" s="189"/>
+      <c r="A58" s="144"/>
+      <c r="B58" s="142"/>
+      <c r="C58" s="79"/>
       <c r="D58" s="144"/>
       <c r="E58" s="79"/>
       <c r="F58" s="145">
         <f t="shared" si="0"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="190"/>
-      <c r="B59" s="188"/>
-      <c r="C59" s="189"/>
+      <c r="A59" s="144"/>
+      <c r="B59" s="142"/>
+      <c r="C59" s="79"/>
       <c r="D59" s="144"/>
       <c r="E59" s="79"/>
       <c r="F59" s="145">
         <f t="shared" si="0"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="191"/>
-      <c r="B60" s="188"/>
-      <c r="C60" s="189"/>
+      <c r="A60" s="141"/>
+      <c r="B60" s="142"/>
+      <c r="C60" s="79"/>
       <c r="D60" s="144"/>
       <c r="E60" s="79"/>
       <c r="F60" s="145">
         <f t="shared" si="0"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="191"/>
-      <c r="B61" s="188"/>
-      <c r="C61" s="189"/>
+      <c r="A61" s="141"/>
+      <c r="B61" s="142"/>
+      <c r="C61" s="79"/>
       <c r="D61" s="144"/>
       <c r="E61" s="79"/>
       <c r="F61" s="145">
         <f t="shared" si="0"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="191"/>
-      <c r="B62" s="188"/>
-      <c r="C62" s="189"/>
+      <c r="A62" s="141"/>
+      <c r="B62" s="142"/>
+      <c r="C62" s="79"/>
       <c r="D62" s="144"/>
       <c r="E62" s="79"/>
       <c r="F62" s="145">
         <f t="shared" si="0"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -6553,7 +6642,7 @@
       <c r="E63" s="79"/>
       <c r="F63" s="145">
         <f t="shared" si="0"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6564,7 +6653,7 @@
       <c r="E64" s="79"/>
       <c r="F64" s="145">
         <f t="shared" si="0"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6575,7 +6664,7 @@
       <c r="E65" s="79"/>
       <c r="F65" s="145">
         <f t="shared" si="0"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6586,7 +6675,7 @@
       <c r="E66" s="79"/>
       <c r="F66" s="145">
         <f t="shared" si="0"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6597,7 +6686,7 @@
       <c r="E67" s="79"/>
       <c r="F67" s="145">
         <f t="shared" si="0"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6608,7 +6697,7 @@
       <c r="E68" s="79"/>
       <c r="F68" s="145">
         <f t="shared" si="0"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6619,7 +6708,7 @@
       <c r="E69" s="79"/>
       <c r="F69" s="145">
         <f t="shared" ref="F69:F97" si="1">F68+C69-E69</f>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6630,7 +6719,7 @@
       <c r="E70" s="79"/>
       <c r="F70" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6641,7 +6730,7 @@
       <c r="E71" s="79"/>
       <c r="F71" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6652,7 +6741,7 @@
       <c r="E72" s="79"/>
       <c r="F72" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6663,7 +6752,7 @@
       <c r="E73" s="79"/>
       <c r="F73" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6674,7 +6763,7 @@
       <c r="E74" s="79"/>
       <c r="F74" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6685,7 +6774,7 @@
       <c r="E75" s="79"/>
       <c r="F75" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6696,7 +6785,7 @@
       <c r="E76" s="79"/>
       <c r="F76" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6707,7 +6796,7 @@
       <c r="E77" s="79"/>
       <c r="F77" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6718,7 +6807,7 @@
       <c r="E78" s="79"/>
       <c r="F78" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6729,7 +6818,7 @@
       <c r="E79" s="79"/>
       <c r="F79" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6740,7 +6829,7 @@
       <c r="E80" s="79"/>
       <c r="F80" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6751,7 +6840,7 @@
       <c r="E81" s="83"/>
       <c r="F81" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6762,7 +6851,7 @@
       <c r="E82" s="83"/>
       <c r="F82" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6773,7 +6862,7 @@
       <c r="E83" s="83"/>
       <c r="F83" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6784,7 +6873,7 @@
       <c r="E84" s="83"/>
       <c r="F84" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6795,7 +6884,7 @@
       <c r="E85" s="83"/>
       <c r="F85" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6806,7 +6895,7 @@
       <c r="E86" s="83"/>
       <c r="F86" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6817,7 +6906,7 @@
       <c r="E87" s="79"/>
       <c r="F87" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6828,7 +6917,7 @@
       <c r="E88" s="79"/>
       <c r="F88" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6839,7 +6928,7 @@
       <c r="E89" s="79"/>
       <c r="F89" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6850,7 +6939,7 @@
       <c r="E90" s="79"/>
       <c r="F90" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6861,7 +6950,7 @@
       <c r="E91" s="79"/>
       <c r="F91" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6872,7 +6961,7 @@
       <c r="E92" s="79"/>
       <c r="F92" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6883,7 +6972,7 @@
       <c r="E93" s="79"/>
       <c r="F93" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6894,7 +6983,7 @@
       <c r="E94" s="79"/>
       <c r="F94" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6905,7 +6994,7 @@
       <c r="E95" s="79"/>
       <c r="F95" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -6916,7 +7005,7 @@
       <c r="E96" s="79"/>
       <c r="F96" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6929,7 +7018,7 @@
       <c r="E97" s="151"/>
       <c r="F97" s="145">
         <f t="shared" si="1"/>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -6941,11 +7030,11 @@
       <c r="D98" s="103"/>
       <c r="E98" s="3">
         <f>SUM(E3:E97)</f>
-        <v>1136818.6299999999</v>
+        <v>1523110.9999999998</v>
       </c>
       <c r="F98" s="153">
         <f>F97</f>
-        <v>386292.37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -7156,8 +7245,8 @@
   </sheetPr>
   <dimension ref="A1:R80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7179,23 +7268,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="235"/>
-      <c r="C1" s="244" t="s">
+      <c r="B1" s="236"/>
+      <c r="C1" s="245" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="245"/>
-      <c r="J1" s="245"/>
-      <c r="K1" s="245"/>
-      <c r="L1" s="245"/>
-      <c r="M1" s="245"/>
+      <c r="D1" s="246"/>
+      <c r="E1" s="246"/>
+      <c r="F1" s="246"/>
+      <c r="G1" s="246"/>
+      <c r="H1" s="246"/>
+      <c r="I1" s="246"/>
+      <c r="J1" s="246"/>
+      <c r="K1" s="246"/>
+      <c r="L1" s="246"/>
+      <c r="M1" s="246"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="236"/>
+      <c r="B2" s="237"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -7205,17 +7294,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="237" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="238"/>
+      <c r="B3" s="238" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="239"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="239" t="s">
+      <c r="H3" s="240" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="239"/>
+      <c r="I3" s="240"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -7231,14 +7320,14 @@
       <c r="D4" s="16">
         <v>44444</v>
       </c>
-      <c r="E4" s="240" t="s">
+      <c r="E4" s="241" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="241"/>
-      <c r="H4" s="242" t="s">
+      <c r="F4" s="242"/>
+      <c r="H4" s="243" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="243"/>
+      <c r="I4" s="244"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -7248,10 +7337,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="229" t="s">
+      <c r="P4" s="230" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="230"/>
+      <c r="Q4" s="231"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -7596,7 +7685,7 @@
       <c r="N12" s="30">
         <v>2198</v>
       </c>
-      <c r="O12" s="254"/>
+      <c r="O12" s="210"/>
       <c r="P12" s="83">
         <f t="shared" si="0"/>
         <v>46630</v>
@@ -7721,19 +7810,19 @@
       <c r="K15" s="40"/>
       <c r="L15" s="35"/>
       <c r="M15" s="138">
-        <f>25000</f>
-        <v>25000</v>
+        <f>25000+20919</f>
+        <v>45919</v>
       </c>
       <c r="N15" s="30">
         <v>0</v>
       </c>
       <c r="P15" s="83">
         <f t="shared" si="0"/>
-        <v>25000</v>
+        <v>45919</v>
       </c>
       <c r="Q15" s="9">
         <f t="shared" si="1"/>
-        <v>-20919</v>
+        <v>0</v>
       </c>
       <c r="R15" s="26"/>
     </row>
@@ -7750,7 +7839,7 @@
         <v>44456</v>
       </c>
       <c r="F16" s="25">
-        <v>0</v>
+        <v>77820</v>
       </c>
       <c r="G16" s="26"/>
       <c r="H16" s="32">
@@ -7763,18 +7852,19 @@
       <c r="K16" s="40"/>
       <c r="L16" s="9"/>
       <c r="M16" s="138">
-        <v>0</v>
+        <f>55000+17820</f>
+        <v>72820</v>
       </c>
       <c r="N16" s="30">
         <v>0</v>
       </c>
       <c r="P16" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>72820</v>
       </c>
       <c r="Q16" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-5000</v>
       </c>
       <c r="R16" s="26"/>
     </row>
@@ -7784,14 +7874,16 @@
         <v>44426</v>
       </c>
       <c r="C17" s="22">
-        <v>0</v>
-      </c>
-      <c r="D17" s="38"/>
+        <v>3060</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>150</v>
+      </c>
       <c r="E17" s="24">
         <v>44457</v>
       </c>
       <c r="F17" s="25">
-        <v>0</v>
+        <v>66071</v>
       </c>
       <c r="G17" s="26"/>
       <c r="H17" s="32">
@@ -7800,22 +7892,29 @@
       <c r="I17" s="28">
         <v>0</v>
       </c>
-      <c r="J17" s="33"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="43"/>
+      <c r="J17" s="33">
+        <v>44457</v>
+      </c>
+      <c r="K17" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="L17" s="43">
+        <v>15042.86</v>
+      </c>
       <c r="M17" s="138">
-        <v>0</v>
+        <f>35000+8825</f>
+        <v>43825</v>
       </c>
       <c r="N17" s="30">
-        <v>0</v>
+        <v>4144</v>
       </c>
       <c r="P17" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>66071.86</v>
       </c>
       <c r="Q17" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.86000000000058208</v>
       </c>
       <c r="R17" s="26"/>
     </row>
@@ -8671,21 +8770,21 @@
       <c r="J39" s="67"/>
       <c r="K39" s="82"/>
       <c r="L39" s="69"/>
-      <c r="M39" s="231">
+      <c r="M39" s="232">
         <f>SUM(M5:M38)</f>
-        <v>452501</v>
-      </c>
-      <c r="N39" s="233">
+        <v>590065</v>
+      </c>
+      <c r="N39" s="234">
         <f>SUM(N5:N38)</f>
-        <v>15436</v>
+        <v>19580</v>
       </c>
       <c r="P39" s="83">
         <f>SUM(P5:P38)</f>
-        <v>503147.29000000004</v>
+        <v>662958.15</v>
       </c>
       <c r="Q39" s="9">
         <f>SUM(Q5:Q38)</f>
-        <v>-20908.71</v>
+        <v>-4988.8499999999985</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -8701,8 +8800,8 @@
       <c r="J40" s="67"/>
       <c r="K40" s="71"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="232"/>
-      <c r="N40" s="234"/>
+      <c r="M40" s="233"/>
+      <c r="N40" s="235"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -8875,7 +8974,7 @@
       </c>
       <c r="C50" s="93">
         <f>SUM(C5:C49)</f>
-        <v>18204</v>
+        <v>21264</v>
       </c>
       <c r="D50" s="94"/>
       <c r="E50" s="95" t="s">
@@ -8883,7 +8982,7 @@
       </c>
       <c r="F50" s="96">
         <f>SUM(F5:F49)</f>
-        <v>524056</v>
+        <v>667947</v>
       </c>
       <c r="G50" s="94"/>
       <c r="H50" s="97" t="s">
@@ -8899,7 +8998,7 @@
       </c>
       <c r="L50" s="101">
         <f>SUM(L5:L49)</f>
-        <v>11014.29</v>
+        <v>26057.15</v>
       </c>
       <c r="M50" s="102"/>
       <c r="N50" s="102"/>
@@ -8917,32 +9016,32 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="219" t="s">
+      <c r="H52" s="220" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="220"/>
+      <c r="I52" s="221"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="221">
+      <c r="K52" s="222">
         <f>I50+L50</f>
-        <v>17006.29</v>
-      </c>
-      <c r="L52" s="222"/>
-      <c r="M52" s="210">
+        <v>32049.15</v>
+      </c>
+      <c r="L52" s="223"/>
+      <c r="M52" s="211">
         <f>N39+M39</f>
-        <v>467937</v>
-      </c>
-      <c r="N52" s="211"/>
+        <v>609645</v>
+      </c>
+      <c r="N52" s="212"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="223" t="s">
+      <c r="D53" s="224" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="223"/>
+      <c r="E53" s="224"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
-        <v>488845.71</v>
+        <v>614633.85</v>
       </c>
       <c r="I53" s="108"/>
       <c r="J53" s="109"/>
@@ -8950,22 +9049,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="224" t="s">
+      <c r="D54" s="225" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="224"/>
+      <c r="E54" s="225"/>
       <c r="F54" s="102">
         <v>0</v>
       </c>
-      <c r="I54" s="225" t="s">
+      <c r="I54" s="226" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="226"/>
-      <c r="K54" s="227">
+      <c r="J54" s="227"/>
+      <c r="K54" s="228">
         <f>F56+F57+F58</f>
-        <v>488845.71</v>
-      </c>
-      <c r="L54" s="228"/>
+        <v>614633.85</v>
+      </c>
+      <c r="L54" s="229"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -8989,17 +9088,17 @@
       </c>
       <c r="F56" s="102">
         <f>SUM(F53:F55)</f>
-        <v>488845.71</v>
+        <v>614633.85</v>
       </c>
       <c r="H56" s="20"/>
       <c r="I56" s="116" t="s">
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="212">
-        <v>0</v>
-      </c>
-      <c r="L56" s="213"/>
+      <c r="K56" s="213">
+        <v>0</v>
+      </c>
+      <c r="L56" s="214"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -9014,22 +9113,22 @@
     </row>
     <row r="58" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C58" s="120"/>
-      <c r="D58" s="214" t="s">
+      <c r="D58" s="215" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="215"/>
+      <c r="E58" s="216"/>
       <c r="F58" s="121">
         <v>0</v>
       </c>
-      <c r="I58" s="216" t="s">
+      <c r="I58" s="217" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="217"/>
-      <c r="K58" s="218">
+      <c r="J58" s="218"/>
+      <c r="K58" s="219">
         <f>K54+K56</f>
-        <v>488845.71</v>
-      </c>
-      <c r="L58" s="218"/>
+        <v>614633.85</v>
+      </c>
+      <c r="L58" s="219"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -9208,8 +9307,8 @@
   </sheetPr>
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9255,292 +9354,456 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="141"/>
-      <c r="B3" s="182"/>
-      <c r="C3" s="79"/>
+      <c r="A3" s="141">
+        <v>44445</v>
+      </c>
+      <c r="B3" s="182" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="79">
+        <v>42896.2</v>
+      </c>
       <c r="D3" s="206"/>
       <c r="E3" s="79"/>
       <c r="F3" s="143">
         <f>C3-E3</f>
-        <v>0</v>
+        <v>42896.2</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="141"/>
-      <c r="B4" s="182"/>
-      <c r="C4" s="79"/>
+      <c r="A4" s="141">
+        <v>44446</v>
+      </c>
+      <c r="B4" s="182" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="79">
+        <v>673.2</v>
+      </c>
       <c r="D4" s="206"/>
       <c r="E4" s="79"/>
       <c r="F4" s="145">
         <f>F3+C4-E4</f>
-        <v>0</v>
+        <v>43569.399999999994</v>
       </c>
       <c r="G4" s="146"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="141"/>
-      <c r="B5" s="182"/>
-      <c r="C5" s="79"/>
+      <c r="A5" s="141">
+        <v>44447</v>
+      </c>
+      <c r="B5" s="182" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="79">
+        <v>59000.22</v>
+      </c>
       <c r="D5" s="206"/>
       <c r="E5" s="79"/>
       <c r="F5" s="145">
         <f t="shared" ref="F5:F68" si="0">F4+C5-E5</f>
-        <v>0</v>
+        <v>102569.62</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="141"/>
-      <c r="B6" s="182"/>
-      <c r="C6" s="79"/>
+      <c r="A6" s="141">
+        <v>44447</v>
+      </c>
+      <c r="B6" s="182" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="79">
+        <v>11075.4</v>
+      </c>
       <c r="D6" s="206"/>
       <c r="E6" s="79"/>
       <c r="F6" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>113645.01999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="141"/>
-      <c r="B7" s="182"/>
-      <c r="C7" s="79"/>
+      <c r="A7" s="141">
+        <v>44448</v>
+      </c>
+      <c r="B7" s="182" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="79">
+        <v>8608.6</v>
+      </c>
       <c r="D7" s="206"/>
       <c r="E7" s="79"/>
       <c r="F7" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>122253.62</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="141"/>
-      <c r="B8" s="182"/>
-      <c r="C8" s="79"/>
+      <c r="A8" s="141">
+        <v>44448</v>
+      </c>
+      <c r="B8" s="182" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="79">
+        <v>45033.9</v>
+      </c>
       <c r="D8" s="206"/>
       <c r="E8" s="79"/>
       <c r="F8" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>167287.51999999999</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="141"/>
-      <c r="B9" s="182"/>
-      <c r="C9" s="79"/>
+      <c r="A9" s="141">
+        <v>44448</v>
+      </c>
+      <c r="B9" s="182" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="79">
+        <v>2191.8000000000002</v>
+      </c>
       <c r="D9" s="206"/>
       <c r="E9" s="79"/>
       <c r="F9" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>169479.31999999998</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="141"/>
-      <c r="B10" s="182"/>
-      <c r="C10" s="79"/>
+      <c r="A10" s="141">
+        <v>44449</v>
+      </c>
+      <c r="B10" s="182" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="79">
+        <v>6894.34</v>
+      </c>
       <c r="D10" s="206"/>
       <c r="E10" s="79"/>
       <c r="F10" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>176373.65999999997</v>
       </c>
       <c r="G10" s="146"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="141"/>
-      <c r="B11" s="142"/>
-      <c r="C11" s="79"/>
+      <c r="A11" s="141">
+        <v>44449</v>
+      </c>
+      <c r="B11" s="142" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="79">
+        <v>12957.4</v>
+      </c>
       <c r="D11" s="144"/>
       <c r="E11" s="79"/>
       <c r="F11" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>189331.05999999997</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="144"/>
-      <c r="B12" s="142"/>
-      <c r="C12" s="79"/>
+      <c r="A12" s="144">
+        <v>44450</v>
+      </c>
+      <c r="B12" s="142" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" s="79">
+        <v>88426.6</v>
+      </c>
       <c r="D12" s="144"/>
       <c r="E12" s="79"/>
       <c r="F12" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>277757.65999999997</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="144"/>
-      <c r="B13" s="142"/>
-      <c r="C13" s="79"/>
+      <c r="A13" s="144">
+        <v>44451</v>
+      </c>
+      <c r="B13" s="142" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" s="79">
+        <v>789.96</v>
+      </c>
       <c r="D13" s="144"/>
       <c r="E13" s="79"/>
       <c r="F13" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>278547.62</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="144"/>
-      <c r="B14" s="142"/>
-      <c r="C14" s="79"/>
+      <c r="A14" s="144">
+        <v>44452</v>
+      </c>
+      <c r="B14" s="142" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="79">
+        <v>41682.5</v>
+      </c>
       <c r="D14" s="144"/>
       <c r="E14" s="79"/>
       <c r="F14" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>320230.12</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="144"/>
-      <c r="B15" s="142"/>
-      <c r="C15" s="79"/>
-      <c r="D15" s="144"/>
-      <c r="E15" s="79"/>
+      <c r="A15" s="144">
+        <v>44452</v>
+      </c>
+      <c r="B15" s="142" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="79">
+        <v>21216.5</v>
+      </c>
+      <c r="D15" s="144">
+        <v>44456</v>
+      </c>
+      <c r="E15" s="79">
+        <v>336878.8</v>
+      </c>
       <c r="F15" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4567.820000000007</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="144"/>
-      <c r="B16" s="142"/>
-      <c r="C16" s="79"/>
+      <c r="A16" s="144">
+        <v>44452</v>
+      </c>
+      <c r="B16" s="142" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="79">
+        <v>13948.78</v>
+      </c>
       <c r="D16" s="144"/>
       <c r="E16" s="79"/>
       <c r="F16" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18516.600000000006</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="144"/>
-      <c r="B17" s="142"/>
-      <c r="C17" s="79"/>
+      <c r="A17" s="144">
+        <v>44453</v>
+      </c>
+      <c r="B17" s="142" t="s">
+        <v>139</v>
+      </c>
+      <c r="C17" s="79">
+        <v>69059.98</v>
+      </c>
       <c r="D17" s="144"/>
       <c r="E17" s="79"/>
       <c r="F17" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>87576.58</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="144"/>
-      <c r="B18" s="142"/>
-      <c r="C18" s="79"/>
+      <c r="A18" s="144">
+        <v>44453</v>
+      </c>
+      <c r="B18" s="142" t="s">
+        <v>140</v>
+      </c>
+      <c r="C18" s="79">
+        <v>23621.5</v>
+      </c>
       <c r="D18" s="144"/>
       <c r="E18" s="79"/>
       <c r="F18" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>111198.08</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="144"/>
-      <c r="B19" s="142"/>
-      <c r="C19" s="79"/>
+      <c r="A19" s="144">
+        <v>44453</v>
+      </c>
+      <c r="B19" s="142" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" s="79">
+        <v>10612.8</v>
+      </c>
       <c r="D19" s="144"/>
       <c r="E19" s="79"/>
       <c r="F19" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>121810.88</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="144"/>
-      <c r="B20" s="142"/>
-      <c r="C20" s="79"/>
+      <c r="A20" s="144">
+        <v>44455</v>
+      </c>
+      <c r="B20" s="142" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" s="79">
+        <v>5853.76</v>
+      </c>
       <c r="D20" s="144"/>
       <c r="E20" s="79"/>
       <c r="F20" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>127664.64</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="144"/>
-      <c r="B21" s="142"/>
-      <c r="C21" s="79"/>
+      <c r="A21" s="144">
+        <v>44455</v>
+      </c>
+      <c r="B21" s="142" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" s="79">
+        <v>42482</v>
+      </c>
       <c r="D21" s="144"/>
       <c r="E21" s="79"/>
       <c r="F21" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>170146.64</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="144"/>
-      <c r="B22" s="142"/>
-      <c r="C22" s="79"/>
+      <c r="A22" s="144">
+        <v>44456</v>
+      </c>
+      <c r="B22" s="142" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" s="79">
+        <v>45247.6</v>
+      </c>
       <c r="D22" s="144"/>
       <c r="E22" s="79"/>
       <c r="F22" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>215394.24000000002</v>
       </c>
       <c r="G22" s="146"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="144"/>
-      <c r="B23" s="142"/>
-      <c r="C23" s="79"/>
+      <c r="A23" s="144">
+        <v>44456</v>
+      </c>
+      <c r="B23" s="142" t="s">
+        <v>145</v>
+      </c>
+      <c r="C23" s="79">
+        <v>1281.5999999999999</v>
+      </c>
       <c r="D23" s="144"/>
       <c r="E23" s="79"/>
       <c r="F23" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>216675.84000000003</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="144"/>
-      <c r="B24" s="142"/>
-      <c r="C24" s="79"/>
+      <c r="A24" s="144">
+        <v>44456</v>
+      </c>
+      <c r="B24" s="142" t="s">
+        <v>146</v>
+      </c>
+      <c r="C24" s="79">
+        <v>19709.2</v>
+      </c>
       <c r="D24" s="144"/>
       <c r="E24" s="79"/>
       <c r="F24" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>236385.04000000004</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="144"/>
-      <c r="B25" s="142"/>
-      <c r="C25" s="79"/>
+      <c r="A25" s="144">
+        <v>44457</v>
+      </c>
+      <c r="B25" s="142" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25" s="79">
+        <v>102622.38</v>
+      </c>
       <c r="D25" s="144"/>
       <c r="E25" s="79"/>
       <c r="F25" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>339007.42000000004</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="144"/>
-      <c r="B26" s="142"/>
-      <c r="C26" s="79"/>
+      <c r="A26" s="144">
+        <v>44457</v>
+      </c>
+      <c r="B26" s="142" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" s="79">
+        <v>2353.4</v>
+      </c>
       <c r="D26" s="144"/>
       <c r="E26" s="79"/>
       <c r="F26" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>341360.82000000007</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="144"/>
-      <c r="B27" s="142"/>
-      <c r="C27" s="79"/>
+      <c r="A27" s="144">
+        <v>44458</v>
+      </c>
+      <c r="B27" s="142" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27" s="79">
+        <v>607.20000000000005</v>
+      </c>
       <c r="D27" s="144"/>
       <c r="E27" s="79"/>
       <c r="F27" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>341968.02000000008</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="144"/>
-      <c r="B28" s="142"/>
-      <c r="C28" s="79"/>
-      <c r="D28" s="144"/>
-      <c r="E28" s="79"/>
+      <c r="A28" s="190">
+        <v>44459</v>
+      </c>
+      <c r="B28" s="188">
+        <v>44459</v>
+      </c>
+      <c r="C28" s="189">
+        <v>31885.45</v>
+      </c>
+      <c r="D28" s="144">
+        <v>44463</v>
+      </c>
+      <c r="E28" s="79">
+        <v>350000</v>
+      </c>
       <c r="F28" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -9551,7 +9814,7 @@
       <c r="E29" s="79"/>
       <c r="F29" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
@@ -9562,7 +9825,7 @@
       <c r="E30" s="79"/>
       <c r="F30" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
       <c r="G30" s="146"/>
     </row>
@@ -9574,7 +9837,7 @@
       <c r="E31" s="79"/>
       <c r="F31" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -9585,7 +9848,7 @@
       <c r="E32" s="79"/>
       <c r="F32" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9596,7 +9859,7 @@
       <c r="E33" s="79"/>
       <c r="F33" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9607,7 +9870,7 @@
       <c r="E34" s="79"/>
       <c r="F34" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9618,7 +9881,7 @@
       <c r="E35" s="79"/>
       <c r="F35" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9629,7 +9892,7 @@
       <c r="E36" s="79"/>
       <c r="F36" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9640,7 +9903,7 @@
       <c r="E37" s="79"/>
       <c r="F37" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9651,7 +9914,7 @@
       <c r="E38" s="79"/>
       <c r="F38" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9662,7 +9925,7 @@
       <c r="E39" s="79"/>
       <c r="F39" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9673,7 +9936,7 @@
       <c r="E40" s="79"/>
       <c r="F40" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9684,7 +9947,7 @@
       <c r="E41" s="79"/>
       <c r="F41" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9695,7 +9958,7 @@
       <c r="E42" s="79"/>
       <c r="F42" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9706,7 +9969,7 @@
       <c r="E43" s="79"/>
       <c r="F43" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9717,7 +9980,7 @@
       <c r="E44" s="79"/>
       <c r="F44" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9728,7 +9991,7 @@
       <c r="E45" s="79"/>
       <c r="F45" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9739,7 +10002,7 @@
       <c r="E46" s="79"/>
       <c r="F46" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9750,7 +10013,7 @@
       <c r="E47" s="79"/>
       <c r="F47" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9761,7 +10024,7 @@
       <c r="E48" s="79"/>
       <c r="F48" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9772,7 +10035,7 @@
       <c r="E49" s="79"/>
       <c r="F49" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9783,7 +10046,7 @@
       <c r="E50" s="79"/>
       <c r="F50" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9794,7 +10057,7 @@
       <c r="E51" s="79"/>
       <c r="F51" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9805,7 +10068,7 @@
       <c r="E52" s="79"/>
       <c r="F52" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9816,7 +10079,7 @@
       <c r="E53" s="79"/>
       <c r="F53" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9827,7 +10090,7 @@
       <c r="E54" s="79"/>
       <c r="F54" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9838,7 +10101,7 @@
       <c r="E55" s="79"/>
       <c r="F55" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9849,7 +10112,7 @@
       <c r="E56" s="79"/>
       <c r="F56" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9860,7 +10123,7 @@
       <c r="E57" s="79"/>
       <c r="F57" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9871,7 +10134,7 @@
       <c r="E58" s="79"/>
       <c r="F58" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9882,7 +10145,7 @@
       <c r="E59" s="79"/>
       <c r="F59" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9893,7 +10156,7 @@
       <c r="E60" s="79"/>
       <c r="F60" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9904,7 +10167,7 @@
       <c r="E61" s="79"/>
       <c r="F61" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -9915,7 +10178,7 @@
       <c r="E62" s="79"/>
       <c r="F62" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -9926,7 +10189,7 @@
       <c r="E63" s="79"/>
       <c r="F63" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -9937,7 +10200,7 @@
       <c r="E64" s="79"/>
       <c r="F64" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -9948,7 +10211,7 @@
       <c r="E65" s="79"/>
       <c r="F65" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -9959,7 +10222,7 @@
       <c r="E66" s="79"/>
       <c r="F66" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -9970,7 +10233,7 @@
       <c r="E67" s="79"/>
       <c r="F67" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -9981,7 +10244,7 @@
       <c r="E68" s="79"/>
       <c r="F68" s="145">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -9992,7 +10255,7 @@
       <c r="E69" s="79"/>
       <c r="F69" s="145">
         <f t="shared" ref="F69:F97" si="1">F68+C69-E69</f>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10003,7 +10266,7 @@
       <c r="E70" s="79"/>
       <c r="F70" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10014,7 +10277,7 @@
       <c r="E71" s="79"/>
       <c r="F71" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10025,7 +10288,7 @@
       <c r="E72" s="79"/>
       <c r="F72" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10036,7 +10299,7 @@
       <c r="E73" s="79"/>
       <c r="F73" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10047,7 +10310,7 @@
       <c r="E74" s="79"/>
       <c r="F74" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10058,7 +10321,7 @@
       <c r="E75" s="79"/>
       <c r="F75" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10069,7 +10332,7 @@
       <c r="E76" s="79"/>
       <c r="F76" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10080,7 +10343,7 @@
       <c r="E77" s="79"/>
       <c r="F77" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10091,7 +10354,7 @@
       <c r="E78" s="79"/>
       <c r="F78" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10102,7 +10365,7 @@
       <c r="E79" s="79"/>
       <c r="F79" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10113,7 +10376,7 @@
       <c r="E80" s="79"/>
       <c r="F80" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10124,7 +10387,7 @@
       <c r="E81" s="83"/>
       <c r="F81" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10135,7 +10398,7 @@
       <c r="E82" s="83"/>
       <c r="F82" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10146,7 +10409,7 @@
       <c r="E83" s="83"/>
       <c r="F83" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10157,7 +10420,7 @@
       <c r="E84" s="83"/>
       <c r="F84" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10168,7 +10431,7 @@
       <c r="E85" s="83"/>
       <c r="F85" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10179,7 +10442,7 @@
       <c r="E86" s="83"/>
       <c r="F86" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10190,7 +10453,7 @@
       <c r="E87" s="79"/>
       <c r="F87" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10201,7 +10464,7 @@
       <c r="E88" s="79"/>
       <c r="F88" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10212,7 +10475,7 @@
       <c r="E89" s="79"/>
       <c r="F89" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10223,7 +10486,7 @@
       <c r="E90" s="79"/>
       <c r="F90" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10234,7 +10497,7 @@
       <c r="E91" s="79"/>
       <c r="F91" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10245,7 +10508,7 @@
       <c r="E92" s="79"/>
       <c r="F92" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10256,7 +10519,7 @@
       <c r="E93" s="79"/>
       <c r="F93" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10267,7 +10530,7 @@
       <c r="E94" s="79"/>
       <c r="F94" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10278,7 +10541,7 @@
       <c r="E95" s="79"/>
       <c r="F95" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10289,7 +10552,7 @@
       <c r="E96" s="79"/>
       <c r="F96" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10302,23 +10565,23 @@
       <c r="E97" s="151"/>
       <c r="F97" s="145">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B98" s="104"/>
       <c r="C98" s="3">
         <f>SUM(C3:C97)</f>
-        <v>0</v>
+        <v>710732.2699999999</v>
       </c>
       <c r="D98" s="103"/>
       <c r="E98" s="3">
         <f>SUM(E3:E97)</f>
-        <v>0</v>
+        <v>686878.8</v>
       </c>
       <c r="F98" s="153">
         <f>F97</f>
-        <v>0</v>
+        <v>23853.470000000088</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -10560,12 +10823,12 @@
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="163"/>
-      <c r="B45" s="249" t="s">
+      <c r="B45" s="250" t="s">
         <v>31</v>
       </c>
-      <c r="C45" s="250"/>
-      <c r="D45" s="250"/>
-      <c r="E45" s="251"/>
+      <c r="C45" s="251"/>
+      <c r="D45" s="251"/>
+      <c r="E45" s="252"/>
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10587,7 +10850,7 @@
       <c r="F46" s="107">
         <v>302</v>
       </c>
-      <c r="G46" s="252"/>
+      <c r="G46" s="253"/>
     </row>
     <row r="47" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="170"/>
@@ -10606,7 +10869,7 @@
       <c r="F47" s="107">
         <v>0</v>
       </c>
-      <c r="G47" s="253"/>
+      <c r="G47" s="254"/>
     </row>
     <row r="48" spans="1:7" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="170"/>

</xml_diff>

<commit_message>
CIERRE DEL 28 SEPT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE  HERRADURA  SEPTIEMBRE   2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE  HERRADURA  SEPTIEMBRE   2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="A G O S T O    2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="159">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -513,12 +513,6 @@
     <t>QUESOS-MAIZ-CONCHA RES</t>
   </si>
   <si>
-    <t>#3225</t>
-  </si>
-  <si>
-    <t># 3227</t>
-  </si>
-  <si>
     <t>CONCHA RES--CHAMBARETE</t>
   </si>
   <si>
@@ -601,6 +595,33 @@
   </si>
   <si>
     <t>NOMINA # 38</t>
+  </si>
+  <si>
+    <t>PEREJIL-CEBOLLA</t>
+  </si>
+  <si>
+    <t>HAMBURGUESA--SALCHICHAS-JAMON-PAPA-MOLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOSTADAS  </t>
+  </si>
+  <si>
+    <t>#3896</t>
+  </si>
+  <si>
+    <t># 3897</t>
+  </si>
+  <si>
+    <t>CHISTORRA--TOCINO--LONGANIZA</t>
+  </si>
+  <si>
+    <t>DELANTERO-SALCHICHA</t>
+  </si>
+  <si>
+    <t>MANCHEGO--TOCINO</t>
+  </si>
+  <si>
+    <t>NOMINA # 39</t>
   </si>
 </sst>
 </file>
@@ -2140,6 +2161,57 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2195,57 +2267,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3440,23 +3461,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="236"/>
-      <c r="C1" s="245" t="s">
+      <c r="B1" s="217"/>
+      <c r="C1" s="226" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="246"/>
-      <c r="E1" s="246"/>
-      <c r="F1" s="246"/>
-      <c r="G1" s="246"/>
-      <c r="H1" s="246"/>
-      <c r="I1" s="246"/>
-      <c r="J1" s="246"/>
-      <c r="K1" s="246"/>
-      <c r="L1" s="246"/>
-      <c r="M1" s="246"/>
+      <c r="D1" s="227"/>
+      <c r="E1" s="227"/>
+      <c r="F1" s="227"/>
+      <c r="G1" s="227"/>
+      <c r="H1" s="227"/>
+      <c r="I1" s="227"/>
+      <c r="J1" s="227"/>
+      <c r="K1" s="227"/>
+      <c r="L1" s="227"/>
+      <c r="M1" s="227"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="237"/>
+      <c r="B2" s="218"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -3466,17 +3487,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="238" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="239"/>
+      <c r="B3" s="219" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="220"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="240" t="s">
+      <c r="H3" s="221" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="240"/>
+      <c r="I3" s="221"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -3492,14 +3513,14 @@
       <c r="D4" s="16">
         <v>44410</v>
       </c>
-      <c r="E4" s="241" t="s">
+      <c r="E4" s="222" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="242"/>
-      <c r="H4" s="243" t="s">
+      <c r="F4" s="223"/>
+      <c r="H4" s="224" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="244"/>
+      <c r="I4" s="225"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -3509,10 +3530,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="230" t="s">
+      <c r="P4" s="211" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="231"/>
+      <c r="Q4" s="212"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -5007,11 +5028,11 @@
       <c r="L39" s="69">
         <v>454.62</v>
       </c>
-      <c r="M39" s="232">
+      <c r="M39" s="213">
         <f>SUM(M5:M38)</f>
         <v>1393675.5</v>
       </c>
-      <c r="N39" s="234">
+      <c r="N39" s="215">
         <f>SUM(N5:N38)</f>
         <v>28399.97</v>
       </c>
@@ -5043,8 +5064,8 @@
       <c r="L40" s="69">
         <v>1195.67</v>
       </c>
-      <c r="M40" s="233"/>
-      <c r="N40" s="235"/>
+      <c r="M40" s="214"/>
+      <c r="N40" s="216"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -5277,29 +5298,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="220" t="s">
+      <c r="H52" s="237" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="221"/>
+      <c r="I52" s="238"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="222">
+      <c r="K52" s="239">
         <f>I50+L50</f>
         <v>80916.84</v>
       </c>
-      <c r="L52" s="223"/>
-      <c r="M52" s="211">
+      <c r="L52" s="240"/>
+      <c r="M52" s="228">
         <f>N39+M39</f>
         <v>1422075.47</v>
       </c>
-      <c r="N52" s="212"/>
+      <c r="N52" s="229"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="224" t="s">
+      <c r="D53" s="241" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="224"/>
+      <c r="E53" s="241"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1396181.44</v>
@@ -5310,22 +5331,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="225" t="s">
+      <c r="D54" s="242" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="225"/>
+      <c r="E54" s="242"/>
       <c r="F54" s="102">
         <v>-1523111</v>
       </c>
-      <c r="I54" s="226" t="s">
+      <c r="I54" s="243" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="227"/>
-      <c r="K54" s="228">
+      <c r="J54" s="244"/>
+      <c r="K54" s="245">
         <f>F56+F57+F58</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L54" s="229"/>
+      <c r="L54" s="246"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -5356,10 +5377,10 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="213">
-        <v>0</v>
-      </c>
-      <c r="L56" s="214"/>
+      <c r="K56" s="230">
+        <v>0</v>
+      </c>
+      <c r="L56" s="231"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -5376,22 +5397,22 @@
       <c r="C58" s="120">
         <v>44444</v>
       </c>
-      <c r="D58" s="215" t="s">
+      <c r="D58" s="232" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="216"/>
+      <c r="E58" s="233"/>
       <c r="F58" s="121">
         <v>136234.76999999999</v>
       </c>
-      <c r="I58" s="217" t="s">
+      <c r="I58" s="234" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="218"/>
-      <c r="K58" s="219">
+      <c r="J58" s="235"/>
+      <c r="K58" s="236">
         <f>K54+K56</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L58" s="219"/>
+      <c r="L58" s="236"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -5535,15 +5556,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="C1:M1"/>
     <mergeCell ref="M52:N52"/>
     <mergeCell ref="K56:L56"/>
     <mergeCell ref="D58:E58"/>
@@ -5555,6 +5567,15 @@
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -7245,8 +7266,8 @@
   </sheetPr>
   <dimension ref="A1:R80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7268,23 +7289,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="236"/>
-      <c r="C1" s="245" t="s">
+      <c r="B1" s="217"/>
+      <c r="C1" s="226" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="246"/>
-      <c r="E1" s="246"/>
-      <c r="F1" s="246"/>
-      <c r="G1" s="246"/>
-      <c r="H1" s="246"/>
-      <c r="I1" s="246"/>
-      <c r="J1" s="246"/>
-      <c r="K1" s="246"/>
-      <c r="L1" s="246"/>
-      <c r="M1" s="246"/>
+      <c r="D1" s="227"/>
+      <c r="E1" s="227"/>
+      <c r="F1" s="227"/>
+      <c r="G1" s="227"/>
+      <c r="H1" s="227"/>
+      <c r="I1" s="227"/>
+      <c r="J1" s="227"/>
+      <c r="K1" s="227"/>
+      <c r="L1" s="227"/>
+      <c r="M1" s="227"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="237"/>
+      <c r="B2" s="218"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -7294,17 +7315,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="238" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="239"/>
+      <c r="B3" s="219" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="220"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="240" t="s">
+      <c r="H3" s="221" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="240"/>
+      <c r="I3" s="221"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -7320,14 +7341,14 @@
       <c r="D4" s="16">
         <v>44444</v>
       </c>
-      <c r="E4" s="241" t="s">
+      <c r="E4" s="222" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="242"/>
-      <c r="H4" s="243" t="s">
+      <c r="F4" s="223"/>
+      <c r="H4" s="224" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="244"/>
+      <c r="I4" s="225"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -7337,10 +7358,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="230" t="s">
+      <c r="P4" s="211" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="231"/>
+      <c r="Q4" s="212"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -7749,7 +7770,7 @@
         <v>4078</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E14" s="24">
         <v>44454</v>
@@ -7856,15 +7877,15 @@
         <v>72820</v>
       </c>
       <c r="N16" s="30">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="P16" s="83">
         <f t="shared" si="0"/>
-        <v>72820</v>
+        <v>77820</v>
       </c>
       <c r="Q16" s="9">
         <f t="shared" si="1"/>
-        <v>-5000</v>
+        <v>0</v>
       </c>
       <c r="R16" s="26"/>
     </row>
@@ -7877,7 +7898,7 @@
         <v>3060</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E17" s="24">
         <v>44457</v>
@@ -7896,7 +7917,7 @@
         <v>44457</v>
       </c>
       <c r="K17" s="40" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L17" s="43">
         <v>15042.86</v>
@@ -7924,14 +7945,16 @@
         <v>44427</v>
       </c>
       <c r="C18" s="22">
-        <v>0</v>
-      </c>
-      <c r="D18" s="31"/>
+        <v>27</v>
+      </c>
+      <c r="D18" s="31" t="s">
+        <v>150</v>
+      </c>
       <c r="E18" s="24">
         <v>44458</v>
       </c>
       <c r="F18" s="25">
-        <v>0</v>
+        <v>77794</v>
       </c>
       <c r="G18" s="26"/>
       <c r="H18" s="32">
@@ -7944,14 +7967,15 @@
       <c r="K18" s="47"/>
       <c r="L18" s="35"/>
       <c r="M18" s="138">
-        <v>0</v>
+        <f>50000+23248</f>
+        <v>73248</v>
       </c>
       <c r="N18" s="30">
-        <v>0</v>
+        <v>4519</v>
       </c>
       <c r="P18" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>77794</v>
       </c>
       <c r="Q18" s="9">
         <f t="shared" si="1"/>
@@ -7965,34 +7989,37 @@
         <v>44428</v>
       </c>
       <c r="C19" s="22">
-        <v>0</v>
-      </c>
-      <c r="D19" s="31"/>
+        <v>2067</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>151</v>
+      </c>
       <c r="E19" s="24">
         <v>44459</v>
       </c>
       <c r="F19" s="25">
-        <v>0</v>
+        <v>51442</v>
       </c>
       <c r="G19" s="26"/>
       <c r="H19" s="32">
         <v>44459</v>
       </c>
       <c r="I19" s="28">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J19" s="33"/>
       <c r="K19" s="48"/>
       <c r="L19" s="49"/>
       <c r="M19" s="138">
-        <v>0</v>
+        <f>28500+20860</f>
+        <v>49360</v>
       </c>
       <c r="N19" s="30">
         <v>0</v>
       </c>
       <c r="P19" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>51442</v>
       </c>
       <c r="Q19" s="9">
         <f t="shared" si="1"/>
@@ -8006,34 +8033,37 @@
         <v>44429</v>
       </c>
       <c r="C20" s="22">
-        <v>0</v>
-      </c>
-      <c r="D20" s="31"/>
+        <v>340</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>152</v>
+      </c>
       <c r="E20" s="24">
         <v>44460</v>
       </c>
       <c r="F20" s="25">
-        <v>0</v>
+        <v>52956</v>
       </c>
       <c r="G20" s="26"/>
       <c r="H20" s="32">
         <v>44460</v>
       </c>
       <c r="I20" s="28">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J20" s="33"/>
       <c r="K20" s="50"/>
       <c r="L20" s="43"/>
       <c r="M20" s="138">
-        <v>0</v>
+        <f>25000+26658</f>
+        <v>51658</v>
       </c>
       <c r="N20" s="30">
-        <v>0</v>
+        <v>950</v>
       </c>
       <c r="P20" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>52956</v>
       </c>
       <c r="Q20" s="9">
         <f t="shared" si="1"/>
@@ -8054,31 +8084,32 @@
         <v>44461</v>
       </c>
       <c r="F21" s="25">
-        <v>0</v>
+        <v>41002</v>
       </c>
       <c r="G21" s="26"/>
       <c r="H21" s="32">
         <v>44461</v>
       </c>
       <c r="I21" s="28">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J21" s="33"/>
       <c r="K21" s="180"/>
       <c r="L21" s="43"/>
       <c r="M21" s="138">
-        <v>0</v>
+        <f>20000+20650</f>
+        <v>40650</v>
       </c>
       <c r="N21" s="30">
-        <v>0</v>
+        <v>342</v>
       </c>
       <c r="P21" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>41004</v>
       </c>
       <c r="Q21" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R21" s="26"/>
     </row>
@@ -8088,34 +8119,37 @@
         <v>44431</v>
       </c>
       <c r="C22" s="22">
-        <v>0</v>
-      </c>
-      <c r="D22" s="31"/>
+        <v>5051</v>
+      </c>
+      <c r="D22" s="31" t="s">
+        <v>155</v>
+      </c>
       <c r="E22" s="24">
         <v>44462</v>
       </c>
       <c r="F22" s="25">
-        <v>0</v>
+        <v>62111</v>
       </c>
       <c r="G22" s="26"/>
       <c r="H22" s="32">
         <v>44462</v>
       </c>
       <c r="I22" s="28">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="J22" s="33"/>
       <c r="K22" s="51"/>
       <c r="L22" s="52"/>
       <c r="M22" s="138">
-        <v>0</v>
+        <f>25000+30485</f>
+        <v>55485</v>
       </c>
       <c r="N22" s="30">
-        <v>0</v>
+        <v>1524</v>
       </c>
       <c r="P22" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>62111</v>
       </c>
       <c r="Q22" s="9">
         <f t="shared" si="1"/>
@@ -8129,38 +8163,41 @@
         <v>44432</v>
       </c>
       <c r="C23" s="22">
-        <v>0</v>
-      </c>
-      <c r="D23" s="31"/>
+        <v>8999</v>
+      </c>
+      <c r="D23" s="31" t="s">
+        <v>156</v>
+      </c>
       <c r="E23" s="24">
         <v>44463</v>
       </c>
       <c r="F23" s="25">
-        <v>0</v>
+        <v>89209</v>
       </c>
       <c r="G23" s="26"/>
       <c r="H23" s="32">
         <v>44463</v>
       </c>
       <c r="I23" s="28">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J23" s="53"/>
       <c r="K23" s="54"/>
       <c r="L23" s="43"/>
       <c r="M23" s="138">
-        <v>0</v>
+        <f>5300+40000+34700</f>
+        <v>80000</v>
       </c>
       <c r="N23" s="30">
-        <v>0</v>
+        <v>195</v>
       </c>
       <c r="P23" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>89210</v>
       </c>
       <c r="Q23" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R23" s="26"/>
     </row>
@@ -8170,38 +8207,47 @@
         <v>44433</v>
       </c>
       <c r="C24" s="22">
-        <v>0</v>
-      </c>
-      <c r="D24" s="31"/>
+        <v>1265</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>157</v>
+      </c>
       <c r="E24" s="24">
         <v>44464</v>
       </c>
       <c r="F24" s="25">
-        <v>0</v>
+        <v>64660</v>
       </c>
       <c r="G24" s="26"/>
       <c r="H24" s="32">
         <v>44464</v>
       </c>
       <c r="I24" s="28">
-        <v>0</v>
-      </c>
-      <c r="J24" s="55"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="57"/>
+        <v>285</v>
+      </c>
+      <c r="J24" s="55">
+        <v>44464</v>
+      </c>
+      <c r="K24" s="56" t="s">
+        <v>158</v>
+      </c>
+      <c r="L24" s="57">
+        <v>10900</v>
+      </c>
       <c r="M24" s="138">
-        <v>0</v>
+        <f>20000+25920</f>
+        <v>45920</v>
       </c>
       <c r="N24" s="30">
-        <v>0</v>
+        <v>6292</v>
       </c>
       <c r="P24" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>64662</v>
       </c>
       <c r="Q24" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R24" s="26"/>
     </row>
@@ -8770,21 +8816,21 @@
       <c r="J39" s="67"/>
       <c r="K39" s="82"/>
       <c r="L39" s="69"/>
-      <c r="M39" s="232">
+      <c r="M39" s="213">
         <f>SUM(M5:M38)</f>
-        <v>590065</v>
-      </c>
-      <c r="N39" s="234">
+        <v>986386</v>
+      </c>
+      <c r="N39" s="215">
         <f>SUM(N5:N38)</f>
-        <v>19580</v>
+        <v>38402</v>
       </c>
       <c r="P39" s="83">
         <f>SUM(P5:P38)</f>
-        <v>662958.15</v>
+        <v>1107137.1499999999</v>
       </c>
       <c r="Q39" s="9">
         <f>SUM(Q5:Q38)</f>
-        <v>-4988.8499999999985</v>
+        <v>16.150000000001455</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -8800,8 +8846,8 @@
       <c r="J40" s="67"/>
       <c r="K40" s="71"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="233"/>
-      <c r="N40" s="235"/>
+      <c r="M40" s="214"/>
+      <c r="N40" s="216"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -8974,7 +9020,7 @@
       </c>
       <c r="C50" s="93">
         <f>SUM(C5:C49)</f>
-        <v>21264</v>
+        <v>39013</v>
       </c>
       <c r="D50" s="94"/>
       <c r="E50" s="95" t="s">
@@ -8982,7 +9028,7 @@
       </c>
       <c r="F50" s="96">
         <f>SUM(F5:F49)</f>
-        <v>667947</v>
+        <v>1107121</v>
       </c>
       <c r="G50" s="94"/>
       <c r="H50" s="97" t="s">
@@ -8990,7 +9036,7 @@
       </c>
       <c r="I50" s="98">
         <f>SUM(I5:I49)</f>
-        <v>5992</v>
+        <v>6379</v>
       </c>
       <c r="J50" s="99"/>
       <c r="K50" s="100" t="s">
@@ -8998,7 +9044,7 @@
       </c>
       <c r="L50" s="101">
         <f>SUM(L5:L49)</f>
-        <v>26057.15</v>
+        <v>36957.15</v>
       </c>
       <c r="M50" s="102"/>
       <c r="N50" s="102"/>
@@ -9016,32 +9062,32 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="220" t="s">
+      <c r="H52" s="237" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="221"/>
+      <c r="I52" s="238"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="222">
+      <c r="K52" s="239">
         <f>I50+L50</f>
-        <v>32049.15</v>
-      </c>
-      <c r="L52" s="223"/>
-      <c r="M52" s="211">
+        <v>43336.15</v>
+      </c>
+      <c r="L52" s="240"/>
+      <c r="M52" s="228">
         <f>N39+M39</f>
-        <v>609645</v>
-      </c>
-      <c r="N52" s="212"/>
+        <v>1024788</v>
+      </c>
+      <c r="N52" s="229"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="224" t="s">
+      <c r="D53" s="241" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="224"/>
+      <c r="E53" s="241"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
-        <v>614633.85</v>
+        <v>1024771.8500000001</v>
       </c>
       <c r="I53" s="108"/>
       <c r="J53" s="109"/>
@@ -9049,22 +9095,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="225" t="s">
+      <c r="D54" s="242" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="225"/>
+      <c r="E54" s="242"/>
       <c r="F54" s="102">
         <v>0</v>
       </c>
-      <c r="I54" s="226" t="s">
+      <c r="I54" s="243" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="227"/>
-      <c r="K54" s="228">
+      <c r="J54" s="244"/>
+      <c r="K54" s="245">
         <f>F56+F57+F58</f>
-        <v>614633.85</v>
-      </c>
-      <c r="L54" s="229"/>
+        <v>1024771.8500000001</v>
+      </c>
+      <c r="L54" s="246"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -9088,17 +9134,17 @@
       </c>
       <c r="F56" s="102">
         <f>SUM(F53:F55)</f>
-        <v>614633.85</v>
+        <v>1024771.8500000001</v>
       </c>
       <c r="H56" s="20"/>
       <c r="I56" s="116" t="s">
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="213">
-        <v>0</v>
-      </c>
-      <c r="L56" s="214"/>
+      <c r="K56" s="230">
+        <v>0</v>
+      </c>
+      <c r="L56" s="231"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -9113,22 +9159,22 @@
     </row>
     <row r="58" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C58" s="120"/>
-      <c r="D58" s="215" t="s">
+      <c r="D58" s="232" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="216"/>
+      <c r="E58" s="233"/>
       <c r="F58" s="121">
         <v>0</v>
       </c>
-      <c r="I58" s="217" t="s">
+      <c r="I58" s="234" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="218"/>
-      <c r="K58" s="219">
+      <c r="J58" s="235"/>
+      <c r="K58" s="236">
         <f>K54+K56</f>
-        <v>614633.85</v>
-      </c>
-      <c r="L58" s="219"/>
+        <v>1024771.8500000001</v>
+      </c>
+      <c r="L58" s="236"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -9272,12 +9318,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -9292,6 +9332,12 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -9358,7 +9404,7 @@
         <v>44445</v>
       </c>
       <c r="B3" s="182" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C3" s="79">
         <v>42896.2</v>
@@ -9375,7 +9421,7 @@
         <v>44446</v>
       </c>
       <c r="B4" s="182" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C4" s="79">
         <v>673.2</v>
@@ -9393,7 +9439,7 @@
         <v>44447</v>
       </c>
       <c r="B5" s="182" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C5" s="79">
         <v>59000.22</v>
@@ -9410,7 +9456,7 @@
         <v>44447</v>
       </c>
       <c r="B6" s="182" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C6" s="79">
         <v>11075.4</v>
@@ -9427,7 +9473,7 @@
         <v>44448</v>
       </c>
       <c r="B7" s="182" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C7" s="79">
         <v>8608.6</v>
@@ -9444,7 +9490,7 @@
         <v>44448</v>
       </c>
       <c r="B8" s="182" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C8" s="79">
         <v>45033.9</v>
@@ -9461,7 +9507,7 @@
         <v>44448</v>
       </c>
       <c r="B9" s="182" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C9" s="79">
         <v>2191.8000000000002</v>
@@ -9478,7 +9524,7 @@
         <v>44449</v>
       </c>
       <c r="B10" s="182" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C10" s="79">
         <v>6894.34</v>
@@ -9496,7 +9542,7 @@
         <v>44449</v>
       </c>
       <c r="B11" s="142" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C11" s="79">
         <v>12957.4</v>
@@ -9513,7 +9559,7 @@
         <v>44450</v>
       </c>
       <c r="B12" s="142" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C12" s="79">
         <v>88426.6</v>
@@ -9530,7 +9576,7 @@
         <v>44451</v>
       </c>
       <c r="B13" s="142" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C13" s="79">
         <v>789.96</v>
@@ -9547,7 +9593,7 @@
         <v>44452</v>
       </c>
       <c r="B14" s="142" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C14" s="79">
         <v>41682.5</v>
@@ -9564,7 +9610,7 @@
         <v>44452</v>
       </c>
       <c r="B15" s="142" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C15" s="79">
         <v>21216.5</v>
@@ -9585,7 +9631,7 @@
         <v>44452</v>
       </c>
       <c r="B16" s="142" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C16" s="79">
         <v>13948.78</v>
@@ -9602,7 +9648,7 @@
         <v>44453</v>
       </c>
       <c r="B17" s="142" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C17" s="79">
         <v>69059.98</v>
@@ -9619,7 +9665,7 @@
         <v>44453</v>
       </c>
       <c r="B18" s="142" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C18" s="79">
         <v>23621.5</v>
@@ -9636,7 +9682,7 @@
         <v>44453</v>
       </c>
       <c r="B19" s="142" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C19" s="79">
         <v>10612.8</v>
@@ -9653,7 +9699,7 @@
         <v>44455</v>
       </c>
       <c r="B20" s="142" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C20" s="79">
         <v>5853.76</v>
@@ -9670,7 +9716,7 @@
         <v>44455</v>
       </c>
       <c r="B21" s="142" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C21" s="79">
         <v>42482</v>
@@ -9687,7 +9733,7 @@
         <v>44456</v>
       </c>
       <c r="B22" s="142" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C22" s="79">
         <v>45247.6</v>
@@ -9705,7 +9751,7 @@
         <v>44456</v>
       </c>
       <c r="B23" s="142" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C23" s="79">
         <v>1281.5999999999999</v>
@@ -9722,7 +9768,7 @@
         <v>44456</v>
       </c>
       <c r="B24" s="142" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C24" s="79">
         <v>19709.2</v>
@@ -9739,7 +9785,7 @@
         <v>44457</v>
       </c>
       <c r="B25" s="142" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C25" s="79">
         <v>102622.38</v>
@@ -9756,7 +9802,7 @@
         <v>44457</v>
       </c>
       <c r="B26" s="142" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C26" s="79">
         <v>2353.4</v>
@@ -9773,7 +9819,7 @@
         <v>44458</v>
       </c>
       <c r="B27" s="142" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C27" s="79">
         <v>607.20000000000005</v>
@@ -10801,7 +10847,7 @@
   <dimension ref="A23:G53"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46:G47"/>
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10833,22 +10879,22 @@
     </row>
     <row r="46" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="170">
-        <v>44454</v>
+        <v>44461</v>
       </c>
       <c r="B46" s="171" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="C46" s="172">
-        <v>304.5</v>
+        <v>132.30000000000001</v>
       </c>
       <c r="D46" s="173" t="s">
         <v>32</v>
       </c>
       <c r="E46" s="174" t="s">
-        <v>123</v>
+        <v>154</v>
       </c>
       <c r="F46" s="107">
-        <v>302</v>
+        <v>96</v>
       </c>
       <c r="G46" s="253"/>
     </row>

</xml_diff>

<commit_message>
CIERRE 5 OCT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE  HERRADURA  SEPTIEMBRE   2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE  HERRADURA  SEPTIEMBRE   2021.xlsx
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="167">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -606,12 +606,6 @@
     <t xml:space="preserve">TOSTADAS  </t>
   </si>
   <si>
-    <t>#3896</t>
-  </si>
-  <si>
-    <t># 3897</t>
-  </si>
-  <si>
     <t>CHISTORRA--TOCINO--LONGANIZA</t>
   </si>
   <si>
@@ -622,6 +616,36 @@
   </si>
   <si>
     <t>NOMINA # 39</t>
+  </si>
+  <si>
+    <t>RECORTE</t>
+  </si>
+  <si>
+    <t>BOTARGAS</t>
+  </si>
+  <si>
+    <t>SALCHICHA-JAMON-PEORONI-BOLSA</t>
+  </si>
+  <si>
+    <t>CHILE--JAMON-TOCINO-PAPAS</t>
+  </si>
+  <si>
+    <t>HAMBURGUESA-QUESO-CONDIMENTO-TOSTADAS</t>
+  </si>
+  <si>
+    <t># 4734</t>
+  </si>
+  <si>
+    <t>#  4735</t>
+  </si>
+  <si>
+    <t># 4750</t>
+  </si>
+  <si>
+    <t># 4753</t>
+  </si>
+  <si>
+    <t>CECINA-QUESOS-VEERDURA</t>
   </si>
 </sst>
 </file>
@@ -985,7 +1009,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1034,6 +1058,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="58">
     <border>
@@ -2091,7 +2121,6 @@
     <xf numFmtId="44" fontId="41" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="20" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2161,6 +2190,63 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="3" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="3" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2212,63 +2298,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="3" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="3" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -2287,12 +2316,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -2302,6 +2330,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF33CCFF"/>
       <color rgb="FF0000FF"/>
       <color rgb="FF9933FF"/>
       <color rgb="FFFF6600"/>
@@ -3461,23 +3490,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="217"/>
-      <c r="C1" s="226" t="s">
+      <c r="B1" s="235"/>
+      <c r="C1" s="244" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="227"/>
-      <c r="E1" s="227"/>
-      <c r="F1" s="227"/>
-      <c r="G1" s="227"/>
-      <c r="H1" s="227"/>
-      <c r="I1" s="227"/>
-      <c r="J1" s="227"/>
-      <c r="K1" s="227"/>
-      <c r="L1" s="227"/>
-      <c r="M1" s="227"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="218"/>
+      <c r="B2" s="236"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -3487,17 +3516,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="219" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="220"/>
+      <c r="B3" s="237" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="238"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="221" t="s">
+      <c r="H3" s="239" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="221"/>
+      <c r="I3" s="239"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -3513,14 +3542,14 @@
       <c r="D4" s="16">
         <v>44410</v>
       </c>
-      <c r="E4" s="222" t="s">
+      <c r="E4" s="240" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="223"/>
-      <c r="H4" s="224" t="s">
+      <c r="F4" s="241"/>
+      <c r="H4" s="242" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="225"/>
+      <c r="I4" s="243"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -3530,10 +3559,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="211" t="s">
+      <c r="P4" s="229" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="212"/>
+      <c r="Q4" s="230"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -4266,7 +4295,7 @@
         <v>42</v>
       </c>
       <c r="J21" s="33"/>
-      <c r="K21" s="180" t="s">
+      <c r="K21" s="179" t="s">
         <v>30</v>
       </c>
       <c r="L21" s="43">
@@ -4492,7 +4521,7 @@
         <f t="shared" si="0"/>
         <v>92849</v>
       </c>
-      <c r="Q26" s="186">
+      <c r="Q26" s="185">
         <f t="shared" si="1"/>
         <v>3146</v>
       </c>
@@ -4832,7 +4861,7 @@
       <c r="J34" s="67">
         <v>44443</v>
       </c>
-      <c r="K34" s="187" t="s">
+      <c r="K34" s="186" t="s">
         <v>106</v>
       </c>
       <c r="L34" s="76">
@@ -4950,7 +4979,7 @@
       <c r="J37" s="67">
         <v>44431</v>
       </c>
-      <c r="K37" s="181" t="s">
+      <c r="K37" s="180" t="s">
         <v>46</v>
       </c>
       <c r="L37" s="76">
@@ -5028,11 +5057,11 @@
       <c r="L39" s="69">
         <v>454.62</v>
       </c>
-      <c r="M39" s="213">
+      <c r="M39" s="231">
         <f>SUM(M5:M38)</f>
         <v>1393675.5</v>
       </c>
-      <c r="N39" s="215">
+      <c r="N39" s="233">
         <f>SUM(N5:N38)</f>
         <v>28399.97</v>
       </c>
@@ -5064,8 +5093,8 @@
       <c r="L40" s="69">
         <v>1195.67</v>
       </c>
-      <c r="M40" s="214"/>
-      <c r="N40" s="216"/>
+      <c r="M40" s="232"/>
+      <c r="N40" s="234"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -5073,23 +5102,23 @@
       <c r="A41" s="20"/>
       <c r="B41" s="21"/>
       <c r="C41" s="84"/>
-      <c r="D41" s="197"/>
-      <c r="E41" s="198"/>
-      <c r="F41" s="199"/>
+      <c r="D41" s="196"/>
+      <c r="E41" s="197"/>
+      <c r="F41" s="198"/>
       <c r="G41" s="26"/>
-      <c r="H41" s="200"/>
+      <c r="H41" s="199"/>
       <c r="I41" s="85"/>
       <c r="J41" s="67" t="s">
         <v>109</v>
       </c>
-      <c r="K41" s="208" t="s">
+      <c r="K41" s="207" t="s">
         <v>114</v>
       </c>
       <c r="L41" s="75">
         <v>7174.1</v>
       </c>
-      <c r="M41" s="202"/>
-      <c r="N41" s="201"/>
+      <c r="M41" s="201"/>
+      <c r="N41" s="200"/>
       <c r="P41" s="83"/>
       <c r="Q41" s="9"/>
     </row>
@@ -5097,11 +5126,11 @@
       <c r="A42" s="20"/>
       <c r="B42" s="21"/>
       <c r="C42" s="84"/>
-      <c r="D42" s="197"/>
-      <c r="E42" s="198"/>
-      <c r="F42" s="199"/>
+      <c r="D42" s="196"/>
+      <c r="E42" s="197"/>
+      <c r="F42" s="198"/>
       <c r="G42" s="26"/>
-      <c r="H42" s="200"/>
+      <c r="H42" s="199"/>
       <c r="I42" s="85"/>
       <c r="J42" s="67" t="s">
         <v>109</v>
@@ -5112,8 +5141,8 @@
       <c r="L42" s="75">
         <v>2552</v>
       </c>
-      <c r="M42" s="202"/>
-      <c r="N42" s="201"/>
+      <c r="M42" s="201"/>
+      <c r="N42" s="200"/>
       <c r="P42" s="83"/>
       <c r="Q42" s="9"/>
     </row>
@@ -5121,11 +5150,11 @@
       <c r="A43" s="20"/>
       <c r="B43" s="21"/>
       <c r="C43" s="84"/>
-      <c r="D43" s="197"/>
-      <c r="E43" s="198"/>
-      <c r="F43" s="199"/>
+      <c r="D43" s="196"/>
+      <c r="E43" s="197"/>
+      <c r="F43" s="198"/>
       <c r="G43" s="26"/>
-      <c r="H43" s="200"/>
+      <c r="H43" s="199"/>
       <c r="I43" s="85"/>
       <c r="J43" s="67" t="s">
         <v>109</v>
@@ -5136,8 +5165,8 @@
       <c r="L43" s="75">
         <v>6994</v>
       </c>
-      <c r="M43" s="202"/>
-      <c r="N43" s="201"/>
+      <c r="M43" s="201"/>
+      <c r="N43" s="200"/>
       <c r="P43" s="83"/>
       <c r="Q43" s="9"/>
     </row>
@@ -5145,17 +5174,17 @@
       <c r="A44" s="20"/>
       <c r="B44" s="21"/>
       <c r="C44" s="84"/>
-      <c r="D44" s="197"/>
-      <c r="E44" s="198"/>
-      <c r="F44" s="199"/>
+      <c r="D44" s="196"/>
+      <c r="E44" s="197"/>
+      <c r="F44" s="198"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="200"/>
+      <c r="H44" s="199"/>
       <c r="I44" s="85"/>
       <c r="J44" s="67"/>
       <c r="K44" s="71"/>
       <c r="L44" s="75"/>
-      <c r="M44" s="202"/>
-      <c r="N44" s="201"/>
+      <c r="M44" s="201"/>
+      <c r="N44" s="200"/>
       <c r="P44" s="83"/>
       <c r="Q44" s="9"/>
     </row>
@@ -5163,17 +5192,17 @@
       <c r="A45" s="20"/>
       <c r="B45" s="21"/>
       <c r="C45" s="84"/>
-      <c r="D45" s="197"/>
-      <c r="E45" s="198"/>
-      <c r="F45" s="199"/>
+      <c r="D45" s="196"/>
+      <c r="E45" s="197"/>
+      <c r="F45" s="198"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="200"/>
+      <c r="H45" s="199"/>
       <c r="I45" s="85"/>
       <c r="J45" s="67"/>
       <c r="K45" s="71"/>
       <c r="L45" s="75"/>
-      <c r="M45" s="202"/>
-      <c r="N45" s="201"/>
+      <c r="M45" s="201"/>
+      <c r="N45" s="200"/>
       <c r="P45" s="83"/>
       <c r="Q45" s="9"/>
     </row>
@@ -5181,17 +5210,17 @@
       <c r="A46" s="20"/>
       <c r="B46" s="21"/>
       <c r="C46" s="84"/>
-      <c r="D46" s="197"/>
-      <c r="E46" s="198"/>
-      <c r="F46" s="199"/>
+      <c r="D46" s="196"/>
+      <c r="E46" s="197"/>
+      <c r="F46" s="198"/>
       <c r="G46" s="26"/>
-      <c r="H46" s="200"/>
+      <c r="H46" s="199"/>
       <c r="I46" s="85"/>
       <c r="J46" s="67"/>
       <c r="K46" s="71"/>
       <c r="L46" s="75"/>
-      <c r="M46" s="202"/>
-      <c r="N46" s="201"/>
+      <c r="M46" s="201"/>
+      <c r="N46" s="200"/>
       <c r="P46" s="83"/>
       <c r="Q46" s="9"/>
     </row>
@@ -5199,17 +5228,17 @@
       <c r="A47" s="20"/>
       <c r="B47" s="21"/>
       <c r="C47" s="84"/>
-      <c r="D47" s="197"/>
-      <c r="E47" s="198"/>
-      <c r="F47" s="199"/>
+      <c r="D47" s="196"/>
+      <c r="E47" s="197"/>
+      <c r="F47" s="198"/>
       <c r="G47" s="26"/>
-      <c r="H47" s="200"/>
+      <c r="H47" s="199"/>
       <c r="I47" s="85"/>
       <c r="J47" s="67"/>
       <c r="K47" s="71"/>
       <c r="L47" s="75"/>
-      <c r="M47" s="202"/>
-      <c r="N47" s="201"/>
+      <c r="M47" s="201"/>
+      <c r="N47" s="200"/>
       <c r="P47" s="83"/>
       <c r="Q47" s="9"/>
     </row>
@@ -5217,17 +5246,17 @@
       <c r="A48" s="20"/>
       <c r="B48" s="21"/>
       <c r="C48" s="84"/>
-      <c r="D48" s="197"/>
-      <c r="E48" s="198"/>
-      <c r="F48" s="199"/>
+      <c r="D48" s="196"/>
+      <c r="E48" s="197"/>
+      <c r="F48" s="198"/>
       <c r="G48" s="26"/>
-      <c r="H48" s="200"/>
+      <c r="H48" s="199"/>
       <c r="I48" s="85"/>
       <c r="J48" s="67"/>
       <c r="K48" s="71"/>
       <c r="L48" s="75"/>
-      <c r="M48" s="202"/>
-      <c r="N48" s="201"/>
+      <c r="M48" s="201"/>
+      <c r="N48" s="200"/>
       <c r="P48" s="83"/>
       <c r="Q48" s="9"/>
     </row>
@@ -5242,7 +5271,7 @@
       <c r="F49" s="84"/>
       <c r="H49" s="91"/>
       <c r="I49" s="85"/>
-      <c r="J49" s="203"/>
+      <c r="J49" s="202"/>
       <c r="K49" s="86"/>
       <c r="L49" s="9"/>
       <c r="M49" s="87"/>
@@ -5298,29 +5327,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="237" t="s">
+      <c r="H52" s="219" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="238"/>
+      <c r="I52" s="220"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="239">
+      <c r="K52" s="221">
         <f>I50+L50</f>
         <v>80916.84</v>
       </c>
-      <c r="L52" s="240"/>
-      <c r="M52" s="228">
+      <c r="L52" s="222"/>
+      <c r="M52" s="210">
         <f>N39+M39</f>
         <v>1422075.47</v>
       </c>
-      <c r="N52" s="229"/>
+      <c r="N52" s="211"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="241" t="s">
+      <c r="D53" s="223" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="241"/>
+      <c r="E53" s="223"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1396181.44</v>
@@ -5331,22 +5360,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="242" t="s">
+      <c r="D54" s="224" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="242"/>
+      <c r="E54" s="224"/>
       <c r="F54" s="102">
         <v>-1523111</v>
       </c>
-      <c r="I54" s="243" t="s">
+      <c r="I54" s="225" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="244"/>
-      <c r="K54" s="245">
+      <c r="J54" s="226"/>
+      <c r="K54" s="227">
         <f>F56+F57+F58</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L54" s="246"/>
+      <c r="L54" s="228"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -5377,10 +5406,10 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="230">
-        <v>0</v>
-      </c>
-      <c r="L56" s="231"/>
+      <c r="K56" s="212">
+        <v>0</v>
+      </c>
+      <c r="L56" s="213"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -5397,22 +5426,22 @@
       <c r="C58" s="120">
         <v>44444</v>
       </c>
-      <c r="D58" s="232" t="s">
+      <c r="D58" s="214" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="233"/>
+      <c r="E58" s="215"/>
       <c r="F58" s="121">
         <v>136234.76999999999</v>
       </c>
-      <c r="I58" s="234" t="s">
+      <c r="I58" s="216" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="235"/>
-      <c r="K58" s="236">
+      <c r="J58" s="217"/>
+      <c r="K58" s="218">
         <f>K54+K56</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L58" s="236"/>
+      <c r="L58" s="218"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -5422,20 +5451,20 @@
       <c r="J59" s="126"/>
     </row>
     <row r="60" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I60" s="195"/>
-      <c r="J60" s="195"/>
-      <c r="K60" s="196"/>
-      <c r="L60" s="196"/>
+      <c r="I60" s="194"/>
+      <c r="J60" s="194"/>
+      <c r="K60" s="195"/>
+      <c r="L60" s="195"/>
     </row>
     <row r="61" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="127"/>
       <c r="C61" s="128"/>
       <c r="D61" s="129"/>
       <c r="E61" s="83"/>
-      <c r="I61" s="195"/>
-      <c r="J61" s="195"/>
-      <c r="K61" s="196"/>
-      <c r="L61" s="196"/>
+      <c r="I61" s="194"/>
+      <c r="J61" s="194"/>
+      <c r="K61" s="195"/>
+      <c r="L61" s="195"/>
       <c r="M61" s="1"/>
       <c r="N61" s="104"/>
     </row>
@@ -5556,6 +5585,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C1:M1"/>
     <mergeCell ref="M52:N52"/>
     <mergeCell ref="K56:L56"/>
     <mergeCell ref="D58:E58"/>
@@ -5567,15 +5605,6 @@
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="C1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5641,13 +5670,13 @@
       <c r="A3" s="141">
         <v>44422</v>
       </c>
-      <c r="B3" s="182">
+      <c r="B3" s="181">
         <v>2232</v>
       </c>
       <c r="C3" s="35">
         <v>3015.96</v>
       </c>
-      <c r="D3" s="247" t="s">
+      <c r="D3" s="246" t="s">
         <v>50</v>
       </c>
       <c r="E3" s="9"/>
@@ -5660,14 +5689,14 @@
       <c r="A4" s="141">
         <v>44422</v>
       </c>
-      <c r="B4" s="182">
+      <c r="B4" s="181">
         <v>2233</v>
       </c>
       <c r="C4" s="35">
         <v>10281</v>
       </c>
-      <c r="D4" s="248"/>
-      <c r="E4" s="183"/>
+      <c r="D4" s="247"/>
+      <c r="E4" s="182"/>
       <c r="F4" s="145">
         <f>F3+C4-E4</f>
         <v>13296.96</v>
@@ -5678,14 +5707,14 @@
       <c r="A5" s="141">
         <v>44422</v>
       </c>
-      <c r="B5" s="182">
+      <c r="B5" s="181">
         <v>2234</v>
       </c>
       <c r="C5" s="35">
         <v>12746.2</v>
       </c>
-      <c r="D5" s="248"/>
-      <c r="E5" s="183"/>
+      <c r="D5" s="247"/>
+      <c r="E5" s="182"/>
       <c r="F5" s="145">
         <f t="shared" ref="F5:F68" si="0">F4+C5-E5</f>
         <v>26043.16</v>
@@ -5695,14 +5724,14 @@
       <c r="A6" s="141">
         <v>44422</v>
       </c>
-      <c r="B6" s="182">
+      <c r="B6" s="181">
         <v>2235</v>
       </c>
       <c r="C6" s="35">
         <v>28974.78</v>
       </c>
-      <c r="D6" s="248"/>
-      <c r="E6" s="183"/>
+      <c r="D6" s="247"/>
+      <c r="E6" s="182"/>
       <c r="F6" s="145">
         <f t="shared" si="0"/>
         <v>55017.94</v>
@@ -5712,14 +5741,14 @@
       <c r="A7" s="141">
         <v>44422</v>
       </c>
-      <c r="B7" s="182">
+      <c r="B7" s="181">
         <v>2236</v>
       </c>
       <c r="C7" s="35">
         <v>44758.6</v>
       </c>
-      <c r="D7" s="248"/>
-      <c r="E7" s="183"/>
+      <c r="D7" s="247"/>
+      <c r="E7" s="182"/>
       <c r="F7" s="145">
         <f t="shared" si="0"/>
         <v>99776.540000000008</v>
@@ -5729,14 +5758,14 @@
       <c r="A8" s="141">
         <v>44422</v>
       </c>
-      <c r="B8" s="182">
+      <c r="B8" s="181">
         <v>2237</v>
       </c>
       <c r="C8" s="35">
         <v>12841.78</v>
       </c>
-      <c r="D8" s="248"/>
-      <c r="E8" s="183"/>
+      <c r="D8" s="247"/>
+      <c r="E8" s="182"/>
       <c r="F8" s="145">
         <f t="shared" si="0"/>
         <v>112618.32</v>
@@ -5746,14 +5775,14 @@
       <c r="A9" s="141">
         <v>44422</v>
       </c>
-      <c r="B9" s="182">
+      <c r="B9" s="181">
         <v>2238</v>
       </c>
       <c r="C9" s="35">
         <v>3898.05</v>
       </c>
-      <c r="D9" s="248"/>
-      <c r="E9" s="183"/>
+      <c r="D9" s="247"/>
+      <c r="E9" s="182"/>
       <c r="F9" s="145">
         <f t="shared" si="0"/>
         <v>116516.37000000001</v>
@@ -5763,14 +5792,14 @@
       <c r="A10" s="141">
         <v>44422</v>
       </c>
-      <c r="B10" s="182">
+      <c r="B10" s="181">
         <v>2239</v>
       </c>
       <c r="C10" s="35">
         <v>1429</v>
       </c>
-      <c r="D10" s="249"/>
-      <c r="E10" s="183"/>
+      <c r="D10" s="248"/>
+      <c r="E10" s="182"/>
       <c r="F10" s="145">
         <f t="shared" si="0"/>
         <v>117945.37000000001</v>
@@ -5781,7 +5810,7 @@
       <c r="A11" s="141"/>
       <c r="B11" s="142"/>
       <c r="C11" s="79"/>
-      <c r="D11" s="184">
+      <c r="D11" s="183">
         <v>44428</v>
       </c>
       <c r="E11" s="79">
@@ -5927,7 +5956,7 @@
       <c r="E19" s="79">
         <v>216899.43</v>
       </c>
-      <c r="F19" s="185">
+      <c r="F19" s="184">
         <f t="shared" si="0"/>
         <v>40000</v>
       </c>
@@ -6068,7 +6097,7 @@
       <c r="E27" s="79">
         <v>235944.57</v>
       </c>
-      <c r="F27" s="185">
+      <c r="F27" s="184">
         <f t="shared" si="0"/>
         <v>30024.739999999991</v>
       </c>
@@ -6656,9 +6685,9 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="191"/>
-      <c r="B63" s="188"/>
-      <c r="C63" s="189"/>
+      <c r="A63" s="190"/>
+      <c r="B63" s="187"/>
+      <c r="C63" s="188"/>
       <c r="D63" s="144"/>
       <c r="E63" s="79"/>
       <c r="F63" s="145">
@@ -6667,9 +6696,9 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="191"/>
-      <c r="B64" s="188"/>
-      <c r="C64" s="189"/>
+      <c r="A64" s="190"/>
+      <c r="B64" s="187"/>
+      <c r="C64" s="188"/>
       <c r="D64" s="144"/>
       <c r="E64" s="79"/>
       <c r="F64" s="145">
@@ -6678,9 +6707,9 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="191"/>
-      <c r="B65" s="188"/>
-      <c r="C65" s="189"/>
+      <c r="A65" s="190"/>
+      <c r="B65" s="187"/>
+      <c r="C65" s="188"/>
       <c r="D65" s="144"/>
       <c r="E65" s="79"/>
       <c r="F65" s="145">
@@ -6689,9 +6718,9 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="191"/>
-      <c r="B66" s="188"/>
-      <c r="C66" s="189"/>
+      <c r="A66" s="190"/>
+      <c r="B66" s="187"/>
+      <c r="C66" s="188"/>
       <c r="D66" s="144"/>
       <c r="E66" s="79"/>
       <c r="F66" s="145">
@@ -6700,9 +6729,9 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="191"/>
-      <c r="B67" s="188"/>
-      <c r="C67" s="189"/>
+      <c r="A67" s="190"/>
+      <c r="B67" s="187"/>
+      <c r="C67" s="188"/>
       <c r="D67" s="144"/>
       <c r="E67" s="79"/>
       <c r="F67" s="145">
@@ -6711,9 +6740,9 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="191"/>
-      <c r="B68" s="188"/>
-      <c r="C68" s="189"/>
+      <c r="A68" s="190"/>
+      <c r="B68" s="187"/>
+      <c r="C68" s="188"/>
       <c r="D68" s="144"/>
       <c r="E68" s="79"/>
       <c r="F68" s="145">
@@ -6722,9 +6751,9 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="191"/>
-      <c r="B69" s="188"/>
-      <c r="C69" s="189"/>
+      <c r="A69" s="190"/>
+      <c r="B69" s="187"/>
+      <c r="C69" s="188"/>
       <c r="D69" s="144"/>
       <c r="E69" s="79"/>
       <c r="F69" s="145">
@@ -6733,9 +6762,9 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="191"/>
-      <c r="B70" s="188"/>
-      <c r="C70" s="189"/>
+      <c r="A70" s="190"/>
+      <c r="B70" s="187"/>
+      <c r="C70" s="188"/>
       <c r="D70" s="144"/>
       <c r="E70" s="79"/>
       <c r="F70" s="145">
@@ -6744,9 +6773,9 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="191"/>
-      <c r="B71" s="188"/>
-      <c r="C71" s="189"/>
+      <c r="A71" s="190"/>
+      <c r="B71" s="187"/>
+      <c r="C71" s="188"/>
       <c r="D71" s="144"/>
       <c r="E71" s="79"/>
       <c r="F71" s="145">
@@ -6755,9 +6784,9 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="191"/>
-      <c r="B72" s="188"/>
-      <c r="C72" s="189"/>
+      <c r="A72" s="190"/>
+      <c r="B72" s="187"/>
+      <c r="C72" s="188"/>
       <c r="D72" s="144"/>
       <c r="E72" s="79"/>
       <c r="F72" s="145">
@@ -6766,9 +6795,9 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="191"/>
-      <c r="B73" s="188"/>
-      <c r="C73" s="189"/>
+      <c r="A73" s="190"/>
+      <c r="B73" s="187"/>
+      <c r="C73" s="188"/>
       <c r="D73" s="144"/>
       <c r="E73" s="79"/>
       <c r="F73" s="145">
@@ -6777,9 +6806,9 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="191"/>
-      <c r="B74" s="188"/>
-      <c r="C74" s="189"/>
+      <c r="A74" s="190"/>
+      <c r="B74" s="187"/>
+      <c r="C74" s="188"/>
       <c r="D74" s="144"/>
       <c r="E74" s="79"/>
       <c r="F74" s="145">
@@ -6788,9 +6817,9 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="191"/>
-      <c r="B75" s="188"/>
-      <c r="C75" s="189"/>
+      <c r="A75" s="190"/>
+      <c r="B75" s="187"/>
+      <c r="C75" s="188"/>
       <c r="D75" s="144"/>
       <c r="E75" s="79"/>
       <c r="F75" s="145">
@@ -6799,9 +6828,9 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="191"/>
-      <c r="B76" s="188"/>
-      <c r="C76" s="189"/>
+      <c r="A76" s="190"/>
+      <c r="B76" s="187"/>
+      <c r="C76" s="188"/>
       <c r="D76" s="144"/>
       <c r="E76" s="79"/>
       <c r="F76" s="145">
@@ -6810,9 +6839,9 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="191"/>
-      <c r="B77" s="188"/>
-      <c r="C77" s="189"/>
+      <c r="A77" s="190"/>
+      <c r="B77" s="187"/>
+      <c r="C77" s="188"/>
       <c r="D77" s="144"/>
       <c r="E77" s="79"/>
       <c r="F77" s="145">
@@ -6821,9 +6850,9 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="191"/>
-      <c r="B78" s="188"/>
-      <c r="C78" s="189"/>
+      <c r="A78" s="190"/>
+      <c r="B78" s="187"/>
+      <c r="C78" s="188"/>
       <c r="D78" s="144"/>
       <c r="E78" s="79"/>
       <c r="F78" s="145">
@@ -6832,9 +6861,9 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="191"/>
-      <c r="B79" s="188"/>
-      <c r="C79" s="189"/>
+      <c r="A79" s="190"/>
+      <c r="B79" s="187"/>
+      <c r="C79" s="188"/>
       <c r="D79" s="144"/>
       <c r="E79" s="79"/>
       <c r="F79" s="145">
@@ -6843,9 +6872,9 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="191"/>
-      <c r="B80" s="188"/>
-      <c r="C80" s="189"/>
+      <c r="A80" s="190"/>
+      <c r="B80" s="187"/>
+      <c r="C80" s="188"/>
       <c r="D80" s="144"/>
       <c r="E80" s="79"/>
       <c r="F80" s="145">
@@ -6854,9 +6883,9 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="192"/>
-      <c r="B81" s="193"/>
-      <c r="C81" s="194"/>
+      <c r="A81" s="191"/>
+      <c r="B81" s="192"/>
+      <c r="C81" s="193"/>
       <c r="D81" s="147"/>
       <c r="E81" s="83"/>
       <c r="F81" s="145">
@@ -6865,9 +6894,9 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="192"/>
-      <c r="B82" s="193"/>
-      <c r="C82" s="194"/>
+      <c r="A82" s="191"/>
+      <c r="B82" s="192"/>
+      <c r="C82" s="193"/>
       <c r="D82" s="147"/>
       <c r="E82" s="83"/>
       <c r="F82" s="145">
@@ -6876,9 +6905,9 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="192"/>
-      <c r="B83" s="193"/>
-      <c r="C83" s="194"/>
+      <c r="A83" s="191"/>
+      <c r="B83" s="192"/>
+      <c r="C83" s="193"/>
       <c r="D83" s="147"/>
       <c r="E83" s="83"/>
       <c r="F83" s="145">
@@ -6887,9 +6916,9 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="192"/>
-      <c r="B84" s="193"/>
-      <c r="C84" s="194"/>
+      <c r="A84" s="191"/>
+      <c r="B84" s="192"/>
+      <c r="C84" s="193"/>
       <c r="D84" s="147"/>
       <c r="E84" s="83"/>
       <c r="F84" s="145">
@@ -6898,9 +6927,9 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="192"/>
-      <c r="B85" s="193"/>
-      <c r="C85" s="194"/>
+      <c r="A85" s="191"/>
+      <c r="B85" s="192"/>
+      <c r="C85" s="193"/>
       <c r="D85" s="147"/>
       <c r="E85" s="83"/>
       <c r="F85" s="145">
@@ -6909,9 +6938,9 @@
       </c>
     </row>
     <row r="86" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="192"/>
-      <c r="B86" s="193"/>
-      <c r="C86" s="194"/>
+      <c r="A86" s="191"/>
+      <c r="B86" s="192"/>
+      <c r="C86" s="193"/>
       <c r="D86" s="147"/>
       <c r="E86" s="83"/>
       <c r="F86" s="145">
@@ -6920,9 +6949,9 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="191"/>
-      <c r="B87" s="188"/>
-      <c r="C87" s="189"/>
+      <c r="A87" s="190"/>
+      <c r="B87" s="187"/>
+      <c r="C87" s="188"/>
       <c r="D87" s="148"/>
       <c r="E87" s="79"/>
       <c r="F87" s="145">
@@ -6931,9 +6960,9 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="191"/>
-      <c r="B88" s="188"/>
-      <c r="C88" s="189"/>
+      <c r="A88" s="190"/>
+      <c r="B88" s="187"/>
+      <c r="C88" s="188"/>
       <c r="D88" s="148"/>
       <c r="E88" s="79"/>
       <c r="F88" s="145">
@@ -6942,9 +6971,9 @@
       </c>
     </row>
     <row r="89" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="191"/>
-      <c r="B89" s="188"/>
-      <c r="C89" s="189"/>
+      <c r="A89" s="190"/>
+      <c r="B89" s="187"/>
+      <c r="C89" s="188"/>
       <c r="D89" s="148"/>
       <c r="E89" s="79"/>
       <c r="F89" s="145">
@@ -6953,9 +6982,9 @@
       </c>
     </row>
     <row r="90" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="191"/>
-      <c r="B90" s="188"/>
-      <c r="C90" s="189"/>
+      <c r="A90" s="190"/>
+      <c r="B90" s="187"/>
+      <c r="C90" s="188"/>
       <c r="D90" s="148"/>
       <c r="E90" s="79"/>
       <c r="F90" s="145">
@@ -6964,9 +6993,9 @@
       </c>
     </row>
     <row r="91" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="191"/>
-      <c r="B91" s="188"/>
-      <c r="C91" s="189"/>
+      <c r="A91" s="190"/>
+      <c r="B91" s="187"/>
+      <c r="C91" s="188"/>
       <c r="D91" s="148"/>
       <c r="E91" s="79"/>
       <c r="F91" s="145">
@@ -6975,9 +7004,9 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="191"/>
-      <c r="B92" s="188"/>
-      <c r="C92" s="189"/>
+      <c r="A92" s="190"/>
+      <c r="B92" s="187"/>
+      <c r="C92" s="188"/>
       <c r="D92" s="148"/>
       <c r="E92" s="79"/>
       <c r="F92" s="145">
@@ -6986,9 +7015,9 @@
       </c>
     </row>
     <row r="93" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="191"/>
-      <c r="B93" s="188"/>
-      <c r="C93" s="189"/>
+      <c r="A93" s="190"/>
+      <c r="B93" s="187"/>
+      <c r="C93" s="188"/>
       <c r="D93" s="148"/>
       <c r="E93" s="79"/>
       <c r="F93" s="145">
@@ -6997,9 +7026,9 @@
       </c>
     </row>
     <row r="94" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="191"/>
-      <c r="B94" s="188"/>
-      <c r="C94" s="189"/>
+      <c r="A94" s="190"/>
+      <c r="B94" s="187"/>
+      <c r="C94" s="188"/>
       <c r="D94" s="148"/>
       <c r="E94" s="79"/>
       <c r="F94" s="145">
@@ -7008,9 +7037,9 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="191"/>
-      <c r="B95" s="188"/>
-      <c r="C95" s="189"/>
+      <c r="A95" s="190"/>
+      <c r="B95" s="187"/>
+      <c r="C95" s="188"/>
       <c r="D95" s="148"/>
       <c r="E95" s="79"/>
       <c r="F95" s="145">
@@ -7019,9 +7048,9 @@
       </c>
     </row>
     <row r="96" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="191"/>
-      <c r="B96" s="188"/>
-      <c r="C96" s="189"/>
+      <c r="A96" s="190"/>
+      <c r="B96" s="187"/>
+      <c r="C96" s="188"/>
       <c r="D96" s="148"/>
       <c r="E96" s="79"/>
       <c r="F96" s="145">
@@ -7264,10 +7293,10 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:R80"/>
+  <dimension ref="A1:S80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="N43" sqref="N43"/>
+    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7289,23 +7318,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="217"/>
-      <c r="C1" s="226" t="s">
+      <c r="B1" s="235"/>
+      <c r="C1" s="244" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="227"/>
-      <c r="E1" s="227"/>
-      <c r="F1" s="227"/>
-      <c r="G1" s="227"/>
-      <c r="H1" s="227"/>
-      <c r="I1" s="227"/>
-      <c r="J1" s="227"/>
-      <c r="K1" s="227"/>
-      <c r="L1" s="227"/>
-      <c r="M1" s="227"/>
+      <c r="D1" s="245"/>
+      <c r="E1" s="245"/>
+      <c r="F1" s="245"/>
+      <c r="G1" s="245"/>
+      <c r="H1" s="245"/>
+      <c r="I1" s="245"/>
+      <c r="J1" s="245"/>
+      <c r="K1" s="245"/>
+      <c r="L1" s="245"/>
+      <c r="M1" s="245"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="218"/>
+      <c r="B2" s="236"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -7315,17 +7344,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="219" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="220"/>
+      <c r="B3" s="237" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="238"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="221" t="s">
+      <c r="H3" s="239" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="221"/>
+      <c r="I3" s="239"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -7341,14 +7370,14 @@
       <c r="D4" s="16">
         <v>44444</v>
       </c>
-      <c r="E4" s="222" t="s">
+      <c r="E4" s="240" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="223"/>
-      <c r="H4" s="224" t="s">
+      <c r="F4" s="241"/>
+      <c r="H4" s="242" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="225"/>
+      <c r="I4" s="243"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -7358,10 +7387,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="211" t="s">
+      <c r="P4" s="229" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="212"/>
+      <c r="Q4" s="230"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -7527,12 +7556,12 @@
       <c r="N8" s="30">
         <v>4257</v>
       </c>
-      <c r="O8" s="209"/>
+      <c r="O8" s="208"/>
       <c r="P8" s="83">
         <f t="shared" si="0"/>
         <v>50471</v>
       </c>
-      <c r="Q8" s="186">
+      <c r="Q8" s="185">
         <f t="shared" si="1"/>
         <v>-40</v>
       </c>
@@ -7706,12 +7735,12 @@
       <c r="N12" s="30">
         <v>2198</v>
       </c>
-      <c r="O12" s="210"/>
+      <c r="O12" s="209"/>
       <c r="P12" s="83">
         <f t="shared" si="0"/>
         <v>46630</v>
       </c>
-      <c r="Q12" s="186">
+      <c r="Q12" s="185">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
@@ -7759,7 +7788,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R13" s="207"/>
+      <c r="R13" s="206"/>
     </row>
     <row r="14" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="20"/>
@@ -7803,7 +7832,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R14" s="207"/>
+      <c r="R14" s="206"/>
     </row>
     <row r="15" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="20"/>
@@ -7889,7 +7918,7 @@
       </c>
       <c r="R16" s="26"/>
     </row>
-    <row r="17" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="20"/>
       <c r="B17" s="21">
         <v>44426</v>
@@ -7939,7 +7968,7 @@
       </c>
       <c r="R17" s="26"/>
     </row>
-    <row r="18" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="20"/>
       <c r="B18" s="21">
         <v>44427</v>
@@ -7983,7 +8012,7 @@
       </c>
       <c r="R18" s="26"/>
     </row>
-    <row r="19" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="20"/>
       <c r="B19" s="21">
         <v>44428</v>
@@ -8027,7 +8056,7 @@
       </c>
       <c r="R19" s="26"/>
     </row>
-    <row r="20" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="20"/>
       <c r="B20" s="21">
         <v>44429</v>
@@ -8071,7 +8100,7 @@
       </c>
       <c r="R20" s="26"/>
     </row>
-    <row r="21" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="20"/>
       <c r="B21" s="21">
         <v>44430</v>
@@ -8094,7 +8123,7 @@
         <v>12</v>
       </c>
       <c r="J21" s="33"/>
-      <c r="K21" s="180"/>
+      <c r="K21" s="179"/>
       <c r="L21" s="43"/>
       <c r="M21" s="138">
         <f>20000+20650</f>
@@ -8113,7 +8142,7 @@
       </c>
       <c r="R21" s="26"/>
     </row>
-    <row r="22" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="20"/>
       <c r="B22" s="21">
         <v>44431</v>
@@ -8122,7 +8151,7 @@
         <v>5051</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E22" s="24">
         <v>44462</v>
@@ -8157,7 +8186,7 @@
       </c>
       <c r="R22" s="26"/>
     </row>
-    <row r="23" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="20"/>
       <c r="B23" s="21">
         <v>44432</v>
@@ -8166,7 +8195,7 @@
         <v>8999</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E23" s="24">
         <v>44463</v>
@@ -8201,7 +8230,7 @@
       </c>
       <c r="R23" s="26"/>
     </row>
-    <row r="24" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="20"/>
       <c r="B24" s="21">
         <v>44433</v>
@@ -8210,7 +8239,7 @@
         <v>1265</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E24" s="24">
         <v>44464</v>
@@ -8229,7 +8258,7 @@
         <v>44464</v>
       </c>
       <c r="K24" s="56" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L24" s="57">
         <v>10900</v>
@@ -8251,89 +8280,100 @@
       </c>
       <c r="R24" s="26"/>
     </row>
-    <row r="25" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="20"/>
       <c r="B25" s="21">
         <v>44434</v>
       </c>
       <c r="C25" s="22">
-        <v>0</v>
-      </c>
-      <c r="D25" s="31"/>
+        <v>132</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>157</v>
+      </c>
       <c r="E25" s="24">
         <v>44465</v>
       </c>
       <c r="F25" s="25">
-        <v>0</v>
+        <v>73362</v>
       </c>
       <c r="G25" s="26"/>
       <c r="H25" s="32">
         <v>44465</v>
       </c>
       <c r="I25" s="28">
-        <v>0</v>
-      </c>
-      <c r="J25" s="58"/>
+        <v>3000</v>
+      </c>
+      <c r="J25" s="58" t="s">
+        <v>158</v>
+      </c>
       <c r="K25" s="59"/>
       <c r="L25" s="60"/>
       <c r="M25" s="138">
-        <v>0</v>
+        <f>55000+11514</f>
+        <v>66514</v>
       </c>
       <c r="N25" s="30">
-        <v>0</v>
+        <v>3716</v>
       </c>
       <c r="P25" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>73362</v>
       </c>
       <c r="Q25" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R25" s="26"/>
-    </row>
-    <row r="26" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="20"/>
       <c r="B26" s="21">
         <v>44435</v>
       </c>
       <c r="C26" s="22">
-        <v>0</v>
-      </c>
-      <c r="D26" s="31"/>
+        <v>3613.5</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>159</v>
+      </c>
       <c r="E26" s="24">
         <v>44466</v>
       </c>
       <c r="F26" s="25">
-        <v>0</v>
+        <v>50804</v>
       </c>
       <c r="G26" s="26"/>
       <c r="H26" s="32">
         <v>44466</v>
       </c>
       <c r="I26" s="28">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J26" s="33"/>
       <c r="K26" s="56"/>
       <c r="L26" s="43"/>
       <c r="M26" s="138">
-        <v>0</v>
+        <f>38000+9182+160</f>
+        <v>47342</v>
       </c>
       <c r="N26" s="30">
         <v>0</v>
       </c>
       <c r="P26" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q26" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>50963.5</v>
+      </c>
+      <c r="Q26" s="254">
+        <f t="shared" si="1"/>
+        <v>159.5</v>
       </c>
       <c r="R26" s="51"/>
     </row>
-    <row r="27" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="20"/>
       <c r="B27" s="21">
         <v>44436</v>
@@ -8346,109 +8386,116 @@
         <v>44467</v>
       </c>
       <c r="F27" s="25">
-        <v>0</v>
+        <v>60651</v>
       </c>
       <c r="G27" s="26"/>
       <c r="H27" s="32">
         <v>44467</v>
       </c>
       <c r="I27" s="28">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="J27" s="61"/>
       <c r="K27" s="62"/>
       <c r="L27" s="60"/>
       <c r="M27" s="138">
-        <v>0</v>
+        <f>30000+30510</f>
+        <v>60510</v>
       </c>
       <c r="N27" s="30">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="P27" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60652</v>
       </c>
       <c r="Q27" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R27" s="26"/>
     </row>
-    <row r="28" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="20"/>
       <c r="B28" s="21">
         <v>44437</v>
       </c>
       <c r="C28" s="22">
-        <v>0</v>
-      </c>
-      <c r="D28" s="38"/>
+        <v>1949</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>160</v>
+      </c>
       <c r="E28" s="24">
         <v>44468</v>
       </c>
       <c r="F28" s="25">
-        <v>0</v>
+        <v>35892</v>
       </c>
       <c r="G28" s="26"/>
       <c r="H28" s="32">
         <v>44468</v>
       </c>
       <c r="I28" s="28">
-        <v>0</v>
+        <v>1006</v>
       </c>
       <c r="J28" s="63"/>
       <c r="K28" s="34"/>
       <c r="L28" s="60"/>
       <c r="M28" s="138">
-        <v>0</v>
+        <f>22620+10000</f>
+        <v>32620</v>
       </c>
       <c r="N28" s="30">
-        <v>0</v>
+        <v>314</v>
       </c>
       <c r="P28" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35889</v>
       </c>
       <c r="Q28" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="R28" s="26"/>
     </row>
-    <row r="29" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="20"/>
       <c r="B29" s="21">
         <v>44438</v>
       </c>
       <c r="C29" s="22">
-        <v>0</v>
-      </c>
-      <c r="D29" s="64"/>
+        <v>1132</v>
+      </c>
+      <c r="D29" s="64" t="s">
+        <v>161</v>
+      </c>
       <c r="E29" s="24">
         <v>44469</v>
       </c>
       <c r="F29" s="25">
-        <v>0</v>
+        <v>55710</v>
       </c>
       <c r="G29" s="26"/>
       <c r="H29" s="32">
         <v>44469</v>
       </c>
       <c r="I29" s="28">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J29" s="65"/>
       <c r="K29" s="66"/>
       <c r="L29" s="60"/>
       <c r="M29" s="138">
-        <v>0</v>
+        <f>34562+20000</f>
+        <v>54562</v>
       </c>
       <c r="N29" s="30">
         <v>0</v>
       </c>
       <c r="P29" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>55710</v>
       </c>
       <c r="Q29" s="9">
         <f t="shared" si="1"/>
@@ -8456,40 +8503,43 @@
       </c>
       <c r="R29" s="26"/>
     </row>
-    <row r="30" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="20"/>
       <c r="B30" s="21">
         <v>44439</v>
       </c>
       <c r="C30" s="22">
-        <v>0</v>
-      </c>
-      <c r="D30" s="64"/>
+        <v>1812</v>
+      </c>
+      <c r="D30" s="64" t="s">
+        <v>166</v>
+      </c>
       <c r="E30" s="24">
         <v>44470</v>
       </c>
       <c r="F30" s="25">
-        <v>0</v>
+        <v>85895</v>
       </c>
       <c r="G30" s="26"/>
       <c r="H30" s="32">
         <v>44470</v>
       </c>
       <c r="I30" s="28">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J30" s="67"/>
       <c r="K30" s="68"/>
       <c r="L30" s="69"/>
       <c r="M30" s="138">
-        <v>0</v>
+        <f>25000+43321+100+14800</f>
+        <v>83221</v>
       </c>
       <c r="N30" s="30">
-        <v>0</v>
+        <v>852</v>
       </c>
       <c r="P30" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>85895</v>
       </c>
       <c r="Q30" s="9">
         <f t="shared" si="1"/>
@@ -8497,7 +8547,7 @@
       </c>
       <c r="R30" s="26"/>
     </row>
-    <row r="31" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="20"/>
       <c r="B31" s="21">
         <v>44440</v>
@@ -8538,7 +8588,7 @@
       </c>
       <c r="R31" s="26"/>
     </row>
-    <row r="32" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="20"/>
       <c r="B32" s="21">
         <v>44441</v>
@@ -8622,28 +8672,22 @@
     </row>
     <row r="34" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="20"/>
-      <c r="B34" s="21">
-        <v>44443</v>
-      </c>
+      <c r="B34" s="21"/>
       <c r="C34" s="22">
         <v>0</v>
       </c>
       <c r="D34" s="73"/>
-      <c r="E34" s="24">
-        <v>44474</v>
-      </c>
+      <c r="E34" s="24"/>
       <c r="F34" s="25">
         <v>0</v>
       </c>
       <c r="G34" s="26"/>
-      <c r="H34" s="32">
-        <v>44474</v>
-      </c>
+      <c r="H34" s="32"/>
       <c r="I34" s="28">
         <v>0</v>
       </c>
       <c r="J34" s="67"/>
-      <c r="K34" s="187"/>
+      <c r="K34" s="186"/>
       <c r="L34" s="76"/>
       <c r="M34" s="138">
         <v>0</v>
@@ -8663,23 +8707,17 @@
     </row>
     <row r="35" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="20"/>
-      <c r="B35" s="21">
-        <v>44444</v>
-      </c>
+      <c r="B35" s="21"/>
       <c r="C35" s="22">
         <v>0</v>
       </c>
       <c r="D35" s="77"/>
-      <c r="E35" s="24">
-        <v>44475</v>
-      </c>
+      <c r="E35" s="24"/>
       <c r="F35" s="25">
         <v>0</v>
       </c>
       <c r="G35" s="26"/>
-      <c r="H35" s="32">
-        <v>44475</v>
-      </c>
+      <c r="H35" s="32"/>
       <c r="I35" s="28">
         <v>0</v>
       </c>
@@ -8754,7 +8792,7 @@
         <v>0</v>
       </c>
       <c r="J37" s="67"/>
-      <c r="K37" s="187"/>
+      <c r="K37" s="186"/>
       <c r="L37" s="76"/>
       <c r="M37" s="138">
         <v>0</v>
@@ -8816,21 +8854,21 @@
       <c r="J39" s="67"/>
       <c r="K39" s="82"/>
       <c r="L39" s="69"/>
-      <c r="M39" s="213">
+      <c r="M39" s="231">
         <f>SUM(M5:M38)</f>
-        <v>986386</v>
-      </c>
-      <c r="N39" s="215">
+        <v>1331155</v>
+      </c>
+      <c r="N39" s="233">
         <f>SUM(N5:N38)</f>
-        <v>38402</v>
+        <v>43306</v>
       </c>
       <c r="P39" s="83">
         <f>SUM(P5:P38)</f>
-        <v>1107137.1499999999</v>
+        <v>1469608.65</v>
       </c>
       <c r="Q39" s="9">
         <f>SUM(Q5:Q38)</f>
-        <v>16.150000000001455</v>
+        <v>173.65000000000146</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -8846,8 +8884,8 @@
       <c r="J40" s="67"/>
       <c r="K40" s="71"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="214"/>
-      <c r="N40" s="216"/>
+      <c r="M40" s="232"/>
+      <c r="N40" s="234"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -8855,17 +8893,17 @@
       <c r="A41" s="20"/>
       <c r="B41" s="21"/>
       <c r="C41" s="84"/>
-      <c r="D41" s="197"/>
-      <c r="E41" s="198"/>
-      <c r="F41" s="199"/>
+      <c r="D41" s="196"/>
+      <c r="E41" s="197"/>
+      <c r="F41" s="198"/>
       <c r="G41" s="26"/>
-      <c r="H41" s="200"/>
+      <c r="H41" s="199"/>
       <c r="I41" s="85"/>
       <c r="J41" s="67"/>
       <c r="K41" s="71"/>
       <c r="L41" s="75"/>
-      <c r="M41" s="202"/>
-      <c r="N41" s="201"/>
+      <c r="M41" s="201"/>
+      <c r="N41" s="200"/>
       <c r="P41" s="83"/>
       <c r="Q41" s="9"/>
     </row>
@@ -8873,17 +8911,17 @@
       <c r="A42" s="20"/>
       <c r="B42" s="21"/>
       <c r="C42" s="84"/>
-      <c r="D42" s="197"/>
-      <c r="E42" s="198"/>
-      <c r="F42" s="199"/>
+      <c r="D42" s="196"/>
+      <c r="E42" s="197"/>
+      <c r="F42" s="198"/>
       <c r="G42" s="26"/>
-      <c r="H42" s="200"/>
+      <c r="H42" s="199"/>
       <c r="I42" s="85"/>
       <c r="J42" s="67"/>
       <c r="K42" s="71"/>
       <c r="L42" s="75"/>
-      <c r="M42" s="202"/>
-      <c r="N42" s="201"/>
+      <c r="M42" s="201"/>
+      <c r="N42" s="200"/>
       <c r="P42" s="83"/>
       <c r="Q42" s="9"/>
     </row>
@@ -8891,17 +8929,17 @@
       <c r="A43" s="20"/>
       <c r="B43" s="21"/>
       <c r="C43" s="84"/>
-      <c r="D43" s="197"/>
-      <c r="E43" s="198"/>
-      <c r="F43" s="199"/>
+      <c r="D43" s="196"/>
+      <c r="E43" s="197"/>
+      <c r="F43" s="198"/>
       <c r="G43" s="26"/>
-      <c r="H43" s="200"/>
+      <c r="H43" s="199"/>
       <c r="I43" s="85"/>
       <c r="J43" s="67"/>
       <c r="K43" s="71"/>
       <c r="L43" s="75"/>
-      <c r="M43" s="202"/>
-      <c r="N43" s="201"/>
+      <c r="M43" s="201"/>
+      <c r="N43" s="200"/>
       <c r="P43" s="83"/>
       <c r="Q43" s="9"/>
     </row>
@@ -8909,17 +8947,17 @@
       <c r="A44" s="20"/>
       <c r="B44" s="21"/>
       <c r="C44" s="84"/>
-      <c r="D44" s="197"/>
-      <c r="E44" s="198"/>
-      <c r="F44" s="199"/>
+      <c r="D44" s="196"/>
+      <c r="E44" s="197"/>
+      <c r="F44" s="198"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="200"/>
+      <c r="H44" s="199"/>
       <c r="I44" s="85"/>
       <c r="J44" s="67"/>
       <c r="K44" s="71"/>
       <c r="L44" s="75"/>
-      <c r="M44" s="202"/>
-      <c r="N44" s="201"/>
+      <c r="M44" s="201"/>
+      <c r="N44" s="200"/>
       <c r="P44" s="83"/>
       <c r="Q44" s="9"/>
     </row>
@@ -8927,17 +8965,17 @@
       <c r="A45" s="20"/>
       <c r="B45" s="21"/>
       <c r="C45" s="84"/>
-      <c r="D45" s="197"/>
-      <c r="E45" s="198"/>
-      <c r="F45" s="199"/>
+      <c r="D45" s="196"/>
+      <c r="E45" s="197"/>
+      <c r="F45" s="198"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="200"/>
+      <c r="H45" s="199"/>
       <c r="I45" s="85"/>
       <c r="J45" s="67"/>
       <c r="K45" s="71"/>
       <c r="L45" s="75"/>
-      <c r="M45" s="202"/>
-      <c r="N45" s="201"/>
+      <c r="M45" s="201"/>
+      <c r="N45" s="200"/>
       <c r="P45" s="83"/>
       <c r="Q45" s="9"/>
     </row>
@@ -8945,17 +8983,17 @@
       <c r="A46" s="20"/>
       <c r="B46" s="21"/>
       <c r="C46" s="84"/>
-      <c r="D46" s="197"/>
-      <c r="E46" s="198"/>
-      <c r="F46" s="199"/>
+      <c r="D46" s="196"/>
+      <c r="E46" s="197"/>
+      <c r="F46" s="198"/>
       <c r="G46" s="26"/>
-      <c r="H46" s="200"/>
+      <c r="H46" s="199"/>
       <c r="I46" s="85"/>
       <c r="J46" s="67"/>
       <c r="K46" s="71"/>
       <c r="L46" s="75"/>
-      <c r="M46" s="202"/>
-      <c r="N46" s="201"/>
+      <c r="M46" s="201"/>
+      <c r="N46" s="200"/>
       <c r="P46" s="83"/>
       <c r="Q46" s="9"/>
     </row>
@@ -8963,17 +9001,17 @@
       <c r="A47" s="20"/>
       <c r="B47" s="21"/>
       <c r="C47" s="84"/>
-      <c r="D47" s="197"/>
-      <c r="E47" s="198"/>
-      <c r="F47" s="199"/>
+      <c r="D47" s="196"/>
+      <c r="E47" s="197"/>
+      <c r="F47" s="198"/>
       <c r="G47" s="26"/>
-      <c r="H47" s="200"/>
+      <c r="H47" s="199"/>
       <c r="I47" s="85"/>
       <c r="J47" s="67"/>
       <c r="K47" s="71"/>
       <c r="L47" s="75"/>
-      <c r="M47" s="202"/>
-      <c r="N47" s="201"/>
+      <c r="M47" s="201"/>
+      <c r="N47" s="200"/>
       <c r="P47" s="83"/>
       <c r="Q47" s="9"/>
     </row>
@@ -8981,17 +9019,17 @@
       <c r="A48" s="20"/>
       <c r="B48" s="21"/>
       <c r="C48" s="84"/>
-      <c r="D48" s="197"/>
-      <c r="E48" s="198"/>
-      <c r="F48" s="199"/>
+      <c r="D48" s="196"/>
+      <c r="E48" s="197"/>
+      <c r="F48" s="198"/>
       <c r="G48" s="26"/>
-      <c r="H48" s="200"/>
+      <c r="H48" s="199"/>
       <c r="I48" s="85"/>
       <c r="J48" s="67"/>
       <c r="K48" s="71"/>
       <c r="L48" s="75"/>
-      <c r="M48" s="202"/>
-      <c r="N48" s="201"/>
+      <c r="M48" s="201"/>
+      <c r="N48" s="200"/>
       <c r="P48" s="83"/>
       <c r="Q48" s="9"/>
     </row>
@@ -9006,7 +9044,7 @@
       <c r="F49" s="84"/>
       <c r="H49" s="91"/>
       <c r="I49" s="85"/>
-      <c r="J49" s="203"/>
+      <c r="J49" s="202"/>
       <c r="K49" s="86"/>
       <c r="L49" s="9"/>
       <c r="M49" s="87"/>
@@ -9020,7 +9058,7 @@
       </c>
       <c r="C50" s="93">
         <f>SUM(C5:C49)</f>
-        <v>39013</v>
+        <v>47651.5</v>
       </c>
       <c r="D50" s="94"/>
       <c r="E50" s="95" t="s">
@@ -9028,7 +9066,7 @@
       </c>
       <c r="F50" s="96">
         <f>SUM(F5:F49)</f>
-        <v>1107121</v>
+        <v>1469435</v>
       </c>
       <c r="G50" s="94"/>
       <c r="H50" s="97" t="s">
@@ -9036,7 +9074,7 @@
       </c>
       <c r="I50" s="98">
         <f>SUM(I5:I49)</f>
-        <v>6379</v>
+        <v>10539</v>
       </c>
       <c r="J50" s="99"/>
       <c r="K50" s="100" t="s">
@@ -9062,32 +9100,32 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="237" t="s">
+      <c r="H52" s="219" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="238"/>
+      <c r="I52" s="220"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="239">
+      <c r="K52" s="221">
         <f>I50+L50</f>
-        <v>43336.15</v>
-      </c>
-      <c r="L52" s="240"/>
-      <c r="M52" s="228">
+        <v>47496.15</v>
+      </c>
+      <c r="L52" s="222"/>
+      <c r="M52" s="210">
         <f>N39+M39</f>
-        <v>1024788</v>
-      </c>
-      <c r="N52" s="229"/>
+        <v>1374461</v>
+      </c>
+      <c r="N52" s="211"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="241" t="s">
+      <c r="D53" s="223" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="241"/>
+      <c r="E53" s="223"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
-        <v>1024771.8500000001</v>
+        <v>1374287.35</v>
       </c>
       <c r="I53" s="108"/>
       <c r="J53" s="109"/>
@@ -9095,22 +9133,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="242" t="s">
+      <c r="D54" s="224" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="242"/>
+      <c r="E54" s="224"/>
       <c r="F54" s="102">
         <v>0</v>
       </c>
-      <c r="I54" s="243" t="s">
+      <c r="I54" s="225" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="244"/>
-      <c r="K54" s="245">
+      <c r="J54" s="226"/>
+      <c r="K54" s="227">
         <f>F56+F57+F58</f>
-        <v>1024771.8500000001</v>
-      </c>
-      <c r="L54" s="246"/>
+        <v>1374287.35</v>
+      </c>
+      <c r="L54" s="228"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -9134,17 +9172,17 @@
       </c>
       <c r="F56" s="102">
         <f>SUM(F53:F55)</f>
-        <v>1024771.8500000001</v>
+        <v>1374287.35</v>
       </c>
       <c r="H56" s="20"/>
       <c r="I56" s="116" t="s">
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="230">
-        <v>0</v>
-      </c>
-      <c r="L56" s="231"/>
+      <c r="K56" s="212">
+        <v>0</v>
+      </c>
+      <c r="L56" s="213"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -9159,22 +9197,22 @@
     </row>
     <row r="58" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C58" s="120"/>
-      <c r="D58" s="232" t="s">
+      <c r="D58" s="214" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="233"/>
+      <c r="E58" s="215"/>
       <c r="F58" s="121">
         <v>0</v>
       </c>
-      <c r="I58" s="234" t="s">
+      <c r="I58" s="216" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="235"/>
-      <c r="K58" s="236">
+      <c r="J58" s="217"/>
+      <c r="K58" s="218">
         <f>K54+K56</f>
-        <v>1024771.8500000001</v>
-      </c>
-      <c r="L58" s="236"/>
+        <v>1374287.35</v>
+      </c>
+      <c r="L58" s="218"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -9184,20 +9222,20 @@
       <c r="J59" s="126"/>
     </row>
     <row r="60" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I60" s="195"/>
-      <c r="J60" s="195"/>
-      <c r="K60" s="196"/>
-      <c r="L60" s="196"/>
+      <c r="I60" s="194"/>
+      <c r="J60" s="194"/>
+      <c r="K60" s="195"/>
+      <c r="L60" s="195"/>
     </row>
     <row r="61" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="127"/>
       <c r="C61" s="128"/>
       <c r="D61" s="129"/>
       <c r="E61" s="83"/>
-      <c r="I61" s="195"/>
-      <c r="J61" s="195"/>
-      <c r="K61" s="196"/>
-      <c r="L61" s="196"/>
+      <c r="I61" s="194"/>
+      <c r="J61" s="194"/>
+      <c r="K61" s="195"/>
+      <c r="L61" s="195"/>
       <c r="M61" s="1"/>
       <c r="N61" s="104"/>
     </row>
@@ -9318,6 +9356,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -9332,12 +9376,6 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -9380,19 +9418,19 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="204" t="s">
+      <c r="A2" s="203" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="204" t="s">
+      <c r="B2" s="203" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="205" t="s">
+      <c r="C2" s="204" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="204" t="s">
+      <c r="D2" s="203" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="205" t="s">
+      <c r="E2" s="204" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="140" t="s">
@@ -9403,13 +9441,13 @@
       <c r="A3" s="141">
         <v>44445</v>
       </c>
-      <c r="B3" s="182" t="s">
+      <c r="B3" s="181" t="s">
         <v>123</v>
       </c>
       <c r="C3" s="79">
         <v>42896.2</v>
       </c>
-      <c r="D3" s="206"/>
+      <c r="D3" s="205"/>
       <c r="E3" s="79"/>
       <c r="F3" s="143">
         <f>C3-E3</f>
@@ -9420,13 +9458,13 @@
       <c r="A4" s="141">
         <v>44446</v>
       </c>
-      <c r="B4" s="182" t="s">
+      <c r="B4" s="181" t="s">
         <v>124</v>
       </c>
       <c r="C4" s="79">
         <v>673.2</v>
       </c>
-      <c r="D4" s="206"/>
+      <c r="D4" s="205"/>
       <c r="E4" s="79"/>
       <c r="F4" s="145">
         <f>F3+C4-E4</f>
@@ -9438,13 +9476,13 @@
       <c r="A5" s="141">
         <v>44447</v>
       </c>
-      <c r="B5" s="182" t="s">
+      <c r="B5" s="181" t="s">
         <v>125</v>
       </c>
       <c r="C5" s="79">
         <v>59000.22</v>
       </c>
-      <c r="D5" s="206"/>
+      <c r="D5" s="205"/>
       <c r="E5" s="79"/>
       <c r="F5" s="145">
         <f t="shared" ref="F5:F68" si="0">F4+C5-E5</f>
@@ -9455,13 +9493,13 @@
       <c r="A6" s="141">
         <v>44447</v>
       </c>
-      <c r="B6" s="182" t="s">
+      <c r="B6" s="181" t="s">
         <v>126</v>
       </c>
       <c r="C6" s="79">
         <v>11075.4</v>
       </c>
-      <c r="D6" s="206"/>
+      <c r="D6" s="205"/>
       <c r="E6" s="79"/>
       <c r="F6" s="145">
         <f t="shared" si="0"/>
@@ -9472,13 +9510,13 @@
       <c r="A7" s="141">
         <v>44448</v>
       </c>
-      <c r="B7" s="182" t="s">
+      <c r="B7" s="181" t="s">
         <v>127</v>
       </c>
       <c r="C7" s="79">
         <v>8608.6</v>
       </c>
-      <c r="D7" s="206"/>
+      <c r="D7" s="205"/>
       <c r="E7" s="79"/>
       <c r="F7" s="145">
         <f t="shared" si="0"/>
@@ -9489,13 +9527,13 @@
       <c r="A8" s="141">
         <v>44448</v>
       </c>
-      <c r="B8" s="182" t="s">
+      <c r="B8" s="181" t="s">
         <v>128</v>
       </c>
       <c r="C8" s="79">
         <v>45033.9</v>
       </c>
-      <c r="D8" s="206"/>
+      <c r="D8" s="205"/>
       <c r="E8" s="79"/>
       <c r="F8" s="145">
         <f t="shared" si="0"/>
@@ -9506,13 +9544,13 @@
       <c r="A9" s="141">
         <v>44448</v>
       </c>
-      <c r="B9" s="182" t="s">
+      <c r="B9" s="181" t="s">
         <v>129</v>
       </c>
       <c r="C9" s="79">
         <v>2191.8000000000002</v>
       </c>
-      <c r="D9" s="206"/>
+      <c r="D9" s="205"/>
       <c r="E9" s="79"/>
       <c r="F9" s="145">
         <f t="shared" si="0"/>
@@ -9523,13 +9561,13 @@
       <c r="A10" s="141">
         <v>44449</v>
       </c>
-      <c r="B10" s="182" t="s">
+      <c r="B10" s="181" t="s">
         <v>130</v>
       </c>
       <c r="C10" s="79">
         <v>6894.34</v>
       </c>
-      <c r="D10" s="206"/>
+      <c r="D10" s="205"/>
       <c r="E10" s="79"/>
       <c r="F10" s="145">
         <f t="shared" si="0"/>
@@ -9832,13 +9870,13 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="190">
+      <c r="A28" s="189">
         <v>44459</v>
       </c>
-      <c r="B28" s="188">
+      <c r="B28" s="187">
         <v>44459</v>
       </c>
-      <c r="C28" s="189">
+      <c r="C28" s="188">
         <v>31885.45</v>
       </c>
       <c r="D28" s="144">
@@ -10228,9 +10266,9 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="191"/>
-      <c r="B63" s="188"/>
-      <c r="C63" s="189"/>
+      <c r="A63" s="190"/>
+      <c r="B63" s="187"/>
+      <c r="C63" s="188"/>
       <c r="D63" s="144"/>
       <c r="E63" s="79"/>
       <c r="F63" s="145">
@@ -10239,9 +10277,9 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="191"/>
-      <c r="B64" s="188"/>
-      <c r="C64" s="189"/>
+      <c r="A64" s="190"/>
+      <c r="B64" s="187"/>
+      <c r="C64" s="188"/>
       <c r="D64" s="144"/>
       <c r="E64" s="79"/>
       <c r="F64" s="145">
@@ -10250,9 +10288,9 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="191"/>
-      <c r="B65" s="188"/>
-      <c r="C65" s="189"/>
+      <c r="A65" s="190"/>
+      <c r="B65" s="187"/>
+      <c r="C65" s="188"/>
       <c r="D65" s="144"/>
       <c r="E65" s="79"/>
       <c r="F65" s="145">
@@ -10261,9 +10299,9 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="191"/>
-      <c r="B66" s="188"/>
-      <c r="C66" s="189"/>
+      <c r="A66" s="190"/>
+      <c r="B66" s="187"/>
+      <c r="C66" s="188"/>
       <c r="D66" s="144"/>
       <c r="E66" s="79"/>
       <c r="F66" s="145">
@@ -10272,9 +10310,9 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="191"/>
-      <c r="B67" s="188"/>
-      <c r="C67" s="189"/>
+      <c r="A67" s="190"/>
+      <c r="B67" s="187"/>
+      <c r="C67" s="188"/>
       <c r="D67" s="144"/>
       <c r="E67" s="79"/>
       <c r="F67" s="145">
@@ -10283,9 +10321,9 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="191"/>
-      <c r="B68" s="188"/>
-      <c r="C68" s="189"/>
+      <c r="A68" s="190"/>
+      <c r="B68" s="187"/>
+      <c r="C68" s="188"/>
       <c r="D68" s="144"/>
       <c r="E68" s="79"/>
       <c r="F68" s="145">
@@ -10294,9 +10332,9 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="191"/>
-      <c r="B69" s="188"/>
-      <c r="C69" s="189"/>
+      <c r="A69" s="190"/>
+      <c r="B69" s="187"/>
+      <c r="C69" s="188"/>
       <c r="D69" s="144"/>
       <c r="E69" s="79"/>
       <c r="F69" s="145">
@@ -10305,9 +10343,9 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="191"/>
-      <c r="B70" s="188"/>
-      <c r="C70" s="189"/>
+      <c r="A70" s="190"/>
+      <c r="B70" s="187"/>
+      <c r="C70" s="188"/>
       <c r="D70" s="144"/>
       <c r="E70" s="79"/>
       <c r="F70" s="145">
@@ -10316,9 +10354,9 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="191"/>
-      <c r="B71" s="188"/>
-      <c r="C71" s="189"/>
+      <c r="A71" s="190"/>
+      <c r="B71" s="187"/>
+      <c r="C71" s="188"/>
       <c r="D71" s="144"/>
       <c r="E71" s="79"/>
       <c r="F71" s="145">
@@ -10327,9 +10365,9 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="191"/>
-      <c r="B72" s="188"/>
-      <c r="C72" s="189"/>
+      <c r="A72" s="190"/>
+      <c r="B72" s="187"/>
+      <c r="C72" s="188"/>
       <c r="D72" s="144"/>
       <c r="E72" s="79"/>
       <c r="F72" s="145">
@@ -10338,9 +10376,9 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="191"/>
-      <c r="B73" s="188"/>
-      <c r="C73" s="189"/>
+      <c r="A73" s="190"/>
+      <c r="B73" s="187"/>
+      <c r="C73" s="188"/>
       <c r="D73" s="144"/>
       <c r="E73" s="79"/>
       <c r="F73" s="145">
@@ -10349,9 +10387,9 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="191"/>
-      <c r="B74" s="188"/>
-      <c r="C74" s="189"/>
+      <c r="A74" s="190"/>
+      <c r="B74" s="187"/>
+      <c r="C74" s="188"/>
       <c r="D74" s="144"/>
       <c r="E74" s="79"/>
       <c r="F74" s="145">
@@ -10360,9 +10398,9 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="191"/>
-      <c r="B75" s="188"/>
-      <c r="C75" s="189"/>
+      <c r="A75" s="190"/>
+      <c r="B75" s="187"/>
+      <c r="C75" s="188"/>
       <c r="D75" s="144"/>
       <c r="E75" s="79"/>
       <c r="F75" s="145">
@@ -10371,9 +10409,9 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="191"/>
-      <c r="B76" s="188"/>
-      <c r="C76" s="189"/>
+      <c r="A76" s="190"/>
+      <c r="B76" s="187"/>
+      <c r="C76" s="188"/>
       <c r="D76" s="144"/>
       <c r="E76" s="79"/>
       <c r="F76" s="145">
@@ -10382,9 +10420,9 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="191"/>
-      <c r="B77" s="188"/>
-      <c r="C77" s="189"/>
+      <c r="A77" s="190"/>
+      <c r="B77" s="187"/>
+      <c r="C77" s="188"/>
       <c r="D77" s="144"/>
       <c r="E77" s="79"/>
       <c r="F77" s="145">
@@ -10393,9 +10431,9 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="191"/>
-      <c r="B78" s="188"/>
-      <c r="C78" s="189"/>
+      <c r="A78" s="190"/>
+      <c r="B78" s="187"/>
+      <c r="C78" s="188"/>
       <c r="D78" s="144"/>
       <c r="E78" s="79"/>
       <c r="F78" s="145">
@@ -10404,9 +10442,9 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="191"/>
-      <c r="B79" s="188"/>
-      <c r="C79" s="189"/>
+      <c r="A79" s="190"/>
+      <c r="B79" s="187"/>
+      <c r="C79" s="188"/>
       <c r="D79" s="144"/>
       <c r="E79" s="79"/>
       <c r="F79" s="145">
@@ -10415,9 +10453,9 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="191"/>
-      <c r="B80" s="188"/>
-      <c r="C80" s="189"/>
+      <c r="A80" s="190"/>
+      <c r="B80" s="187"/>
+      <c r="C80" s="188"/>
       <c r="D80" s="144"/>
       <c r="E80" s="79"/>
       <c r="F80" s="145">
@@ -10426,9 +10464,9 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="192"/>
-      <c r="B81" s="193"/>
-      <c r="C81" s="194"/>
+      <c r="A81" s="191"/>
+      <c r="B81" s="192"/>
+      <c r="C81" s="193"/>
       <c r="D81" s="147"/>
       <c r="E81" s="83"/>
       <c r="F81" s="145">
@@ -10437,9 +10475,9 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="192"/>
-      <c r="B82" s="193"/>
-      <c r="C82" s="194"/>
+      <c r="A82" s="191"/>
+      <c r="B82" s="192"/>
+      <c r="C82" s="193"/>
       <c r="D82" s="147"/>
       <c r="E82" s="83"/>
       <c r="F82" s="145">
@@ -10448,9 +10486,9 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="192"/>
-      <c r="B83" s="193"/>
-      <c r="C83" s="194"/>
+      <c r="A83" s="191"/>
+      <c r="B83" s="192"/>
+      <c r="C83" s="193"/>
       <c r="D83" s="147"/>
       <c r="E83" s="83"/>
       <c r="F83" s="145">
@@ -10459,9 +10497,9 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="192"/>
-      <c r="B84" s="193"/>
-      <c r="C84" s="194"/>
+      <c r="A84" s="191"/>
+      <c r="B84" s="192"/>
+      <c r="C84" s="193"/>
       <c r="D84" s="147"/>
       <c r="E84" s="83"/>
       <c r="F84" s="145">
@@ -10470,9 +10508,9 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="192"/>
-      <c r="B85" s="193"/>
-      <c r="C85" s="194"/>
+      <c r="A85" s="191"/>
+      <c r="B85" s="192"/>
+      <c r="C85" s="193"/>
       <c r="D85" s="147"/>
       <c r="E85" s="83"/>
       <c r="F85" s="145">
@@ -10481,9 +10519,9 @@
       </c>
     </row>
     <row r="86" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="192"/>
-      <c r="B86" s="193"/>
-      <c r="C86" s="194"/>
+      <c r="A86" s="191"/>
+      <c r="B86" s="192"/>
+      <c r="C86" s="193"/>
       <c r="D86" s="147"/>
       <c r="E86" s="83"/>
       <c r="F86" s="145">
@@ -10492,9 +10530,9 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="191"/>
-      <c r="B87" s="188"/>
-      <c r="C87" s="189"/>
+      <c r="A87" s="190"/>
+      <c r="B87" s="187"/>
+      <c r="C87" s="188"/>
       <c r="D87" s="148"/>
       <c r="E87" s="79"/>
       <c r="F87" s="145">
@@ -10503,9 +10541,9 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="191"/>
-      <c r="B88" s="188"/>
-      <c r="C88" s="189"/>
+      <c r="A88" s="190"/>
+      <c r="B88" s="187"/>
+      <c r="C88" s="188"/>
       <c r="D88" s="148"/>
       <c r="E88" s="79"/>
       <c r="F88" s="145">
@@ -10514,9 +10552,9 @@
       </c>
     </row>
     <row r="89" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="191"/>
-      <c r="B89" s="188"/>
-      <c r="C89" s="189"/>
+      <c r="A89" s="190"/>
+      <c r="B89" s="187"/>
+      <c r="C89" s="188"/>
       <c r="D89" s="148"/>
       <c r="E89" s="79"/>
       <c r="F89" s="145">
@@ -10525,9 +10563,9 @@
       </c>
     </row>
     <row r="90" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="191"/>
-      <c r="B90" s="188"/>
-      <c r="C90" s="189"/>
+      <c r="A90" s="190"/>
+      <c r="B90" s="187"/>
+      <c r="C90" s="188"/>
       <c r="D90" s="148"/>
       <c r="E90" s="79"/>
       <c r="F90" s="145">
@@ -10536,9 +10574,9 @@
       </c>
     </row>
     <row r="91" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="191"/>
-      <c r="B91" s="188"/>
-      <c r="C91" s="189"/>
+      <c r="A91" s="190"/>
+      <c r="B91" s="187"/>
+      <c r="C91" s="188"/>
       <c r="D91" s="148"/>
       <c r="E91" s="79"/>
       <c r="F91" s="145">
@@ -10547,9 +10585,9 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="191"/>
-      <c r="B92" s="188"/>
-      <c r="C92" s="189"/>
+      <c r="A92" s="190"/>
+      <c r="B92" s="187"/>
+      <c r="C92" s="188"/>
       <c r="D92" s="148"/>
       <c r="E92" s="79"/>
       <c r="F92" s="145">
@@ -10558,9 +10596,9 @@
       </c>
     </row>
     <row r="93" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="191"/>
-      <c r="B93" s="188"/>
-      <c r="C93" s="189"/>
+      <c r="A93" s="190"/>
+      <c r="B93" s="187"/>
+      <c r="C93" s="188"/>
       <c r="D93" s="148"/>
       <c r="E93" s="79"/>
       <c r="F93" s="145">
@@ -10569,9 +10607,9 @@
       </c>
     </row>
     <row r="94" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="191"/>
-      <c r="B94" s="188"/>
-      <c r="C94" s="189"/>
+      <c r="A94" s="190"/>
+      <c r="B94" s="187"/>
+      <c r="C94" s="188"/>
       <c r="D94" s="148"/>
       <c r="E94" s="79"/>
       <c r="F94" s="145">
@@ -10580,9 +10618,9 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="191"/>
-      <c r="B95" s="188"/>
-      <c r="C95" s="189"/>
+      <c r="A95" s="190"/>
+      <c r="B95" s="187"/>
+      <c r="C95" s="188"/>
       <c r="D95" s="148"/>
       <c r="E95" s="79"/>
       <c r="F95" s="145">
@@ -10591,9 +10629,9 @@
       </c>
     </row>
     <row r="96" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="191"/>
-      <c r="B96" s="188"/>
-      <c r="C96" s="189"/>
+      <c r="A96" s="190"/>
+      <c r="B96" s="187"/>
+      <c r="C96" s="188"/>
       <c r="D96" s="148"/>
       <c r="E96" s="79"/>
       <c r="F96" s="145">
@@ -10846,8 +10884,8 @@
   </sheetPr>
   <dimension ref="A23:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10869,55 +10907,57 @@
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="163"/>
-      <c r="B45" s="250" t="s">
+      <c r="B45" s="249" t="s">
         <v>31</v>
       </c>
-      <c r="C45" s="251"/>
-      <c r="D45" s="251"/>
-      <c r="E45" s="252"/>
+      <c r="C45" s="250"/>
+      <c r="D45" s="250"/>
+      <c r="E45" s="251"/>
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="170">
-        <v>44461</v>
+        <v>44470</v>
       </c>
       <c r="B46" s="171" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="C46" s="172">
-        <v>132.30000000000001</v>
+        <v>425.64</v>
       </c>
       <c r="D46" s="173" t="s">
         <v>32</v>
       </c>
       <c r="E46" s="174" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="F46" s="107">
-        <v>96</v>
+        <v>383</v>
       </c>
       <c r="G46" s="253"/>
     </row>
     <row r="47" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="170"/>
+      <c r="A47" s="170">
+        <v>44470</v>
+      </c>
       <c r="B47" s="171" t="s">
-        <v>48</v>
+        <v>164</v>
       </c>
       <c r="C47" s="172">
-        <v>0</v>
+        <v>9825.6</v>
       </c>
       <c r="D47" s="175" t="s">
         <v>32</v>
       </c>
       <c r="E47" s="174" t="s">
-        <v>33</v>
+        <v>165</v>
       </c>
       <c r="F47" s="107">
-        <v>0</v>
-      </c>
-      <c r="G47" s="254"/>
-    </row>
-    <row r="48" spans="1:7" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5126</v>
+      </c>
+      <c r="G47" s="252"/>
+    </row>
+    <row r="48" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="170"/>
       <c r="B48" s="171" t="s">
         <v>33</v>
@@ -10928,14 +10968,14 @@
       <c r="D48" s="175" t="s">
         <v>32</v>
       </c>
-      <c r="E48" s="179" t="s">
-        <v>33</v>
+      <c r="E48" s="174" t="s">
+        <v>48</v>
       </c>
       <c r="F48" s="107">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="170"/>
       <c r="B49" s="171" t="s">
         <v>33</v>
@@ -10946,8 +10986,8 @@
       <c r="D49" s="175" t="s">
         <v>32</v>
       </c>
-      <c r="E49" s="179" t="s">
-        <v>33</v>
+      <c r="E49" s="174" t="s">
+        <v>48</v>
       </c>
       <c r="F49" s="107">
         <v>0</v>
@@ -10964,8 +11004,8 @@
       <c r="D50" s="167" t="s">
         <v>32</v>
       </c>
-      <c r="E50" s="179" t="s">
-        <v>33</v>
+      <c r="E50" s="174" t="s">
+        <v>48</v>
       </c>
       <c r="F50" s="107">
         <v>0</v>
@@ -10982,8 +11022,8 @@
       <c r="D51" s="167" t="s">
         <v>32</v>
       </c>
-      <c r="E51" s="179" t="s">
-        <v>33</v>
+      <c r="E51" s="174" t="s">
+        <v>48</v>
       </c>
       <c r="F51" s="107">
         <v>0</v>
@@ -11000,8 +11040,8 @@
       <c r="D52" s="167" t="s">
         <v>32</v>
       </c>
-      <c r="E52" s="179" t="s">
-        <v>33</v>
+      <c r="E52" s="174" t="s">
+        <v>48</v>
       </c>
       <c r="F52" s="107">
         <v>0</v>
@@ -11018,17 +11058,16 @@
       <c r="D53" s="169" t="s">
         <v>32</v>
       </c>
-      <c r="E53" s="179" t="s">
-        <v>33</v>
+      <c r="E53" s="174" t="s">
+        <v>48</v>
       </c>
       <c r="F53" s="107">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="B45:E45"/>
-    <mergeCell ref="G46:G47"/>
   </mergeCells>
   <pageMargins left="0.39" right="0.13" top="0.75" bottom="0.27" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
CIERRRE 8 OCT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE  HERRADURA  SEPTIEMBRE   2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 09  SEPTIEMBRE 2021/BALANCE  HERRADURA  SEPTIEMBRE   2021.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17190" windowHeight="10725" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="A G O S T O    2 0 2 1     " sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="187">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -643,6 +643,69 @@
   </si>
   <si>
     <t>NOMINA # 40</t>
+  </si>
+  <si>
+    <t>20629 B</t>
+  </si>
+  <si>
+    <t>20728 B</t>
+  </si>
+  <si>
+    <t>20764 B</t>
+  </si>
+  <si>
+    <t>20875 B</t>
+  </si>
+  <si>
+    <t>21070 B</t>
+  </si>
+  <si>
+    <t>21071 B</t>
+  </si>
+  <si>
+    <t>21130 B</t>
+  </si>
+  <si>
+    <t>21206 B</t>
+  </si>
+  <si>
+    <t>21336 B</t>
+  </si>
+  <si>
+    <t>21390 B</t>
+  </si>
+  <si>
+    <t>21463 B</t>
+  </si>
+  <si>
+    <t>21474 B</t>
+  </si>
+  <si>
+    <t>21559 B</t>
+  </si>
+  <si>
+    <t>21666 B</t>
+  </si>
+  <si>
+    <t>21845 B</t>
+  </si>
+  <si>
+    <t>21945 B</t>
+  </si>
+  <si>
+    <t>21974 B</t>
+  </si>
+  <si>
+    <t>SEPT-,21</t>
+  </si>
+  <si>
+    <t>BATAS</t>
+  </si>
+  <si>
+    <t>XXXXX</t>
+  </si>
+  <si>
+    <t>ADT</t>
   </si>
 </sst>
 </file>
@@ -1796,7 +1859,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="256">
+  <cellXfs count="258">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
@@ -2197,6 +2260,71 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="44" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="44" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="3" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="3" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2248,63 +2376,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="48" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="3" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="3" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="41" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -2323,8 +2394,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="44" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="44" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -3494,23 +3563,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="218"/>
-      <c r="C1" s="227" t="s">
+      <c r="B1" s="241"/>
+      <c r="C1" s="250" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="228"/>
-      <c r="E1" s="228"/>
-      <c r="F1" s="228"/>
-      <c r="G1" s="228"/>
-      <c r="H1" s="228"/>
-      <c r="I1" s="228"/>
-      <c r="J1" s="228"/>
-      <c r="K1" s="228"/>
-      <c r="L1" s="228"/>
-      <c r="M1" s="228"/>
+      <c r="D1" s="251"/>
+      <c r="E1" s="251"/>
+      <c r="F1" s="251"/>
+      <c r="G1" s="251"/>
+      <c r="H1" s="251"/>
+      <c r="I1" s="251"/>
+      <c r="J1" s="251"/>
+      <c r="K1" s="251"/>
+      <c r="L1" s="251"/>
+      <c r="M1" s="251"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="219"/>
+      <c r="B2" s="242"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -3520,17 +3589,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="220" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="221"/>
+      <c r="B3" s="243" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="244"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="222" t="s">
+      <c r="H3" s="245" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="222"/>
+      <c r="I3" s="245"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -3546,14 +3615,14 @@
       <c r="D4" s="16">
         <v>44410</v>
       </c>
-      <c r="E4" s="223" t="s">
+      <c r="E4" s="246" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="224"/>
-      <c r="H4" s="225" t="s">
+      <c r="F4" s="247"/>
+      <c r="H4" s="248" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="226"/>
+      <c r="I4" s="249"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -3563,10 +3632,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="212" t="s">
+      <c r="P4" s="235" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="213"/>
+      <c r="Q4" s="236"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -5061,11 +5130,11 @@
       <c r="L39" s="69">
         <v>454.62</v>
       </c>
-      <c r="M39" s="214">
+      <c r="M39" s="237">
         <f>SUM(M5:M38)</f>
         <v>1393675.5</v>
       </c>
-      <c r="N39" s="216">
+      <c r="N39" s="239">
         <f>SUM(N5:N38)</f>
         <v>28399.97</v>
       </c>
@@ -5097,8 +5166,8 @@
       <c r="L40" s="69">
         <v>1195.67</v>
       </c>
-      <c r="M40" s="215"/>
-      <c r="N40" s="217"/>
+      <c r="M40" s="238"/>
+      <c r="N40" s="240"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -5331,29 +5400,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="238" t="s">
+      <c r="H52" s="225" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="239"/>
+      <c r="I52" s="226"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="240">
+      <c r="K52" s="227">
         <f>I50+L50</f>
         <v>80916.84</v>
       </c>
-      <c r="L52" s="241"/>
-      <c r="M52" s="229">
+      <c r="L52" s="228"/>
+      <c r="M52" s="216">
         <f>N39+M39</f>
         <v>1422075.47</v>
       </c>
-      <c r="N52" s="230"/>
+      <c r="N52" s="217"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="242" t="s">
+      <c r="D53" s="229" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="242"/>
+      <c r="E53" s="229"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1396181.44</v>
@@ -5364,22 +5433,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="243" t="s">
+      <c r="D54" s="230" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="243"/>
+      <c r="E54" s="230"/>
       <c r="F54" s="102">
         <v>-1523111</v>
       </c>
-      <c r="I54" s="244" t="s">
+      <c r="I54" s="231" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="245"/>
-      <c r="K54" s="246">
+      <c r="J54" s="232"/>
+      <c r="K54" s="233">
         <f>F56+F57+F58</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L54" s="247"/>
+      <c r="L54" s="234"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -5410,10 +5479,10 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="231">
-        <v>0</v>
-      </c>
-      <c r="L56" s="232"/>
+      <c r="K56" s="218">
+        <v>0</v>
+      </c>
+      <c r="L56" s="219"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -5430,22 +5499,22 @@
       <c r="C58" s="120">
         <v>44444</v>
       </c>
-      <c r="D58" s="233" t="s">
+      <c r="D58" s="220" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="234"/>
+      <c r="E58" s="221"/>
       <c r="F58" s="121">
         <v>136234.76999999999</v>
       </c>
-      <c r="I58" s="235" t="s">
+      <c r="I58" s="222" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="236"/>
-      <c r="K58" s="237">
+      <c r="J58" s="223"/>
+      <c r="K58" s="224">
         <f>K54+K56</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L58" s="237"/>
+      <c r="L58" s="224"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -5589,6 +5658,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C1:M1"/>
     <mergeCell ref="M52:N52"/>
     <mergeCell ref="K56:L56"/>
     <mergeCell ref="D58:E58"/>
@@ -5600,15 +5678,6 @@
     <mergeCell ref="D54:E54"/>
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="C1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5680,7 +5749,7 @@
       <c r="C3" s="35">
         <v>3015.96</v>
       </c>
-      <c r="D3" s="248" t="s">
+      <c r="D3" s="252" t="s">
         <v>49</v>
       </c>
       <c r="E3" s="9"/>
@@ -5699,7 +5768,7 @@
       <c r="C4" s="35">
         <v>10281</v>
       </c>
-      <c r="D4" s="249"/>
+      <c r="D4" s="253"/>
       <c r="E4" s="181"/>
       <c r="F4" s="145">
         <f>F3+C4-E4</f>
@@ -5717,7 +5786,7 @@
       <c r="C5" s="35">
         <v>12746.2</v>
       </c>
-      <c r="D5" s="249"/>
+      <c r="D5" s="253"/>
       <c r="E5" s="181"/>
       <c r="F5" s="145">
         <f t="shared" ref="F5:F68" si="0">F4+C5-E5</f>
@@ -5734,7 +5803,7 @@
       <c r="C6" s="35">
         <v>28974.78</v>
       </c>
-      <c r="D6" s="249"/>
+      <c r="D6" s="253"/>
       <c r="E6" s="181"/>
       <c r="F6" s="145">
         <f t="shared" si="0"/>
@@ -5751,7 +5820,7 @@
       <c r="C7" s="35">
         <v>44758.6</v>
       </c>
-      <c r="D7" s="249"/>
+      <c r="D7" s="253"/>
       <c r="E7" s="181"/>
       <c r="F7" s="145">
         <f t="shared" si="0"/>
@@ -5768,7 +5837,7 @@
       <c r="C8" s="35">
         <v>12841.78</v>
       </c>
-      <c r="D8" s="249"/>
+      <c r="D8" s="253"/>
       <c r="E8" s="181"/>
       <c r="F8" s="145">
         <f t="shared" si="0"/>
@@ -5785,7 +5854,7 @@
       <c r="C9" s="35">
         <v>3898.05</v>
       </c>
-      <c r="D9" s="249"/>
+      <c r="D9" s="253"/>
       <c r="E9" s="181"/>
       <c r="F9" s="145">
         <f t="shared" si="0"/>
@@ -5802,7 +5871,7 @@
       <c r="C10" s="35">
         <v>1429</v>
       </c>
-      <c r="D10" s="250"/>
+      <c r="D10" s="254"/>
       <c r="E10" s="181"/>
       <c r="F10" s="145">
         <f t="shared" si="0"/>
@@ -7299,8 +7368,8 @@
   </sheetPr>
   <dimension ref="A1:S80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G22" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7322,23 +7391,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="218"/>
-      <c r="C1" s="227" t="s">
+      <c r="B1" s="241"/>
+      <c r="C1" s="250" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="228"/>
-      <c r="E1" s="228"/>
-      <c r="F1" s="228"/>
-      <c r="G1" s="228"/>
-      <c r="H1" s="228"/>
-      <c r="I1" s="228"/>
-      <c r="J1" s="228"/>
-      <c r="K1" s="228"/>
-      <c r="L1" s="228"/>
-      <c r="M1" s="228"/>
+      <c r="D1" s="251"/>
+      <c r="E1" s="251"/>
+      <c r="F1" s="251"/>
+      <c r="G1" s="251"/>
+      <c r="H1" s="251"/>
+      <c r="I1" s="251"/>
+      <c r="J1" s="251"/>
+      <c r="K1" s="251"/>
+      <c r="L1" s="251"/>
+      <c r="M1" s="251"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="219"/>
+      <c r="B2" s="242"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -7348,17 +7417,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="220" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="221"/>
+      <c r="B3" s="243" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="244"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="222" t="s">
+      <c r="H3" s="245" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="222"/>
+      <c r="I3" s="245"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -7374,14 +7443,14 @@
       <c r="D4" s="16">
         <v>44444</v>
       </c>
-      <c r="E4" s="223" t="s">
+      <c r="E4" s="246" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="224"/>
-      <c r="H4" s="225" t="s">
+      <c r="F4" s="247"/>
+      <c r="H4" s="248" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="226"/>
+      <c r="I4" s="249"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -7391,10 +7460,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="212" t="s">
+      <c r="P4" s="235" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="213"/>
+      <c r="Q4" s="236"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -7565,7 +7634,7 @@
         <f t="shared" si="0"/>
         <v>50471</v>
       </c>
-      <c r="Q8" s="255">
+      <c r="Q8" s="213">
         <f t="shared" si="1"/>
         <v>-40</v>
       </c>
@@ -8457,7 +8526,7 @@
         <f t="shared" si="0"/>
         <v>35889</v>
       </c>
-      <c r="Q28" s="254">
+      <c r="Q28" s="212">
         <f t="shared" si="1"/>
         <v>-3</v>
       </c>
@@ -8595,7 +8664,7 @@
         <f t="shared" si="0"/>
         <v>87027</v>
       </c>
-      <c r="Q31" s="254">
+      <c r="Q31" s="212">
         <f t="shared" si="1"/>
         <v>-6</v>
       </c>
@@ -8657,9 +8726,15 @@
       <c r="G33" s="26"/>
       <c r="H33" s="32"/>
       <c r="I33" s="28"/>
-      <c r="J33" s="67"/>
-      <c r="K33" s="71"/>
-      <c r="L33" s="75"/>
+      <c r="J33" s="67" t="s">
+        <v>183</v>
+      </c>
+      <c r="K33" s="71" t="s">
+        <v>184</v>
+      </c>
+      <c r="L33" s="75">
+        <v>3422</v>
+      </c>
       <c r="M33" s="138">
         <v>0</v>
       </c>
@@ -8667,7 +8742,6 @@
         <v>0</v>
       </c>
       <c r="P33" s="83">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q33" s="9">
@@ -8692,9 +8766,15 @@
       <c r="I34" s="28">
         <v>0</v>
       </c>
-      <c r="J34" s="67"/>
-      <c r="K34" s="185"/>
-      <c r="L34" s="76"/>
+      <c r="J34" s="67" t="s">
+        <v>183</v>
+      </c>
+      <c r="K34" s="214" t="s">
+        <v>185</v>
+      </c>
+      <c r="L34" s="76">
+        <v>4999.6000000000004</v>
+      </c>
       <c r="M34" s="138">
         <v>0</v>
       </c>
@@ -8702,7 +8782,6 @@
         <v>0</v>
       </c>
       <c r="P34" s="83">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q34" s="9">
@@ -8727,9 +8806,15 @@
       <c r="I35" s="28">
         <v>0</v>
       </c>
-      <c r="J35" s="67"/>
-      <c r="K35" s="71"/>
-      <c r="L35" s="75"/>
+      <c r="J35" s="67" t="s">
+        <v>183</v>
+      </c>
+      <c r="K35" s="215" t="s">
+        <v>185</v>
+      </c>
+      <c r="L35" s="75">
+        <v>1195.68</v>
+      </c>
       <c r="M35" s="138">
         <v>0</v>
       </c>
@@ -8737,7 +8822,6 @@
         <v>0</v>
       </c>
       <c r="P35" s="83">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q35" s="9">
@@ -8762,9 +8846,15 @@
       <c r="I36" s="28">
         <v>0</v>
       </c>
-      <c r="J36" s="67"/>
-      <c r="K36" s="78"/>
-      <c r="L36" s="76"/>
+      <c r="J36" s="67" t="s">
+        <v>183</v>
+      </c>
+      <c r="K36" s="78" t="s">
+        <v>110</v>
+      </c>
+      <c r="L36" s="76">
+        <v>1392</v>
+      </c>
       <c r="M36" s="138">
         <v>0</v>
       </c>
@@ -8772,7 +8862,6 @@
         <v>0</v>
       </c>
       <c r="P36" s="83">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q36" s="9">
@@ -8797,9 +8886,15 @@
       <c r="I37" s="28">
         <v>0</v>
       </c>
-      <c r="J37" s="67"/>
-      <c r="K37" s="185"/>
-      <c r="L37" s="76"/>
+      <c r="J37" s="67" t="s">
+        <v>183</v>
+      </c>
+      <c r="K37" s="185" t="s">
+        <v>186</v>
+      </c>
+      <c r="L37" s="76">
+        <v>836.84</v>
+      </c>
       <c r="M37" s="138">
         <v>0</v>
       </c>
@@ -8860,11 +8955,11 @@
       <c r="J39" s="67"/>
       <c r="K39" s="82"/>
       <c r="L39" s="69"/>
-      <c r="M39" s="214">
+      <c r="M39" s="237">
         <f>SUM(M5:M38)</f>
         <v>1464441</v>
       </c>
-      <c r="N39" s="216">
+      <c r="N39" s="239">
         <f>SUM(N5:N38)</f>
         <v>53494</v>
       </c>
@@ -8890,8 +8985,8 @@
       <c r="J40" s="67"/>
       <c r="K40" s="71"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="215"/>
-      <c r="N40" s="217"/>
+      <c r="M40" s="238"/>
+      <c r="N40" s="240"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -9088,7 +9183,7 @@
       </c>
       <c r="L50" s="101">
         <f>SUM(L5:L49)</f>
-        <v>47257.15</v>
+        <v>59103.27</v>
       </c>
       <c r="M50" s="102"/>
       <c r="N50" s="102"/>
@@ -9106,32 +9201,32 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="238" t="s">
+      <c r="H52" s="225" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="239"/>
+      <c r="I52" s="226"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="240">
+      <c r="K52" s="227">
         <f>I50+L50</f>
-        <v>57796.15</v>
-      </c>
-      <c r="L52" s="241"/>
-      <c r="M52" s="229">
+        <v>69642.26999999999</v>
+      </c>
+      <c r="L52" s="228"/>
+      <c r="M52" s="216">
         <f>N39+M39</f>
         <v>1517935</v>
       </c>
-      <c r="N52" s="230"/>
+      <c r="N52" s="217"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="242" t="s">
+      <c r="D53" s="229" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="242"/>
+      <c r="E53" s="229"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
-        <v>1517767.35</v>
+        <v>1505921.23</v>
       </c>
       <c r="I53" s="108"/>
       <c r="J53" s="109"/>
@@ -9139,22 +9234,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="243" t="s">
+      <c r="D54" s="230" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="243"/>
+      <c r="E54" s="230"/>
       <c r="F54" s="102">
-        <v>0</v>
-      </c>
-      <c r="I54" s="244" t="s">
+        <v>-1424333.95</v>
+      </c>
+      <c r="I54" s="231" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="245"/>
-      <c r="K54" s="246">
+      <c r="J54" s="232"/>
+      <c r="K54" s="233">
         <f>F56+F57+F58</f>
-        <v>1652616.2400000002</v>
-      </c>
-      <c r="L54" s="247"/>
+        <v>222140.17000000004</v>
+      </c>
+      <c r="L54" s="234"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -9178,17 +9273,17 @@
       </c>
       <c r="F56" s="102">
         <f>SUM(F53:F55)</f>
-        <v>1517767.35</v>
+        <v>81587.280000000028</v>
       </c>
       <c r="H56" s="20"/>
       <c r="I56" s="116" t="s">
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="231">
-        <v>0</v>
-      </c>
-      <c r="L56" s="232"/>
+      <c r="K56" s="218">
+        <v>0</v>
+      </c>
+      <c r="L56" s="219"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -9198,29 +9293,29 @@
         <v>15</v>
       </c>
       <c r="F57" s="119">
-        <v>0</v>
+        <v>5704</v>
       </c>
     </row>
     <row r="58" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C58" s="120">
         <v>44472</v>
       </c>
-      <c r="D58" s="233" t="s">
+      <c r="D58" s="220" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="234"/>
+      <c r="E58" s="221"/>
       <c r="F58" s="121">
         <v>134848.89000000001</v>
       </c>
-      <c r="I58" s="235" t="s">
+      <c r="I58" s="222" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="236"/>
-      <c r="K58" s="237">
+      <c r="J58" s="223"/>
+      <c r="K58" s="224">
         <f>K54+K56</f>
-        <v>1652616.2400000002</v>
-      </c>
-      <c r="L58" s="237"/>
+        <v>222140.17000000004</v>
+      </c>
+      <c r="L58" s="224"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -9364,6 +9459,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -9378,12 +9479,6 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -9399,8 +9494,8 @@
   </sheetPr>
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9878,13 +9973,13 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="188">
+      <c r="A28" s="144">
         <v>44459</v>
       </c>
-      <c r="B28" s="186">
-        <v>44459</v>
-      </c>
-      <c r="C28" s="187">
+      <c r="B28" s="142" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" s="79">
         <v>31885.45</v>
       </c>
       <c r="D28" s="144">
@@ -9899,180 +9994,280 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="144"/>
-      <c r="B29" s="142"/>
-      <c r="C29" s="79"/>
+      <c r="A29" s="144">
+        <v>44460</v>
+      </c>
+      <c r="B29" s="142" t="s">
+        <v>167</v>
+      </c>
+      <c r="C29" s="79">
+        <v>36425.199999999997</v>
+      </c>
       <c r="D29" s="144"/>
       <c r="E29" s="79"/>
       <c r="F29" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>60278.670000000086</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="144"/>
-      <c r="B30" s="142"/>
-      <c r="C30" s="79"/>
+      <c r="A30" s="144">
+        <v>44461</v>
+      </c>
+      <c r="B30" s="142" t="s">
+        <v>168</v>
+      </c>
+      <c r="C30" s="79">
+        <v>50568.800000000003</v>
+      </c>
       <c r="D30" s="144"/>
       <c r="E30" s="79"/>
       <c r="F30" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>110847.47000000009</v>
       </c>
       <c r="G30" s="146"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="144"/>
-      <c r="B31" s="142"/>
-      <c r="C31" s="79"/>
+      <c r="A31" s="144">
+        <v>44462</v>
+      </c>
+      <c r="B31" s="142" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" s="79">
+        <v>59040.6</v>
+      </c>
       <c r="D31" s="144"/>
       <c r="E31" s="79"/>
       <c r="F31" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>169888.07000000009</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="144"/>
-      <c r="B32" s="142"/>
-      <c r="C32" s="79"/>
+      <c r="A32" s="144">
+        <v>44463</v>
+      </c>
+      <c r="B32" s="142" t="s">
+        <v>170</v>
+      </c>
+      <c r="C32" s="79">
+        <v>79386.06</v>
+      </c>
       <c r="D32" s="144"/>
       <c r="E32" s="79"/>
       <c r="F32" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>249274.13000000009</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="144"/>
-      <c r="B33" s="142"/>
-      <c r="C33" s="79"/>
+      <c r="A33" s="144">
+        <v>44463</v>
+      </c>
+      <c r="B33" s="142" t="s">
+        <v>171</v>
+      </c>
+      <c r="C33" s="79">
+        <v>975</v>
+      </c>
       <c r="D33" s="144"/>
       <c r="E33" s="79"/>
       <c r="F33" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>250249.13000000009</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="144"/>
-      <c r="B34" s="142"/>
-      <c r="C34" s="79"/>
+      <c r="A34" s="144">
+        <v>44464</v>
+      </c>
+      <c r="B34" s="142" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" s="79">
+        <v>26659.84</v>
+      </c>
       <c r="D34" s="144"/>
       <c r="E34" s="79"/>
       <c r="F34" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>276908.97000000009</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="144"/>
-      <c r="B35" s="142"/>
-      <c r="C35" s="79"/>
+      <c r="A35" s="144">
+        <v>44464</v>
+      </c>
+      <c r="B35" s="142" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" s="79">
+        <v>63162.2</v>
+      </c>
       <c r="D35" s="144"/>
       <c r="E35" s="79"/>
       <c r="F35" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>340071.1700000001</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="144"/>
-      <c r="B36" s="142"/>
-      <c r="C36" s="79"/>
+      <c r="A36" s="144">
+        <v>44466</v>
+      </c>
+      <c r="B36" s="142" t="s">
+        <v>174</v>
+      </c>
+      <c r="C36" s="79">
+        <v>42269.1</v>
+      </c>
       <c r="D36" s="144"/>
       <c r="E36" s="79"/>
       <c r="F36" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>382340.27000000008</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="144"/>
-      <c r="B37" s="142"/>
-      <c r="C37" s="79"/>
+      <c r="A37" s="144">
+        <v>44466</v>
+      </c>
+      <c r="B37" s="142" t="s">
+        <v>175</v>
+      </c>
+      <c r="C37" s="79">
+        <v>3041</v>
+      </c>
       <c r="D37" s="144"/>
       <c r="E37" s="79"/>
       <c r="F37" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>385381.27000000008</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="144"/>
-      <c r="B38" s="142"/>
-      <c r="C38" s="79"/>
-      <c r="D38" s="144"/>
-      <c r="E38" s="79"/>
+      <c r="A38" s="188">
+        <v>44467</v>
+      </c>
+      <c r="B38" s="186" t="s">
+        <v>176</v>
+      </c>
+      <c r="C38" s="187">
+        <v>59570.38</v>
+      </c>
+      <c r="D38" s="144">
+        <v>44470</v>
+      </c>
+      <c r="E38" s="79">
+        <v>400000</v>
+      </c>
       <c r="F38" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>44951.650000000081</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="144"/>
-      <c r="B39" s="142"/>
-      <c r="C39" s="79"/>
+      <c r="A39" s="188">
+        <v>44467</v>
+      </c>
+      <c r="B39" s="186" t="s">
+        <v>177</v>
+      </c>
+      <c r="C39" s="187">
+        <v>7939.6</v>
+      </c>
       <c r="D39" s="144"/>
       <c r="E39" s="79"/>
       <c r="F39" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>52891.25000000008</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="144"/>
-      <c r="B40" s="142"/>
-      <c r="C40" s="79"/>
+      <c r="A40" s="188">
+        <v>44468</v>
+      </c>
+      <c r="B40" s="186" t="s">
+        <v>178</v>
+      </c>
+      <c r="C40" s="187">
+        <v>38874.400000000001</v>
+      </c>
       <c r="D40" s="144"/>
       <c r="E40" s="79"/>
       <c r="F40" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>91765.650000000081</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="144"/>
-      <c r="B41" s="142"/>
-      <c r="C41" s="79"/>
+      <c r="A41" s="188">
+        <v>44469</v>
+      </c>
+      <c r="B41" s="186" t="s">
+        <v>179</v>
+      </c>
+      <c r="C41" s="187">
+        <v>92182.8</v>
+      </c>
       <c r="D41" s="144"/>
       <c r="E41" s="79"/>
       <c r="F41" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>183948.45000000007</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="144"/>
-      <c r="B42" s="142"/>
-      <c r="C42" s="79"/>
+      <c r="A42" s="188">
+        <v>44470</v>
+      </c>
+      <c r="B42" s="186" t="s">
+        <v>180</v>
+      </c>
+      <c r="C42" s="187">
+        <v>66246</v>
+      </c>
       <c r="D42" s="144"/>
       <c r="E42" s="79"/>
       <c r="F42" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>250194.45000000007</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="144"/>
-      <c r="B43" s="142"/>
-      <c r="C43" s="79"/>
+      <c r="A43" s="188">
+        <v>44471</v>
+      </c>
+      <c r="B43" s="186" t="s">
+        <v>181</v>
+      </c>
+      <c r="C43" s="187">
+        <v>85535.7</v>
+      </c>
       <c r="D43" s="144"/>
       <c r="E43" s="79"/>
       <c r="F43" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>335730.15000000008</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="144"/>
-      <c r="B44" s="142"/>
-      <c r="C44" s="79"/>
+      <c r="A44" s="188">
+        <v>44471</v>
+      </c>
+      <c r="B44" s="186" t="s">
+        <v>182</v>
+      </c>
+      <c r="C44" s="187">
+        <v>1725</v>
+      </c>
       <c r="D44" s="144"/>
       <c r="E44" s="79"/>
       <c r="F44" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10083,7 +10278,7 @@
       <c r="E45" s="79"/>
       <c r="F45" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10094,7 +10289,7 @@
       <c r="E46" s="79"/>
       <c r="F46" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10105,7 +10300,7 @@
       <c r="E47" s="79"/>
       <c r="F47" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10116,7 +10311,7 @@
       <c r="E48" s="79"/>
       <c r="F48" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10127,7 +10322,7 @@
       <c r="E49" s="79"/>
       <c r="F49" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10138,7 +10333,7 @@
       <c r="E50" s="79"/>
       <c r="F50" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10149,7 +10344,7 @@
       <c r="E51" s="79"/>
       <c r="F51" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10160,7 +10355,7 @@
       <c r="E52" s="79"/>
       <c r="F52" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10171,7 +10366,7 @@
       <c r="E53" s="79"/>
       <c r="F53" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10182,7 +10377,7 @@
       <c r="E54" s="79"/>
       <c r="F54" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10193,7 +10388,7 @@
       <c r="E55" s="79"/>
       <c r="F55" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10204,7 +10399,7 @@
       <c r="E56" s="79"/>
       <c r="F56" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10215,7 +10410,7 @@
       <c r="E57" s="79"/>
       <c r="F57" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10226,7 +10421,7 @@
       <c r="E58" s="79"/>
       <c r="F58" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10237,7 +10432,7 @@
       <c r="E59" s="79"/>
       <c r="F59" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10248,7 +10443,7 @@
       <c r="E60" s="79"/>
       <c r="F60" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10259,7 +10454,7 @@
       <c r="E61" s="79"/>
       <c r="F61" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -10270,7 +10465,7 @@
       <c r="E62" s="79"/>
       <c r="F62" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -10281,7 +10476,7 @@
       <c r="E63" s="79"/>
       <c r="F63" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10292,7 +10487,7 @@
       <c r="E64" s="79"/>
       <c r="F64" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10303,7 +10498,7 @@
       <c r="E65" s="79"/>
       <c r="F65" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10314,7 +10509,7 @@
       <c r="E66" s="79"/>
       <c r="F66" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10325,7 +10520,7 @@
       <c r="E67" s="79"/>
       <c r="F67" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10336,7 +10531,7 @@
       <c r="E68" s="79"/>
       <c r="F68" s="145">
         <f t="shared" si="0"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10347,7 +10542,7 @@
       <c r="E69" s="79"/>
       <c r="F69" s="145">
         <f t="shared" ref="F69:F97" si="1">F68+C69-E69</f>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10358,7 +10553,7 @@
       <c r="E70" s="79"/>
       <c r="F70" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10369,7 +10564,7 @@
       <c r="E71" s="79"/>
       <c r="F71" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10380,7 +10575,7 @@
       <c r="E72" s="79"/>
       <c r="F72" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10391,7 +10586,7 @@
       <c r="E73" s="79"/>
       <c r="F73" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10402,7 +10597,7 @@
       <c r="E74" s="79"/>
       <c r="F74" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10413,7 +10608,7 @@
       <c r="E75" s="79"/>
       <c r="F75" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10424,7 +10619,7 @@
       <c r="E76" s="79"/>
       <c r="F76" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10435,7 +10630,7 @@
       <c r="E77" s="79"/>
       <c r="F77" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10446,7 +10641,7 @@
       <c r="E78" s="79"/>
       <c r="F78" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10457,7 +10652,7 @@
       <c r="E79" s="79"/>
       <c r="F79" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10468,7 +10663,7 @@
       <c r="E80" s="79"/>
       <c r="F80" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10479,7 +10674,7 @@
       <c r="E81" s="83"/>
       <c r="F81" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10490,7 +10685,7 @@
       <c r="E82" s="83"/>
       <c r="F82" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10501,7 +10696,7 @@
       <c r="E83" s="83"/>
       <c r="F83" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10512,7 +10707,7 @@
       <c r="E84" s="83"/>
       <c r="F84" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10523,7 +10718,7 @@
       <c r="E85" s="83"/>
       <c r="F85" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10534,7 +10729,7 @@
       <c r="E86" s="83"/>
       <c r="F86" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10545,7 +10740,7 @@
       <c r="E87" s="79"/>
       <c r="F87" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10556,7 +10751,7 @@
       <c r="E88" s="79"/>
       <c r="F88" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10567,7 +10762,7 @@
       <c r="E89" s="79"/>
       <c r="F89" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10578,7 +10773,7 @@
       <c r="E90" s="79"/>
       <c r="F90" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10589,7 +10784,7 @@
       <c r="E91" s="79"/>
       <c r="F91" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10600,7 +10795,7 @@
       <c r="E92" s="79"/>
       <c r="F92" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10611,7 +10806,7 @@
       <c r="E93" s="79"/>
       <c r="F93" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10622,7 +10817,7 @@
       <c r="E94" s="79"/>
       <c r="F94" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10633,7 +10828,7 @@
       <c r="E95" s="79"/>
       <c r="F95" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -10644,7 +10839,7 @@
       <c r="E96" s="79"/>
       <c r="F96" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -10657,23 +10852,23 @@
       <c r="E97" s="151"/>
       <c r="F97" s="145">
         <f t="shared" si="1"/>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B98" s="104"/>
       <c r="C98" s="3">
         <f>SUM(C3:C97)</f>
-        <v>710732.2699999999</v>
+        <v>1424333.9499999997</v>
       </c>
       <c r="D98" s="103"/>
       <c r="E98" s="3">
         <f>SUM(E3:E97)</f>
-        <v>686878.8</v>
+        <v>1086878.8</v>
       </c>
       <c r="F98" s="153">
         <f>F97</f>
-        <v>23853.470000000088</v>
+        <v>337455.15000000008</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -10915,12 +11110,12 @@
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="163"/>
-      <c r="B45" s="251" t="s">
+      <c r="B45" s="255" t="s">
         <v>31</v>
       </c>
-      <c r="C45" s="252"/>
-      <c r="D45" s="252"/>
-      <c r="E45" s="253"/>
+      <c r="C45" s="256"/>
+      <c r="D45" s="256"/>
+      <c r="E45" s="257"/>
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>